<commit_message>
feat: wip portfolio mgmt
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>stock_info</t>
+          <t>next_ex_dividend_dt</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>dividend_history</t>
+          <t>dividend_yield</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -517,19 +517,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>11.3</v>
       </c>
       <c r="F2" t="n">
-        <v>79.10000000000001</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>12.81</v>
+        <v>13.399</v>
       </c>
       <c r="H2" t="n">
-        <v>89.67</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>10</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>9.94</v>
+        <v>10.285</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -599,19 +599,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>86</v>
       </c>
       <c r="F4" t="n">
-        <v>430</v>
+        <v>258</v>
       </c>
       <c r="G4" t="n">
-        <v>129.33</v>
+        <v>130.8301</v>
       </c>
       <c r="H4" t="n">
-        <v>646.6500000000001</v>
+        <v>392.4902999999999</v>
       </c>
       <c r="I4" t="n">
         <v>86</v>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>17.93</v>
+        <v>17.86</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>5.09</v>
+        <v>5.34</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4.1</v>
+        <v>4.505</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -772,10 +772,10 @@
         <v>101.22</v>
       </c>
       <c r="G8" t="n">
-        <v>6.72</v>
+        <v>6.62</v>
       </c>
       <c r="H8" t="n">
-        <v>94.08</v>
+        <v>92.68000000000001</v>
       </c>
       <c r="I8" t="n">
         <v>7</v>
@@ -813,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>5.48</v>
+        <v>5.92</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -841,7 +841,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -854,10 +854,10 @@
         <v>153.75</v>
       </c>
       <c r="G10" t="n">
-        <v>10.19</v>
+        <v>10.355</v>
       </c>
       <c r="H10" t="n">
-        <v>152.85</v>
+        <v>155.325</v>
       </c>
       <c r="I10" t="n">
         <v>10.25</v>
@@ -895,10 +895,10 @@
         <v>74.69999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>13.3</v>
+        <v>13.79</v>
       </c>
       <c r="H11" t="n">
-        <v>79.80000000000001</v>
+        <v>82.73999999999999</v>
       </c>
       <c r="I11" t="n">
         <v>12.45</v>
@@ -923,7 +923,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -936,10 +936,10 @@
         <v>42</v>
       </c>
       <c r="G12" t="n">
-        <v>48.37</v>
+        <v>44.81</v>
       </c>
       <c r="H12" t="n">
-        <v>48.37</v>
+        <v>44.81</v>
       </c>
       <c r="I12" t="n">
         <v>42</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>14.35</v>
+        <v>13.5</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1018,10 +1018,10 @@
         <v>71.55</v>
       </c>
       <c r="G14" t="n">
-        <v>5.23</v>
+        <v>5.15</v>
       </c>
       <c r="H14" t="n">
-        <v>78.45</v>
+        <v>77.25</v>
       </c>
       <c r="I14" t="n">
         <v>4.77</v>
@@ -1059,10 +1059,10 @@
         <v>70.75</v>
       </c>
       <c r="G15" t="n">
-        <v>13.98</v>
+        <v>13.3539</v>
       </c>
       <c r="H15" t="n">
-        <v>69.90000000000001</v>
+        <v>66.76949999999999</v>
       </c>
       <c r="I15" t="n">
         <v>14.15</v>
@@ -1100,10 +1100,10 @@
         <v>76.32000000000001</v>
       </c>
       <c r="G16" t="n">
-        <v>7.7</v>
+        <v>7.3</v>
       </c>
       <c r="H16" t="n">
-        <v>69.3</v>
+        <v>65.7</v>
       </c>
       <c r="I16" t="n">
         <v>8.48</v>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1141,10 +1141,10 @@
         <v>418.988</v>
       </c>
       <c r="G17" t="n">
-        <v>122.34</v>
+        <v>119.87</v>
       </c>
       <c r="H17" t="n">
-        <v>489.36</v>
+        <v>479.48</v>
       </c>
       <c r="I17" t="n">
         <v>104.747</v>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>3.69</v>
+        <v>3.65</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1214,25 +1214,25 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E19" t="n">
-        <v>26.8</v>
+        <v>24.376</v>
       </c>
       <c r="F19" t="n">
-        <v>214.4</v>
+        <v>804.408</v>
       </c>
       <c r="G19" t="n">
-        <v>24.63</v>
+        <v>23.84</v>
       </c>
       <c r="H19" t="n">
-        <v>197.04</v>
+        <v>786.72</v>
       </c>
       <c r="I19" t="n">
-        <v>26.8</v>
+        <v>24.376</v>
       </c>
       <c r="J19" t="n">
-        <v>30.82</v>
+        <v>28.03</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1251,23 +1251,23 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
         <v>4.55</v>
       </c>
       <c r="F20" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>5.32</v>
+        <v>5.0799</v>
       </c>
       <c r="H20" t="n">
-        <v>106.4</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>4.55</v>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>10.92</v>
+        <v>11.44</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1346,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>20.12</v>
+        <v>20.59</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>9.65</v>
+        <v>9.9</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>7.15</v>
+        <v>7.89</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>9.970000000000001</v>
+        <v>10.3675</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1497,29 +1497,29 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>216</v>
+        <v>366</v>
       </c>
       <c r="E26" t="n">
-        <v>5.01</v>
+        <v>4.916</v>
       </c>
       <c r="F26" t="n">
-        <v>1082.16</v>
+        <v>1799.256</v>
       </c>
       <c r="G26" t="n">
-        <v>4.8</v>
+        <v>4.975</v>
       </c>
       <c r="H26" t="n">
-        <v>1036.8</v>
+        <v>1820.85</v>
       </c>
       <c r="I26" t="n">
-        <v>5.01</v>
+        <v>4.916</v>
       </c>
       <c r="J26" t="n">
-        <v>5.76</v>
+        <v>5.65</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -1542,19 +1542,19 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>6.15</v>
       </c>
       <c r="F27" t="n">
-        <v>61.5</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>6.65</v>
+        <v>7.23</v>
       </c>
       <c r="H27" t="n">
-        <v>66.5</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>6.15</v>
@@ -1592,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>19.1</v>
+        <v>19.64</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1633,10 +1633,10 @@
         <v>96.25</v>
       </c>
       <c r="G29" t="n">
-        <v>18.03</v>
+        <v>17.125</v>
       </c>
       <c r="H29" t="n">
-        <v>90.15000000000001</v>
+        <v>85.625</v>
       </c>
       <c r="I29" t="n">
         <v>19.25</v>
@@ -1674,10 +1674,10 @@
         <v>9.16</v>
       </c>
       <c r="G30" t="n">
-        <v>8.279999999999999</v>
+        <v>9.037599999999999</v>
       </c>
       <c r="H30" t="n">
-        <v>8.279999999999999</v>
+        <v>9.037599999999999</v>
       </c>
       <c r="I30" t="n">
         <v>3</v>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>7.52</v>
+        <v>7.345</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1756,10 +1756,10 @@
         <v>281.915</v>
       </c>
       <c r="G32" t="n">
-        <v>256.6</v>
+        <v>257.5918</v>
       </c>
       <c r="H32" t="n">
-        <v>256.6</v>
+        <v>257.5918</v>
       </c>
       <c r="I32" t="n">
         <v>24.33</v>
@@ -1797,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>13.17</v>
+        <v>13.605</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
chore: update data and tracker
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -551,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>10.13</v>
+        <v>10.6</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -568,10 +568,10 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.1367</v>
+        <v>0.1321</v>
       </c>
       <c r="M2" t="n">
-        <v>10.28</v>
+        <v>10.37</v>
       </c>
       <c r="N2" t="n">
         <v>7.52</v>
@@ -581,7 +581,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-27 20:30:S', '2023-07-31 20:30:S'], 'earningsAverage': 0.29, 'earningsLow': 0.24, 'earningsHigh': 0.35, 'revenueAverage': 26470000, 'revenueLow': 25300000, 'revenueHigh': 28600000}</t>
+          <t>{'earningsDate': ['2023-08-02 20:30:S'], 'earningsAverage': 0.29, 'earningsLow': 0.24, 'earningsHigh': 0.35, 'revenueAverage': 26470000, 'revenueLow': 25300000, 'revenueHigh': 28600000}</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -621,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>12.59</v>
+        <v>12.8</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.1418</v>
+        <v>0.15</v>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
@@ -649,7 +649,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-07 20:30:S', '2023-08-11 20:30:S'], 'earningsAverage': 0.52, 'earningsLow': 0.42, 'earningsHigh': 0.56, 'revenueAverage': 16720000, 'revenueLow': 15150000, 'revenueHigh': 17760000}</t>
+          <t>{'earningsDate': ['2023-08-07 20:30:S', '2023-08-11 20:30:S'], 'earningsAverage': 0.53, 'earningsLow': 0.49, 'earningsHigh': 0.56, 'revenueAverage': 17110000, 'revenueLow': 16670000, 'revenueHigh': 17760000}</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>9.970000000000001</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -706,10 +706,10 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.1399</v>
+        <v>0.1444</v>
       </c>
       <c r="M4" t="n">
-        <v>11.95</v>
+        <v>11.99</v>
       </c>
       <c r="N4" t="n">
         <v>7.3</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-24 18:59:S', '2023-07-28 20:00:S'], 'earningsAverage': 0.62, 'earningsLow': 0.55, 'earningsHigh': 0.73, 'revenueAverage': 378860000, 'revenueLow': 334440000, 'revenueHigh': 443000000}</t>
+          <t>{'earningsDate': ['2023-07-25 04:00:S'], 'earningsAverage': 0.62, 'earningsLow': 0.55, 'earningsHigh': 0.73, 'revenueAverage': 378860000, 'revenueLow': 334440000, 'revenueHigh': 443000000}</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>6.95</v>
+        <v>6.97</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -776,10 +776,10 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.1396</v>
+        <v>0.1163</v>
       </c>
       <c r="M5" t="n">
-        <v>9.76</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="N5" t="n">
         <v>5.15</v>
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>9.039999999999999</v>
+        <v>9.5</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -846,10 +846,10 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0.36200002</v>
+        <v>0.33040002</v>
       </c>
       <c r="M6" t="n">
-        <v>6.25</v>
+        <v>6.81</v>
       </c>
       <c r="N6" t="n">
         <v>8.01</v>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>130.22</v>
+        <v>128.78</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -921,7 +921,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-26 18:59:S', '2023-07-31 20:00:S'], 'earningsAverage': 0.35, 'earningsLow': 0.14, 'earningsHigh': 0.45, 'revenueAverage': 131326000000, 'revenueLow': 127000000000, 'revenueHigh': 133130000000}</t>
+          <t>{'earningsDate': ['2023-07-26 18:59:S', '2023-07-31 20:00:S'], 'earningsAverage': 0.35, 'earningsLow': 0.14, 'earningsHigh': 0.47, 'revenueAverage': 131375000000, 'revenueLow': 127000000000, 'revenueHigh': 133130000000}</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>8.1</v>
+        <v>8.4</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.1576</v>
+        <v>0.1557</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>18.86</v>
+        <v>18.98</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.1567</v>
+        <v>0.1551</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>5.31</v>
+        <v>5.11</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1114,10 +1114,10 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.18049999</v>
+        <v>0.1857</v>
       </c>
       <c r="M10" t="n">
-        <v>14.69</v>
+        <v>14.87</v>
       </c>
       <c r="N10" t="n">
         <v>4.38</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>7.88</v>
+        <v>7.7</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1184,10 +1184,10 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.1276</v>
+        <v>0.1295</v>
       </c>
       <c r="M11" t="n">
-        <v>7.61</v>
+        <v>7.6</v>
       </c>
       <c r="N11" t="n">
         <v>6.96</v>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-07 18:59:S', '2023-08-11 20:00:S'], 'earningsAverage': 0.29, 'earningsLow': 0.26, 'earningsHigh': 0.31, 'revenueAverage': 70640000, 'revenueLow': 67360000, 'revenueHigh': 73330000}</t>
+          <t>{'earningsDate': ['2023-08-10 04:00:S'], 'earningsAverage': 0.29, 'earningsLow': 0.26, 'earningsHigh': 0.31, 'revenueAverage': 70640000, 'revenueLow': 67360000, 'revenueHigh': 73330000}</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>4.89</v>
+        <v>4.71</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1254,10 +1254,10 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>0.16700001</v>
+        <v>0.16139999</v>
       </c>
       <c r="M12" t="n">
-        <v>7.08</v>
+        <v>7.29</v>
       </c>
       <c r="N12" t="n">
         <v>3.42</v>
@@ -1307,10 +1307,10 @@
         <v>101.22</v>
       </c>
       <c r="G13" t="n">
-        <v>7.02</v>
+        <v>7.46</v>
       </c>
       <c r="H13" t="n">
-        <v>98.28</v>
+        <v>104.44</v>
       </c>
       <c r="I13" t="n">
         <v>6.35</v>
@@ -1324,7 +1324,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>0.1714</v>
+        <v>0.1542</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-01 20:30:S', '2023-08-07 20:30:S'], 'earningsAverage': 0.01, 'earningsLow': -0.07, 'earningsHigh': 0.11, 'revenueAverage': 173630000, 'revenueLow': 145900000, 'revenueHigh': 202000000}</t>
+          <t>{'earningsDate': ['2023-08-02 20:30:S'], 'earningsAverage': 0.01, 'earningsLow': -0.07, 'earningsHigh': 0.11, 'revenueAverage': 173630000, 'revenueLow': 145900000, 'revenueHigh': 202000000}</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.91</v>
+        <v>0.9525</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>0.67230004</v>
+        <v>0.6422</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1443,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>5.63</v>
+        <v>5.65</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1460,10 +1460,10 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>0.1224</v>
+        <v>0.1319</v>
       </c>
       <c r="M15" t="n">
-        <v>13.31</v>
+        <v>13.38</v>
       </c>
       <c r="N15" t="n">
         <v>4.48</v>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02 20:30:S', '2023-08-07 20:30:S'], 'earningsAverage': 0.17, 'earningsLow': 0.12, 'earningsHigh': 0.21, 'revenueAverage': 80650000, 'revenueLow': 70290000, 'revenueHigh': 88500000}</t>
+          <t>{'earningsDate': ['2023-08-02 20:30:S', '2023-08-07 20:30:S'], 'earningsAverage': 0.17, 'earningsLow': 0.12, 'earningsHigh': 0.21, 'revenueAverage': 79770000, 'revenueLow': 70290000, 'revenueHigh': 88500000}</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1513,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>10.53</v>
+        <v>10.66</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>0.132</v>
+        <v>0.127</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-08 03:00:S', '2023-08-12 03:00:S'], 'earningsAverage': 0.45, 'earningsLow': 0.37, 'earningsHigh': 0.54, 'revenueAverage': 58650000, 'revenueLow': 51290000, 'revenueHigh': 66000000}</t>
+          <t>{'earningsDate': ['2023-08-09 20:30:S'], 'earningsAverage': 0.45, 'earningsLow': 0.37, 'earningsHigh': 0.54, 'revenueAverage': 58650000, 'revenueLow': 51290000, 'revenueHigh': 66000000}</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>11.28</v>
+        <v>11.5</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1598,7 +1598,7 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>0.1273</v>
+        <v>0.1295</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-01 11:24:S', '2023-08-05 11:24:S'], 'earningsAverage': 0.35, 'earningsLow': 0.3, 'earningsHigh': 0.41, 'revenueAverage': 76630000, 'revenueLow': 74000000, 'revenueHigh': 79270000}</t>
+          <t>{'earningsDate': ['2023-08-01 11:24:S', '2023-08-05 11:24:S'], 'earningsAverage': 0.34, 'earningsLow': 0.29, 'earningsHigh': 0.41, 'revenueAverage': 76630000, 'revenueLow': 74000000, 'revenueHigh': 79270000}</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>7.14</v>
+        <v>7.03</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1662,14 +1662,14 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2023-06-29 08:00:00</t>
+          <t>2023-07-28 08:00:00</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>0.1308</v>
+        <v>0.1366</v>
       </c>
       <c r="M18" t="n">
-        <v>12.38</v>
+        <v>12.37</v>
       </c>
       <c r="N18" t="n">
         <v>5.7</v>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1719,10 +1719,10 @@
         <v>153.75</v>
       </c>
       <c r="G19" t="n">
-        <v>10.18</v>
+        <v>10.12</v>
       </c>
       <c r="H19" t="n">
-        <v>152.7</v>
+        <v>151.8</v>
       </c>
       <c r="I19" t="n">
         <v>10.16</v>
@@ -1736,16 +1736,16 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>0.16440001</v>
+        <v>0.16389999</v>
       </c>
       <c r="M19" t="n">
-        <v>14.15</v>
+        <v>14.32</v>
       </c>
       <c r="N19" t="n">
         <v>9.960000000000001</v>
       </c>
       <c r="O19" t="n">
-        <v>12.47</v>
+        <v>12.1</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1789,10 +1789,10 @@
         <v>74.69999999999999</v>
       </c>
       <c r="G20" t="n">
-        <v>13.54</v>
+        <v>13.75</v>
       </c>
       <c r="H20" t="n">
-        <v>81.23999999999999</v>
+        <v>82.5</v>
       </c>
       <c r="I20" t="n">
         <v>11.03</v>
@@ -1802,14 +1802,14 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2023-06-29 08:00:00</t>
+          <t>2023-07-28 08:00:00</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>0.1302</v>
+        <v>0.1309</v>
       </c>
       <c r="M20" t="n">
-        <v>11.02</v>
+        <v>11.06</v>
       </c>
       <c r="N20" t="n">
         <v>10.81</v>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02 18:59:S', '2023-08-07 20:00:S'], 'earningsAverage': 0.45, 'earningsLow': 0.42, 'earningsHigh': 0.48, 'revenueAverage': 49040000, 'revenueLow': 26660000, 'revenueHigh': 75200000}</t>
+          <t>{'earningsDate': ['2023-08-02 18:59:S', '2023-08-07 20:00:S'], 'earningsAverage': 0.45, 'earningsLow': 0.42, 'earningsHigh': 0.48, 'revenueAverage': 49020000, 'revenueLow': 26550000, 'revenueHigh': 75200000}</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -1859,10 +1859,10 @@
         <v>42</v>
       </c>
       <c r="G21" t="n">
-        <v>46.78</v>
+        <v>45.94</v>
       </c>
       <c r="H21" t="n">
-        <v>46.78</v>
+        <v>45.94</v>
       </c>
       <c r="I21" t="n">
         <v>39.94</v>
@@ -1876,7 +1876,7 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>0.102</v>
+        <v>0.1001</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
@@ -1887,7 +1887,7 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-03 04:00:S', '2023-08-08 04:00:S'], 'earningsAverage': 0.89, 'earningsLow': 0.66, 'earningsHigh': 1.29, 'revenueAverage': 104530000, 'revenueLow': 67540000, 'revenueHigh': 122240000}</t>
+          <t>{'earningsDate': ['2023-08-04 04:00:S'], 'earningsAverage': 0.86, 'earningsLow': 0.44, 'earningsHigh': 1.29, 'revenueAverage': 102880000, 'revenueLow': 67540000, 'revenueHigh': 122240000}</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1927,13 +1927,13 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>14.6</v>
+        <v>15.7</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>7.66</v>
+        <v>8.4</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1944,11 +1944,11 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>0.2039</v>
+        <v>0.1856</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
-        <v>7.51</v>
+        <v>8.24</v>
       </c>
       <c r="O22" t="n">
         <v>19.29</v>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>19.25</v>
+        <v>19.51</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2012,10 +2012,10 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>0.1472</v>
+        <v>0.1435</v>
       </c>
       <c r="M23" t="n">
-        <v>13.5</v>
+        <v>13.55</v>
       </c>
       <c r="N23" t="n">
         <v>16.7</v>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>7.73</v>
+        <v>7.77</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2082,16 +2082,16 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>0.18180001</v>
+        <v>0.18090001</v>
       </c>
       <c r="M24" t="n">
-        <v>18.34</v>
+        <v>18.5</v>
       </c>
       <c r="N24" t="n">
         <v>7.51</v>
       </c>
       <c r="O24" t="n">
-        <v>12.75</v>
+        <v>12.6</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -2135,13 +2135,13 @@
         <v>71.55</v>
       </c>
       <c r="G25" t="n">
-        <v>5.35</v>
+        <v>5.41</v>
       </c>
       <c r="H25" t="n">
-        <v>80.25</v>
+        <v>81.15000000000001</v>
       </c>
       <c r="I25" t="n">
-        <v>3.83</v>
+        <v>3.91</v>
       </c>
       <c r="J25" t="n">
         <v>5.49</v>
@@ -2152,20 +2152,20 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>0.123500004</v>
+        <v>0.12189999</v>
       </c>
       <c r="M25" t="n">
-        <v>5.17</v>
+        <v>5.36</v>
       </c>
       <c r="N25" t="n">
-        <v>3.752381</v>
+        <v>3.828571</v>
       </c>
       <c r="O25" t="n">
         <v>6.342857</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.26, 'earningsLow': 0.26, 'earningsHigh': 0.26, 'revenueAverage': 3929910000, 'revenueLow': 3929910000, 'revenueHigh': 3929910000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.28, 'earningsLow': 0.26, 'earningsHigh': 0.29, 'revenueAverage': 3868710000, 'revenueLow': 3868710000, 'revenueHigh': 3868710000}</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
@@ -2205,10 +2205,10 @@
         <v>70.75</v>
       </c>
       <c r="G26" t="n">
-        <v>13.86</v>
+        <v>13.63</v>
       </c>
       <c r="H26" t="n">
-        <v>69.3</v>
+        <v>68.15000000000001</v>
       </c>
       <c r="I26" t="n">
         <v>12.16</v>
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="L26" t="n">
-        <v>0.1381</v>
+        <v>0.14060001</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-01 18:59:S', '2023-08-07 20:00:S'], 'earningsAverage': 0.31, 'earningsLow': 0.19, 'earningsHigh': 0.43, 'revenueAverage': 70780000, 'revenueLow': 62240000, 'revenueHigh': 101810000}</t>
+          <t>{'earningsDate': ['2023-08-04 20:30:S'], 'earningsAverage': 0.27, 'earningsLow': 0.13, 'earningsHigh': 0.4, 'revenueAverage': 70300000, 'revenueLow': 62240000, 'revenueHigh': 98920000}</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>10.57</v>
+        <v>11.16</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2286,14 +2286,14 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2023-04-12 08:00:00</t>
+          <t>2023-07-12 08:00:00</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>0.1619</v>
+        <v>0.14840001</v>
       </c>
       <c r="M27" t="n">
-        <v>10.99</v>
+        <v>11.07</v>
       </c>
       <c r="N27" t="n">
         <v>8.84</v>
@@ -2343,10 +2343,10 @@
         <v>76.32000000000001</v>
       </c>
       <c r="G28" t="n">
-        <v>7.53</v>
+        <v>7.75</v>
       </c>
       <c r="H28" t="n">
-        <v>67.77</v>
+        <v>69.75</v>
       </c>
       <c r="I28" t="n">
         <v>7.13</v>
@@ -2360,7 +2360,7 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>0.1696</v>
+        <v>0.1658</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
@@ -2411,10 +2411,10 @@
         <v>418.988</v>
       </c>
       <c r="G29" t="n">
-        <v>119.9</v>
+        <v>117.14</v>
       </c>
       <c r="H29" t="n">
-        <v>479.6</v>
+        <v>468.56</v>
       </c>
       <c r="I29" t="n">
         <v>85.01000000000001</v>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-25 04:00:S', '2023-07-29 04:00:S'], 'earningsAverage': 1.34, 'earningsLow': 1.06, 'earningsHigh': 1.5, 'revenueAverage': 72775800000, 'revenueLow': 70692600000, 'revenueHigh': 74329000000}</t>
+          <t>{'earningsDate': ['2023-07-25 04:00:S', '2023-07-29 04:00:S'], 'earningsAverage': 1.34, 'earningsLow': 1.06, 'earningsHigh': 1.5, 'revenueAverage': 72772800000, 'revenueLow': 70692600000, 'revenueHigh': 74329000000}</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>5.27</v>
+        <v>5.42</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2490,10 +2490,10 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>0.14840001</v>
+        <v>0.15010001</v>
       </c>
       <c r="M30" t="n">
-        <v>11.14</v>
+        <v>11.27</v>
       </c>
       <c r="N30" t="n">
         <v>3.97</v>
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.34</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>0.1514</v>
+        <v>0.1522</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>3.68</v>
+        <v>3.9129</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>0.144</v>
+        <v>0.1329</v>
       </c>
       <c r="M32" t="n">
-        <v>15.17</v>
+        <v>15.24</v>
       </c>
       <c r="N32" t="n">
         <v>3.18</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>11.26</v>
+        <v>11.13</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2698,10 +2698,10 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>0.13430001</v>
+        <v>0.1436</v>
       </c>
       <c r="M33" t="n">
-        <v>20.66</v>
+        <v>20.79</v>
       </c>
       <c r="N33" t="n">
         <v>9.48</v>
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8651</v>
+        <v>1.06</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -2768,7 +2768,7 @@
         </is>
       </c>
       <c r="L34" t="n">
-        <v>0.48259997</v>
+        <v>0.4635</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
@@ -2806,7 +2806,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -2819,13 +2819,13 @@
         <v>1647.513</v>
       </c>
       <c r="G35" t="n">
-        <v>23.39</v>
+        <v>23.46</v>
       </c>
       <c r="H35" t="n">
-        <v>1613.91</v>
+        <v>1618.74</v>
       </c>
       <c r="I35" t="n">
-        <v>23.49</v>
+        <v>23.31</v>
       </c>
       <c r="J35" t="n">
         <v>27.46</v>
@@ -2836,11 +2836,11 @@
         </is>
       </c>
       <c r="L35" t="n">
-        <v>0.5484</v>
+        <v>0.5548999999999999</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
-        <v>23.03</v>
+        <v>22.85</v>
       </c>
       <c r="O35" t="n">
         <v>48.2</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>12.25</v>
+        <v>12.71</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -2904,10 +2904,10 @@
         </is>
       </c>
       <c r="L36" t="n">
-        <v>0.1389</v>
+        <v>0.1353</v>
       </c>
       <c r="M36" t="n">
-        <v>9.380000000000001</v>
+        <v>9.48</v>
       </c>
       <c r="N36" t="n">
         <v>9.94</v>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-24 18:59:S', '2023-07-28 20:00:S'], 'earningsAverage': 0.27, 'earningsLow': -0.12, 'earningsHigh': 0.46, 'revenueAverage': 48380000, 'revenueLow': 44900000, 'revenueHigh': 55600000}</t>
+          <t>{'earningsDate': ['2023-07-25 04:00:S'], 'earningsAverage': 0.27, 'earningsLow': -0.12, 'earningsHigh': 0.46, 'revenueAverage': 48380000, 'revenueLow': 44900000, 'revenueHigh': 55600000}</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
@@ -2957,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.27</v>
+        <v>5.29</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -2974,10 +2974,10 @@
         </is>
       </c>
       <c r="L37" t="n">
-        <v>0.1899</v>
+        <v>0.1924</v>
       </c>
       <c r="M37" t="n">
-        <v>7.7</v>
+        <v>7.86</v>
       </c>
       <c r="N37" t="n">
         <v>4.11</v>
@@ -3014,7 +3014,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -3027,13 +3027,13 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>6.82</v>
+        <v>6.75</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>4.54</v>
+        <v>4.61</v>
       </c>
       <c r="J38" t="n">
         <v>0</v>
@@ -3044,18 +3044,18 @@
         </is>
       </c>
       <c r="L38" t="n">
-        <v>0.1145</v>
+        <v>0.1201</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="n">
-        <v>4.447</v>
+        <v>4.52</v>
       </c>
       <c r="O38" t="n">
         <v>7.95</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 212660000, 'revenueLow': 212660000, 'revenueHigh': 212660000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 207270000, 'revenueLow': 207270000, 'revenueHigh': 207270000}</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>1.51</v>
+        <v>1.52</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -3112,18 +3112,18 @@
         </is>
       </c>
       <c r="L39" t="n">
-        <v>0.1457</v>
+        <v>0.1507</v>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
         <v>1.23</v>
       </c>
       <c r="O39" t="n">
-        <v>6.15</v>
+        <v>5.32</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-03 04:00:S', '2023-08-08 04:00:S'], 'earningsAverage': 0.05, 'earningsLow': 0.05, 'earningsHigh': 0.06, 'revenueAverage': 1436620000, 'revenueLow': 1285690000, 'revenueHigh': 1550630000}</t>
+          <t>{'earningsDate': ['2023-08-03 04:00:S', '2023-08-08 04:00:S'], 'earningsAverage': 0.05, 'earningsLow': 0.05, 'earningsHigh': 0.06, 'revenueAverage': 1422040000, 'revenueLow': 1272640000, 'revenueHigh': 1534900000}</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
@@ -3150,7 +3150,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>11.17</v>
+        <v>11.09</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -3180,10 +3180,10 @@
         </is>
       </c>
       <c r="L40" t="n">
-        <v>0.1221</v>
+        <v>0.1258</v>
       </c>
       <c r="M40" t="n">
-        <v>13.23</v>
+        <v>13.28</v>
       </c>
       <c r="N40" t="n">
         <v>7.15</v>
@@ -3233,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>20.45</v>
+        <v>18.82</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -3250,10 +3250,10 @@
         </is>
       </c>
       <c r="L41" t="n">
-        <v>0.24239999</v>
+        <v>0.2469</v>
       </c>
       <c r="M41" t="n">
-        <v>12.17</v>
+        <v>12.08</v>
       </c>
       <c r="N41" t="n">
         <v>16.56</v>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -3303,13 +3303,13 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>3.67</v>
+        <v>3.74</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>1.84</v>
+        <v>1.93</v>
       </c>
       <c r="J42" t="n">
         <v>0</v>
@@ -3320,13 +3320,13 @@
         </is>
       </c>
       <c r="L42" t="n">
-        <v>0.1719</v>
+        <v>0.1604</v>
       </c>
       <c r="M42" t="n">
-        <v>6.52</v>
+        <v>6.59</v>
       </c>
       <c r="N42" t="n">
-        <v>1.8</v>
+        <v>1.89</v>
       </c>
       <c r="O42" t="n">
         <v>4.65</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>19.76</v>
+        <v>19.66</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -3390,10 +3390,10 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>0.1262</v>
+        <v>0.1331</v>
       </c>
       <c r="M43" t="n">
-        <v>12.41</v>
+        <v>12.47</v>
       </c>
       <c r="N43" t="n">
         <v>15.11</v>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-25 18:59:S', '2023-07-31 20:00:S'], 'earningsAverage': 0.74, 'earningsLow': 0.62, 'earningsHigh': 0.85, 'revenueAverage': 869020000, 'revenueLow': 770000000, 'revenueHigh': 996000000}</t>
+          <t>{'earningsDate': ['2023-07-27 04:00:S'], 'earningsAverage': 0.74, 'earningsLow': 0.62, 'earningsHigh': 0.85, 'revenueAverage': 869020000, 'revenueLow': 770000000, 'revenueHigh': 996000000}</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
@@ -3430,7 +3430,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>9.93</v>
+        <v>10</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="L44" t="n">
-        <v>0.1228</v>
+        <v>0.12060001</v>
       </c>
       <c r="M44" t="n">
-        <v>14.35</v>
+        <v>14.38</v>
       </c>
       <c r="N44" t="n">
         <v>8.279999999999999</v>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-31 18:59:S', '2023-08-04 20:00:S'], 'earningsAverage': 0.1, 'earningsLow': 0.03, 'earningsHigh': 0.28, 'revenueAverage': 20650000, 'revenueLow': 17400000, 'revenueHigh': 23720000}</t>
+          <t>{'earningsDate': ['2023-08-03 04:00:S'], 'earningsAverage': 0.1, 'earningsLow': 0.04, 'earningsHigh': 0.28, 'revenueAverage': 20650000, 'revenueLow': 17400000, 'revenueHigh': 23720000}</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
@@ -3500,7 +3500,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -3513,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>8.460000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -3530,7 +3530,7 @@
         </is>
       </c>
       <c r="L45" t="n">
-        <v>0.2613</v>
+        <v>0.2616</v>
       </c>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>7.87</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -3598,16 +3598,16 @@
         </is>
       </c>
       <c r="L46" t="n">
-        <v>0.1284</v>
+        <v>0.1266</v>
       </c>
       <c r="M46" t="n">
-        <v>12.1</v>
+        <v>12.33</v>
       </c>
       <c r="N46" t="n">
         <v>5.86</v>
       </c>
       <c r="O46" t="n">
-        <v>20.94</v>
+        <v>20.93</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
@@ -3638,7 +3638,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -3651,7 +3651,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>10.25</v>
+        <v>10.03</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -3668,7 +3668,7 @@
         </is>
       </c>
       <c r="L47" t="n">
-        <v>0.1825</v>
+        <v>0.1899</v>
       </c>
       <c r="M47" t="n">
         <v>18.59</v>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02 18:59:S', '2023-08-07 20:00:S'], 'earningsAverage': -0.01, 'earningsLow': -0.2, 'earningsHigh': 0.09, 'revenueAverage': 9850000, 'revenueLow': 4100000, 'revenueHigh': 15600000}</t>
+          <t>{'earningsDate': ['2023-07-28 04:00:S'], 'earningsAverage': -0.01, 'earningsLow': -0.2, 'earningsHigh': 0.09, 'revenueAverage': 9850000, 'revenueLow': 4100000, 'revenueHigh': 15600000}</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
@@ -3708,23 +3708,23 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>379</v>
+        <v>398</v>
       </c>
       <c r="E48" t="n">
-        <v>4.914</v>
+        <v>4.91</v>
       </c>
       <c r="F48" t="n">
-        <v>1862.406</v>
+        <v>1954.18</v>
       </c>
       <c r="G48" t="n">
-        <v>4.89</v>
+        <v>4.98</v>
       </c>
       <c r="H48" t="n">
-        <v>1853.31</v>
+        <v>1982.04</v>
       </c>
       <c r="I48" t="n">
         <v>4.86</v>
@@ -3738,10 +3738,10 @@
         </is>
       </c>
       <c r="L48" t="n">
-        <v>0.1928</v>
+        <v>0.19510001</v>
       </c>
       <c r="M48" t="n">
-        <v>18.4</v>
+        <v>18.46</v>
       </c>
       <c r="N48" t="n">
         <v>4.76</v>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>2.73</v>
+        <v>2.88</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -3808,10 +3808,10 @@
         </is>
       </c>
       <c r="L49" t="n">
-        <v>0.1609</v>
+        <v>0.1458</v>
       </c>
       <c r="M49" t="n">
-        <v>14.75</v>
+        <v>14.82</v>
       </c>
       <c r="N49" t="n">
         <v>2.6</v>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-24 20:30:S', '2023-07-28 20:30:S'], 'earningsAverage': 0.11, 'earningsLow': 0.11, 'earningsHigh': 0.11, 'revenueAverage': 12719000, 'revenueLow': 12200000, 'revenueHigh': 12200000}</t>
+          <t>{'earningsDate': ['2023-07-24 20:30:S', '2023-07-28 20:30:S'], 'earningsAverage': 0.11, 'earningsLow': 0.11, 'earningsHigh': 0.11, 'revenueAverage': 12100000, 'revenueLow': 12100000, 'revenueHigh': 12100000}</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>13.97</v>
+        <v>13.56</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>0.4022</v>
+        <v>0.42610002</v>
       </c>
       <c r="M50" t="n">
-        <v>13.63</v>
+        <v>14.32</v>
       </c>
       <c r="N50" t="n">
         <v>8.880000000000001</v>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.73, 'earningsLow': 0.54, 'earningsHigh': 0.88, 'revenueAverage': 24494000000, 'revenueLow': 23460700000, 'revenueHigh': 25915000000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.72, 'earningsLow': 0.54, 'earningsHigh': 0.87, 'revenueAverage': 24277800000, 'revenueLow': 23138000000, 'revenueHigh': 25915000000}</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>7.6</v>
+        <v>7.78</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -3948,10 +3948,10 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>0.116000004</v>
+        <v>0.111</v>
       </c>
       <c r="M51" t="n">
-        <v>5.53</v>
+        <v>5.65</v>
       </c>
       <c r="N51" t="n">
         <v>5.99</v>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-26 04:00:S', '2023-08-01 04:00:S'], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 143210000, 'revenueLow': 142430000, 'revenueHigh': 144000000}</t>
+          <t>{'earningsDate': ['2023-07-27 04:00:S'], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 143210000, 'revenueLow': 142430000, 'revenueHigh': 144000000}</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
@@ -4001,7 +4001,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>20.06</v>
+        <v>20.33</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -4018,7 +4018,7 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>0.1437</v>
+        <v>0.1387</v>
       </c>
       <c r="M52" t="n">
         <v>13.53</v>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>7</v>
+        <v>7.35</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4084,11 +4084,11 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>2023-04-12 08:00:00</t>
+          <t>2023-07-12 08:00:00</t>
         </is>
       </c>
       <c r="L53" t="n">
-        <v>0.1304</v>
+        <v>0.115600005</v>
       </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>3.51</v>
+        <v>3.6</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -4156,7 +4156,7 @@
         </is>
       </c>
       <c r="L54" t="n">
-        <v>0.1525</v>
+        <v>0.1494</v>
       </c>
       <c r="M54" t="n">
         <v>11.65</v>
@@ -4209,10 +4209,10 @@
         <v>96.25</v>
       </c>
       <c r="G55" t="n">
-        <v>17.58</v>
+        <v>17.21</v>
       </c>
       <c r="H55" t="n">
-        <v>87.89999999999999</v>
+        <v>86.05000000000001</v>
       </c>
       <c r="I55" t="n">
         <v>17.19</v>
@@ -4226,7 +4226,7 @@
         </is>
       </c>
       <c r="L55" t="n">
-        <v>0.21440001</v>
+        <v>0.082100004</v>
       </c>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
@@ -4277,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>10.39</v>
+        <v>10.59</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -4294,7 +4294,7 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>0.1367</v>
+        <v>0.1385</v>
       </c>
       <c r="M56" t="n">
         <v>7.49</v>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-26 04:00:S', '2023-08-01 04:00:S'], 'earningsAverage': 0.34, 'earningsLow': 0.33, 'earningsHigh': 0.36, 'revenueAverage': 8760000, 'revenueLow': 8500000, 'revenueHigh': 9020000}</t>
+          <t>{'earningsDate': ['2023-08-01 04:00:S'], 'earningsAverage': 0.34, 'earningsLow': 0.33, 'earningsHigh': 0.36, 'revenueAverage': 8760000, 'revenueLow': 8500000, 'revenueHigh': 9020000}</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
@@ -4347,10 +4347,10 @@
         <v>9.16</v>
       </c>
       <c r="G57" t="n">
-        <v>8.52</v>
+        <v>9.07</v>
       </c>
       <c r="H57" t="n">
-        <v>8.52</v>
+        <v>9.07</v>
       </c>
       <c r="I57" t="n">
         <v>4.32</v>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-31 18:59:S', '2023-08-04 20:00:S'], 'earningsAverage': -0.06, 'earningsLow': -0.1, 'earningsHigh': 0.0, 'revenueAverage': 476190000, 'revenueLow': 437860000, 'revenueHigh': 503000000}</t>
+          <t>{'earningsDate': ['2023-07-31 20:00:S'], 'earningsAverage': -0.06, 'earningsLow': -0.1, 'earningsHigh': 0.0, 'revenueAverage': 475940000, 'revenueLow': 437860000, 'revenueHigh': 503000000}</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
@@ -4396,7 +4396,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -4409,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>11.94</v>
+        <v>12.4</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -4426,10 +4426,10 @@
         </is>
       </c>
       <c r="L58" t="n">
-        <v>0.1412</v>
+        <v>0.132</v>
       </c>
       <c r="M58" t="n">
-        <v>11.17</v>
+        <v>11.19</v>
       </c>
       <c r="N58" t="n">
         <v>9.41</v>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02 04:00:S', '2023-08-08 04:00:S'], 'earningsAverage': 0.5, 'earningsLow': 0.47, 'earningsHigh': 0.53, 'revenueAverage': 34190000, 'revenueLow': 31700000, 'revenueHigh': 38050000}</t>
+          <t>{'earningsDate': ['2023-08-02 04:00:S', '2023-08-08 04:00:S'], 'earningsAverage': 0.5, 'earningsLow': 0.47, 'earningsHigh': 0.53, 'revenueAverage': 34770000, 'revenueLow': 31700000, 'revenueHigh': 38050000}</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -4479,7 +4479,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>13.75</v>
+        <v>14.55</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -4496,7 +4496,7 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>0.1514</v>
+        <v>0.1416</v>
       </c>
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="n">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-04 04:00:S'], 'earningsAverage': 0.53, 'earningsLow': 0.5, 'earningsHigh': 0.56, 'revenueAverage': 41190000, 'revenueLow': 40620000, 'revenueHigh': 42480000}</t>
+          <t>{'earningsDate': ['2023-08-02 20:30:S'], 'earningsAverage': 0.53, 'earningsLow': 0.5, 'earningsHigh': 0.56, 'revenueAverage': 41370000, 'revenueLow': 40620000, 'revenueHigh': 42480000}</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
@@ -4534,7 +4534,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -4547,7 +4547,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>7.33</v>
+        <v>7.27</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -4564,10 +4564,10 @@
         </is>
       </c>
       <c r="L60" t="n">
-        <v>0.1277</v>
+        <v>0.132</v>
       </c>
       <c r="M60" t="n">
-        <v>10.43</v>
+        <v>10.52</v>
       </c>
       <c r="N60" t="n">
         <v>5.14</v>
@@ -4617,10 +4617,10 @@
         <v>281.915</v>
       </c>
       <c r="G61" t="n">
-        <v>279.82</v>
+        <v>269.79</v>
       </c>
       <c r="H61" t="n">
-        <v>279.82</v>
+        <v>269.79</v>
       </c>
       <c r="I61" t="n">
         <v>103.85</v>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-19 04:00:S', '2023-07-25 04:00:S'], 'earningsAverage': 0.79, 'earningsLow': 0.64, 'earningsHigh': 0.9, 'revenueAverage': 24079100000, 'revenueLow': 22301800000, 'revenueHigh': 26376200000}</t>
+          <t>{'earningsDate': ['2023-07-20 04:00:S'], 'earningsAverage': 0.82, 'earningsLow': 0.64, 'earningsHigh': 0.93, 'revenueAverage': 24569200000, 'revenueLow': 22301800000, 'revenueHigh': 26376200000}</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
@@ -4666,7 +4666,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -4679,7 +4679,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>13.3</v>
+        <v>13.06</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -4696,10 +4696,10 @@
         </is>
       </c>
       <c r="L62" t="n">
-        <v>0.13430001</v>
+        <v>0.1388</v>
       </c>
       <c r="M62" t="n">
-        <v>12.85</v>
+        <v>12.96</v>
       </c>
       <c r="N62" t="n">
         <v>11.57</v>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -4749,7 +4749,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>8.609999999999999</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -4766,10 +4766,10 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>0.1532</v>
+        <v>0.16690001</v>
       </c>
       <c r="M63" t="n">
-        <v>16.06</v>
+        <v>16.14</v>
       </c>
       <c r="N63" t="n">
         <v>7</v>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02 18:59:S', '2023-08-07 20:00:S'], 'earningsAverage': 0.28, 'earningsLow': 0.28, 'earningsHigh': 0.28, 'revenueAverage': 5330000, 'revenueLow': 5330000, 'revenueHigh': 5330000}</t>
+          <t>{'earningsDate': ['2023-08-02 18:59:S', '2023-08-07 20:00:S'], 'revenueAverage': 5330000, 'revenueLow': 5330000, 'revenueHigh': 5330000}</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">

</xml_diff>

<commit_message>
feat(wip): balance sheet analysis
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -548,7 +548,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>10.47</v>
+        <v>10.69</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.1336</t>
+          <t>0.1337</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -645,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>14.17</v>
+        <v>14.24</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.1356</t>
+          <t>0.1341</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>10.22</v>
+        <v>10.33</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -764,7 +764,7 @@
         <v>7.3</v>
       </c>
       <c r="P4" t="n">
-        <v>12.89</v>
+        <v>12.85</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -836,7 +836,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.113299996</t>
+          <t>0.1154</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02', '2023-08-07'], 'earningsAverage': 0.0, 'earningsLow': -0.03, 'earningsHigh': 0.02, 'revenueAverage': 6790000, 'revenueLow': 5700000, 'revenueHigh': 7970000}</t>
+          <t>{'earningsDate': ['2023-08-03'], 'earningsAverage': 0.0, 'earningsLow': -0.03, 'earningsHigh': 0.02, 'revenueAverage': 6790000, 'revenueLow': 5700000, 'revenueHigh': 7970000}</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>10.067</v>
+        <v>10.12</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>128.25</v>
+        <v>132.21</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>9.33</v>
+        <v>9.49</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.1368</t>
+          <t>0.1342</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>18.86</v>
+        <v>19.15</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.1461</t>
+          <t>0.1462</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>5.19</v>
+        <v>5.16</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 0.24, 'earningsLow': 0.17, 'earningsHigh': 0.29, 'revenueAverage': 26248000, 'revenueLow': 32500000, 'revenueHigh': 66600000}</t>
+          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 0.23, 'earningsLow': 0.17, 'earningsHigh': 0.27, 'revenueAverage': 55260000, 'revenueLow': 33040000, 'revenueHigh': 71340000}</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1309,7 +1309,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>8.4475</v>
+        <v>8.4282</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.22940001</t>
+          <t>0.23979999</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>8.27</v>
+        <v>8.32</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>4.81</v>
+        <v>4.99</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.158</t>
+          <t>0.1523</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1504,7 +1504,7 @@
         <v>3.42</v>
       </c>
       <c r="P13" t="n">
-        <v>9.43</v>
+        <v>9.33</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1553,10 +1553,10 @@
         <v>101.22</v>
       </c>
       <c r="G14" t="n">
-        <v>7.71</v>
+        <v>7.65</v>
       </c>
       <c r="H14" t="n">
-        <v>107.94</v>
+        <v>107.1</v>
       </c>
       <c r="I14" t="n">
         <v>6.3</v>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>6.29</v>
+        <v>6.39</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.11270001</t>
+          <t>0.1145</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1672,7 +1672,7 @@
         <v>4.48</v>
       </c>
       <c r="P15" t="n">
-        <v>10.66</v>
+        <v>10.61</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
@@ -1721,7 +1721,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>11.1</v>
+        <v>11.11</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>12.22</v>
+        <v>12.34</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.1167</t>
+          <t>0.1161</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>10.08</v>
       </c>
       <c r="P17" t="n">
-        <v>19.4</v>
+        <v>18.96</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>7.4</v>
+        <v>7.36</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.1297</t>
+          <t>0.1304</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1973,10 +1973,10 @@
         <v>153.75</v>
       </c>
       <c r="G19" t="n">
-        <v>10.26</v>
+        <v>10.32</v>
       </c>
       <c r="H19" t="n">
-        <v>153.9</v>
+        <v>154.8</v>
       </c>
       <c r="I19" t="n">
         <v>10.12</v>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>13.68</v>
+        <v>13.67</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2092,7 +2092,7 @@
         <v>10.81</v>
       </c>
       <c r="P20" t="n">
-        <v>16.38</v>
+        <v>16.3</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
@@ -2141,10 +2141,10 @@
         <v>42</v>
       </c>
       <c r="G21" t="n">
-        <v>44.51</v>
+        <v>45.86</v>
       </c>
       <c r="H21" t="n">
-        <v>44.51</v>
+        <v>45.86</v>
       </c>
       <c r="I21" t="n">
         <v>39.28</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>0.1041</t>
+          <t>0.10560001</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>15.54</v>
+        <v>16.08</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.1785</t>
+          <t>0.17989999</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>9.35</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="P22" t="n">
         <v>19.29</v>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>20.07</v>
+        <v>20.21</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>0.1389</t>
+          <t>0.13949999</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>8.279999999999999</v>
+        <v>8.26</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.1681</t>
+          <t>0.16950001</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>5.97</v>
+        <v>5.96</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.1069</t>
+          <t>0.1094</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.29, 'earningsLow': 0.28, 'earningsHigh': 0.3, 'revenueAverage': 3999510000, 'revenueLow': 3999510000, 'revenueHigh': 3999510000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.29, 'earningsLow': 0.28, 'earningsHigh': 0.3, 'revenueAverage': 4006430000, 'revenueLow': 4006430000, 'revenueHigh': 4006430000}</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -2561,10 +2561,10 @@
         <v>70.75</v>
       </c>
       <c r="G26" t="n">
-        <v>13.87</v>
+        <v>14.5</v>
       </c>
       <c r="H26" t="n">
-        <v>69.34999999999999</v>
+        <v>72.5</v>
       </c>
       <c r="I26" t="n">
         <v>12.41</v>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.14050001</t>
+          <t>0.1391</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>10.93</v>
+        <v>10.8</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.1444</t>
+          <t>0.14310001</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2729,10 +2729,10 @@
         <v>1023.26</v>
       </c>
       <c r="G28" t="n">
-        <v>7.5</v>
+        <v>7.73</v>
       </c>
       <c r="H28" t="n">
-        <v>1050</v>
+        <v>1082.2</v>
       </c>
       <c r="I28" t="n">
         <v>7.06</v>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.16780001</t>
+          <t>0.1667</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2813,10 +2813,10 @@
         <v>418.988</v>
       </c>
       <c r="G29" t="n">
-        <v>129.4</v>
+        <v>132.58</v>
       </c>
       <c r="H29" t="n">
-        <v>517.6</v>
+        <v>530.3200000000001</v>
       </c>
       <c r="I29" t="n">
         <v>85.01000000000001</v>
@@ -2844,7 +2844,7 @@
         <v>83.34</v>
       </c>
       <c r="P29" t="n">
-        <v>133.24</v>
+        <v>133.74</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.43, 'earningsLow': 1.27, 'earningsHigh': 1.55, 'revenueAverage': 75685400000, 'revenueLow': 72863000000, 'revenueHigh': 77922700000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.43, 'earningsLow': 1.27, 'earningsHigh': 1.55, 'revenueAverage': 75767700000, 'revenueLow': 72863000000, 'revenueHigh': 77922700000}</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>5.75</v>
+        <v>5.88</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>0.13939999</t>
+          <t>0.1391</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2928,7 +2928,7 @@
         <v>3.97</v>
       </c>
       <c r="P30" t="n">
-        <v>10.825</v>
+        <v>10.79</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-07', '2023-08-11'], 'earningsAverage': 0.14, 'earningsLow': 0.12, 'earningsHigh': 0.18, 'revenueAverage': 20950000, 'revenueLow': 20180000, 'revenueHigh': 22500000}</t>
+          <t>{'earningsDate': ['2023-08-08'], 'earningsAverage': 0.14, 'earningsLow': 0.12, 'earningsHigh': 0.18, 'revenueAverage': 20950000, 'revenueLow': 20180000, 'revenueHigh': 22500000}</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>9</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3145,7 +3145,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>11.95</v>
+        <v>12.13</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>0.13069999</t>
+          <t>0.1339</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>1.1</v>
+        <v>1.11</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>0.38259998</t>
+          <t>0.3729</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -3313,10 +3313,10 @@
         <v>1647.513</v>
       </c>
       <c r="G35" t="n">
-        <v>25.34</v>
+        <v>25.75</v>
       </c>
       <c r="H35" t="n">
-        <v>1748.46</v>
+        <v>1776.75</v>
       </c>
       <c r="I35" t="n">
         <v>23.01</v>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>0.50560004</t>
+          <t>0.5146</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -3397,7 +3397,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>12.2</v>
+        <v>12.59</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>0.1351</t>
+          <t>0.141</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.28, 'earningsLow': -0.34, 'earningsHigh': 0.92, 'revenueAverage': 45050000, 'revenueLow': 41000000, 'revenueHigh': 50000000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.1, 'earningsLow': -0.34, 'earningsHigh': 0.46, 'revenueAverage': 44170000, 'revenueLow': 41000000, 'revenueHigh': 50000000}</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.52</v>
+        <v>5.49</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3565,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>6.63</v>
+        <v>6.65</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>0.115600005</t>
+          <t>0.12149999</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -3597,7 +3597,7 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>5.178</v>
+        <v>5.68</v>
       </c>
       <c r="P38" t="n">
         <v>7.95</v>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 202150000, 'revenueLow': 200360000, 'revenueHigh': 203930000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 202410000, 'revenueLow': 199270000, 'revenueHigh': 205540000}</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -3649,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>1.76</v>
+        <v>1.82</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>0.131</t>
+          <t>0.120900005</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
@@ -3693,7 +3693,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02', '2023-08-07'], 'earningsAverage': 0.05, 'earningsLow': 0.05, 'earningsHigh': 0.06, 'revenueAverage': 1442230000, 'revenueLow': 1290700000, 'revenueHigh': 1556690000}</t>
+          <t>{'earningsDate': ['2023-08-02', '2023-08-07'], 'earningsAverage': 0.05, 'earningsLow': 0.05, 'earningsHigh': 0.06, 'revenueAverage': 1436980000, 'revenueLow': 1286010000, 'revenueHigh': 1551020000}</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>11.48</v>
+        <v>11.6</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>0.120299995</t>
+          <t>0.120699994</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -3817,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>18.34</v>
+        <v>18.5</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>0.28530002</t>
+          <t>0.2754</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -3897,7 +3897,7 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
-        <v>4.1</v>
+        <v>4.25</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -3912,7 +3912,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>0.1471</t>
+          <t>0.1412</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>4.1</v>
+        <v>4.25</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>0.1471</t>
+          <t>0.1412</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -4044,7 +4044,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -4057,7 +4057,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>20.07</v>
+        <v>20.35</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4080,7 +4080,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.1278</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4092,7 +4092,7 @@
         <v>15.11</v>
       </c>
       <c r="P44" t="n">
-        <v>27.96</v>
+        <v>27.8</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 0.74, 'earningsLow': 0.69, 'earningsHigh': 0.85, 'revenueAverage': 921494000, 'revenueLow': 806000000, 'revenueHigh': 996000000}</t>
+          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 0.73, 'earningsLow': 0.67, 'earningsHigh': 0.84, 'revenueAverage': 918860000, 'revenueLow': 865000000, 'revenueHigh': 1032000000}</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -4141,7 +4141,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>10.3</v>
+        <v>10.34</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4164,7 +4164,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>0.1144</t>
+          <t>0.1161</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -4225,7 +4225,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>8.1</v>
+        <v>8.17</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>0.2683</t>
+          <t>0.2693</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>7.42</v>
+        <v>7.51</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>0.20459999</t>
+          <t>0.2156</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -4344,7 +4344,7 @@
         <v>5.86</v>
       </c>
       <c r="P47" t="n">
-        <v>20.93</v>
+        <v>20.8</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': -0.03, 'earningsLow': -0.04, 'earningsHigh': -0.02, 'revenueAverage': 133997000, 'revenueLow': 130640000, 'revenueHigh': 134800000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': -0.09, 'earningsLow': -0.09, 'earningsHigh': -0.09, 'revenueAverage': 131280000, 'revenueLow': 127860000, 'revenueHigh': 134700000}</t>
         </is>
       </c>
       <c r="S47" t="inlineStr">
@@ -4380,7 +4380,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>10.89</v>
+        <v>10.7</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>0.17629999</t>
+          <t>0.17940001</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -4432,12 +4432,12 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>1.620901</t>
+          <t>{}</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-28'], 'earningsAverage': -0.01, 'earningsLow': -0.2, 'earningsHigh': 0.09, 'revenueAverage': 9850000, 'revenueLow': 4100000, 'revenueHigh': 15600000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': -0.01, 'earningsLow': -0.2, 'earningsHigh': 0.09, 'revenueAverage': 9850000, 'revenueLow': 4100000, 'revenueHigh': 15600000}</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
@@ -4468,25 +4468,25 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E49" t="n">
-        <v>4.54</v>
+        <v>3.69</v>
       </c>
       <c r="F49" t="n">
-        <v>908</v>
+        <v>369</v>
       </c>
       <c r="G49" t="n">
-        <v>5.37</v>
+        <v>5.43</v>
       </c>
       <c r="H49" t="n">
-        <v>1074</v>
+        <v>543</v>
       </c>
       <c r="I49" t="n">
         <v>4.8</v>
       </c>
       <c r="J49" t="n">
-        <v>4.99</v>
+        <v>4.06</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4561,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>3.02</v>
+        <v>3.04</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>0.1391</t>
+          <t>0.1382</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -4605,7 +4605,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-27', '2023-08-11'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 12100000, 'revenueLow': 12100000, 'revenueHigh': 12100000}</t>
+          <t>{'earningsDate': ['2023-07-31', '2023-08-11'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 12100000, 'revenueLow': 12100000, 'revenueHigh': 12100000}</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -4645,7 +4645,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>13.69</v>
+        <v>13.93</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>0.3989</t>
+          <t>0.4163</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.7, 'earningsLow': 0.54, 'earningsHigh': 0.89, 'revenueAverage': 24524500000, 'revenueLow': 23353500000, 'revenueHigh': 25915000000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.75, 'earningsLow': 0.54, 'earningsHigh': 0.93, 'revenueAverage': 24788400000, 'revenueLow': 23460700000, 'revenueHigh': 25915000000}</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
@@ -4716,7 +4716,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -4729,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>7.22</v>
+        <v>7.35</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -4747,12 +4747,12 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2023-05-25</t>
+          <t>2023-08-24</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.1175</t>
+          <t>0.068</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -4764,7 +4764,7 @@
         <v>5.99</v>
       </c>
       <c r="P52" t="n">
-        <v>13.83</v>
+        <v>13.68</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>20.525</v>
+        <v>20.62</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4836,7 +4836,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>0.1351</t>
+          <t>0.1345</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -4897,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>7.25</v>
+        <v>7.16</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -4920,7 +4920,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>0.1149</t>
+          <t>0.1146</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -4968,7 +4968,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -4981,7 +4981,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>3.7</v>
+        <v>3.81</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -4999,12 +4999,12 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>2023-08-04</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>0.14479999</t>
+          <t>0.1365</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02', '2023-08-07'], 'earningsAverage': 0.11, 'earningsLow': 0.09, 'earningsHigh': 0.14, 'revenueAverage': 14560000, 'revenueLow': 13720000, 'revenueHigh': 15480000}</t>
+          <t>{'earningsDate': ['2023-08-05'], 'earningsAverage': 0.11, 'earningsLow': 0.09, 'earningsHigh': 0.14, 'revenueAverage': 14560000, 'revenueLow': 13720000, 'revenueHigh': 15480000}</t>
         </is>
       </c>
       <c r="S55" t="inlineStr">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -5065,10 +5065,10 @@
         <v>1263.55</v>
       </c>
       <c r="G56" t="n">
-        <v>17.4</v>
+        <v>18.17</v>
       </c>
       <c r="H56" t="n">
-        <v>1287.6</v>
+        <v>1344.58</v>
       </c>
       <c r="I56" t="n">
         <v>17.05</v>
@@ -5149,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>10.14</v>
+        <v>10.07</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5233,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>9.09</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5313,7 +5313,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>12.41</v>
+        <v>12.49</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>0.1287</t>
+          <t>0.1289</t>
         </is>
       </c>
       <c r="N59" t="inlineStr">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -5397,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>14.62</v>
+        <v>14.6</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -5420,7 +5420,7 @@
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>0.1397</t>
+          <t>0.1409</t>
         </is>
       </c>
       <c r="N60" t="inlineStr">
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>7.66</v>
+        <v>7.77</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>0.1247</t>
+          <t>0.1236</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -5565,10 +5565,10 @@
         <v>281.915</v>
       </c>
       <c r="G62" t="n">
-        <v>255.71</v>
+        <v>266.44</v>
       </c>
       <c r="H62" t="n">
-        <v>255.71</v>
+        <v>266.44</v>
       </c>
       <c r="I62" t="n">
         <v>103.85</v>
@@ -5645,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>13.61</v>
+        <v>13.6</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>0.13229999</t>
+          <t>0.13239999</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
@@ -5680,7 +5680,7 @@
         <v>11.57</v>
       </c>
       <c r="P63" t="n">
-        <v>21.84</v>
+        <v>21.8</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
@@ -5729,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>9.539999999999999</v>
+        <v>9.75</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -5809,7 +5809,7 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="n">
-        <v>14.39</v>
+        <v>15.22</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
feat: balance sheet analysis
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -584,7 +584,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.1337</t>
+          <t>0.131</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.1341</t>
+          <t>0.1348</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-03'], 'earningsAverage': 0.35, 'earningsLow': 0.14, 'earningsHigh': 0.47, 'revenueAverage': 131466000000, 'revenueLow': 127000000000, 'revenueHigh': 133312000000}</t>
+          <t>{'earningsDate': ['2023-08-03'], 'earningsAverage': 0.32, 'earningsLow': 0.13, 'earningsHigh': 0.43, 'revenueAverage': 119161000000, 'revenueLow': 115113000000, 'revenueHigh': 120834000000}</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.1342</t>
+          <t>0.1349</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.23979999</t>
+          <t>0.2373</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.1238</t>
+          <t>0.12020001</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': -0.04, 'earningsLow': -0.04, 'earningsHigh': -0.04, 'revenueAverage': 130970000, 'revenueLow': 128000000, 'revenueHigh': 133000000}</t>
+          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': -0.04, 'earningsLow': -0.04, 'earningsHigh': -0.04, 'revenueAverage': 130970000, 'revenueLow': 128000000, 'revenueHigh': 133000000}</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0.122</t>
+          <t>0.1224</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.1161</t>
+          <t>0.119899996</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.17989999</t>
+          <t>0.1741</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>8.26</v>
+        <v>8.25</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.14310001</t>
+          <t>0.1481</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.1667</t>
+          <t>0.1617</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2880,7 +2880,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>0.18540001</t>
+          <t>0.1844</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 202410000, 'revenueLow': 199270000, 'revenueHigh': 205540000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 202350000, 'revenueLow': 199220000, 'revenueHigh': 205480000}</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -4920,7 +4920,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>0.1146</t>
+          <t>0.1187</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>0.0805</t>
+          <t>0.0771</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>0.1273</t>
+          <t>0.1291</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.81, 'earningsLow': 0.65, 'earningsHigh': 1.02, 'revenueAverage': 24715200000, 'revenueLow': 20270000000, 'revenueHigh': 27284000000}</t>
+          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.73, 'earningsLow': 0.59, 'earningsHigh': 0.92, 'revenueAverage': 22401900000, 'revenueLow': 18372700000, 'revenueHigh': 24730200000}</t>
         </is>
       </c>
       <c r="S62" t="inlineStr">
@@ -5716,7 +5716,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D64" t="n">

</xml_diff>

<commit_message>
chore: upgrade project lib
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>6.87</v>
+        <v>6.88</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -645,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>10.59</v>
+        <v>10.69</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.1342</t>
+          <t>0.1284</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -682,7 +682,11 @@
       <c r="P3" t="n">
         <v>14.01</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>1.429511</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr">
         <is>
           <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.27, 'earningsLow': 0.13, 'earningsHigh': 0.34, 'revenueAverage': 27920000, 'revenueLow': 25000000, 'revenueHigh': 29500000}</t>
@@ -725,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>13.79</v>
+        <v>13.37</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -748,7 +752,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.1423</t>
+          <t>0.1392</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
@@ -805,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>12.8</v>
+        <v>12.5</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -828,7 +832,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.1345</t>
+          <t>0.1318</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -889,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>9.91</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -912,7 +916,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.1434</t>
+          <t>0.1453</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -973,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>6.79</v>
+        <v>6.83</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1010,7 +1014,11 @@
       <c r="P7" t="n">
         <v>10.6</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1.773467</t>
+        </is>
+      </c>
       <c r="R7" t="inlineStr">
         <is>
           <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 7630000, 'revenueLow': 7000000, 'revenueHigh': 8390000}</t>
@@ -1053,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>9.399900000000001</v>
+        <v>9.569800000000001</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1076,7 +1084,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.3158</t>
+          <t>0.3339</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1090,11 +1098,7 @@
       <c r="P8" t="n">
         <v>14.79</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>1.271006</t>
-        </is>
-      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
           <t>{'earningsDate': [], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
@@ -1137,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>139.57</v>
+        <v>142.22</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1205,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>9.109999999999999</v>
+        <v>9.25</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1285,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>10.72</v>
+        <v>10.82</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1308,7 +1312,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.133</t>
+          <t>0.1306</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1369,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>19.41</v>
+        <v>19.51</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1449,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>5.11</v>
+        <v>5.09</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1533,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1613,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>8.43</v>
+        <v>8.48</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1697,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>4.96</v>
+        <v>5.06</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1781,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>9.91</v>
+        <v>9.75</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1861,10 +1865,10 @@
         <v>101.22</v>
       </c>
       <c r="G18" t="n">
-        <v>8.119999999999999</v>
+        <v>8.18</v>
       </c>
       <c r="H18" t="n">
-        <v>113.68</v>
+        <v>114.52</v>
       </c>
       <c r="I18" t="n">
         <v>6.3</v>
@@ -1884,7 +1888,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.1447</t>
+          <t>0.1515</t>
         </is>
       </c>
       <c r="N18" t="inlineStr"/>
@@ -1941,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>4.18</v>
+        <v>4.15</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1964,7 +1968,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0.1392</t>
+          <t>0.1435</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1973,12 +1977,16 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>4.1</v>
+        <v>4.09</v>
       </c>
       <c r="P19" t="n">
         <v>7.24</v>
       </c>
-      <c r="Q19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>1.295808</t>
+        </is>
+      </c>
       <c r="R19" t="inlineStr">
         <is>
           <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.21, 'earningsLow': 0.21, 'earningsHigh': 0.21, 'revenueAverage': 6150000, 'revenueLow': 6150000, 'revenueHigh': 6150000}</t>
@@ -2021,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>6.02</v>
+        <v>5.93</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2058,7 +2066,11 @@
       <c r="P20" t="n">
         <v>9.65</v>
       </c>
-      <c r="Q20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>1.623138</t>
+        </is>
+      </c>
       <c r="R20" t="inlineStr">
         <is>
           <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 0.18, 'earningsLow': 0.12, 'earningsHigh': 0.23, 'revenueAverage': 82610000, 'revenueLow': 69430000, 'revenueHigh': 93400000}</t>
@@ -2101,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>10.97</v>
+        <v>10.99</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2177,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>11.19</v>
+        <v>11.25</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2208,12 +2220,12 @@
         <v>10.08</v>
       </c>
       <c r="P22" t="n">
-        <v>18.96</v>
+        <v>18.88</v>
       </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-02'], 'earningsAverage': 0.33, 'earningsLow': 0.14, 'earningsHigh': 0.43, 'revenueAverage': 77420000, 'revenueLow': 74000000, 'revenueHigh': 81770000}</t>
+          <t>{'earningsDate': ['2023-11-07', '2023-11-11'], 'earningsAverage': 0.33, 'earningsLow': 0.14, 'earningsHigh': 0.43, 'revenueAverage': 77420000, 'revenueLow': 74000000, 'revenueHigh': 81770000}</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2253,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>8.380000000000001</v>
+        <v>8.44</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2276,7 +2288,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>0.1656</t>
+          <t>0.168</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2337,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>4.02</v>
+        <v>4.011</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2421,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>3.92</v>
+        <v>3.95</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2497,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>7.05</v>
+        <v>7.03</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2568,7 +2580,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -2581,10 +2593,10 @@
         <v>153.75</v>
       </c>
       <c r="G27" t="n">
-        <v>10.29</v>
+        <v>10.44</v>
       </c>
       <c r="H27" t="n">
-        <v>154.35</v>
+        <v>156.6</v>
       </c>
       <c r="I27" t="n">
         <v>10.12</v>
@@ -2604,7 +2616,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.16219999</t>
+          <t>0.1633</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2665,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>13.31</v>
+        <v>13.37</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -2688,7 +2700,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.1331</t>
+          <t>0.13520001</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2709,7 +2721,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-07'], 'earningsAverage': 0.44, 'earningsLow': 0.37, 'earningsHigh': 0.48, 'revenueAverage': 45620000, 'revenueLow': 26550000, 'revenueHigh': 75200000}</t>
+          <t>{'earningsDate': ['2023-08-08'], 'earningsAverage': 0.44, 'earningsLow': 0.37, 'earningsHigh': 0.48, 'revenueAverage': 45620000, 'revenueLow': 26550000, 'revenueHigh': 75200000}</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -2749,10 +2761,10 @@
         <v>42</v>
       </c>
       <c r="G29" t="n">
-        <v>44.76</v>
+        <v>45.48</v>
       </c>
       <c r="H29" t="n">
-        <v>44.76</v>
+        <v>45.48</v>
       </c>
       <c r="I29" t="n">
         <v>39.28</v>
@@ -2829,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>5.91</v>
+        <v>5.86</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2852,7 +2864,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>0.1366</t>
+          <t>0.1402</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2913,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>17.24</v>
+        <v>17.26</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2993,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>20.21</v>
+        <v>20.41</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3016,7 +3028,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0.1385</t>
+          <t>0.1372</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3037,7 +3049,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-07'], 'earningsAverage': 0.75, 'earningsLow': 0.75, 'earningsHigh': 0.78, 'revenueAverage': 447050000, 'revenueLow': 438000000, 'revenueHigh': 453250000}</t>
+          <t>{'earningsDate': ['2023-08-08'], 'earningsAverage': 0.75, 'earningsLow': 0.75, 'earningsHigh': 0.78, 'revenueAverage': 447050000, 'revenueLow': 438000000, 'revenueHigh': 453250000}</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -3077,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>9.550000000000001</v>
+        <v>9.56</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3100,7 +3112,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>0.1673</t>
+          <t>0.15689999</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -3112,7 +3124,7 @@
         <v>7.51</v>
       </c>
       <c r="P33" t="n">
-        <v>12.305</v>
+        <v>12.25</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
@@ -3161,7 +3173,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>5.73</v>
+        <v>5.6</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3245,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>6.24</v>
+        <v>6.28</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -3268,7 +3280,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>0.1397</t>
+          <t>0.1401</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -3316,7 +3328,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -3329,10 +3341,10 @@
         <v>70.75</v>
       </c>
       <c r="G36" t="n">
-        <v>13.94</v>
+        <v>14.01</v>
       </c>
       <c r="H36" t="n">
-        <v>69.7</v>
+        <v>70.05</v>
       </c>
       <c r="I36" t="n">
         <v>12.41</v>
@@ -3347,12 +3359,12 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2023-05-15</t>
+          <t>2023-08-15</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>0.1385</t>
+          <t>0.112799995</t>
         </is>
       </c>
       <c r="N36" t="inlineStr"/>
@@ -3369,7 +3381,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-04'], 'earningsAverage': 0.24, 'earningsLow': 0.13, 'earningsHigh': 0.4, 'revenueAverage': 68290000, 'revenueLow': 58390000, 'revenueHigh': 98920000}</t>
+          <t>{'earningsDate': ['2023-11-07', '2023-11-13'], 'earningsAverage': 0.24, 'earningsLow': 0.13, 'earningsHigh': 0.4, 'revenueAverage': 68290000, 'revenueLow': 58390000, 'revenueHigh': 98920000}</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3409,7 +3421,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>10.62</v>
+        <v>11.12</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3493,10 +3505,10 @@
         <v>1023.26</v>
       </c>
       <c r="G38" t="n">
-        <v>7.65</v>
+        <v>7.71</v>
       </c>
       <c r="H38" t="n">
-        <v>1071</v>
+        <v>1079.4</v>
       </c>
       <c r="I38" t="n">
         <v>7.06</v>
@@ -3516,7 +3528,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>0.1619</t>
+          <t>0.1634</t>
         </is>
       </c>
       <c r="N38" t="inlineStr"/>
@@ -3573,10 +3585,10 @@
         <v>418.988</v>
       </c>
       <c r="G39" t="n">
-        <v>128.11</v>
+        <v>131.53</v>
       </c>
       <c r="H39" t="n">
-        <v>512.4400000000001</v>
+        <v>526.12</v>
       </c>
       <c r="I39" t="n">
         <v>85.01000000000001</v>
@@ -3641,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>5.67</v>
+        <v>5.63</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -3725,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>8.59</v>
+        <v>8.33</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -3805,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>6.03</v>
+        <v>6.55</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -3889,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>3.87</v>
+        <v>3.9352</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -3973,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>25.09</v>
+        <v>23.66</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -3996,7 +4008,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.3189</t>
+          <t>0.1691</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4057,7 +4069,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>11.43</v>
+        <v>11.65</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4080,7 +4092,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>0.13319999</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -4092,7 +4104,7 @@
         <v>9.48</v>
       </c>
       <c r="P45" t="n">
-        <v>17.95</v>
+        <v>17.73</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
@@ -4141,7 +4153,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>1.37</v>
+        <v>1.33</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4164,7 +4176,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>0.3964</t>
+          <t>0.33080003</t>
         </is>
       </c>
       <c r="N46" t="inlineStr"/>
@@ -4221,10 +4233,10 @@
         <v>1647.513</v>
       </c>
       <c r="G47" t="n">
-        <v>25.605</v>
+        <v>25.85</v>
       </c>
       <c r="H47" t="n">
-        <v>1766.745</v>
+        <v>1783.65</v>
       </c>
       <c r="I47" t="n">
         <v>23.01</v>
@@ -4301,7 +4313,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>12.46</v>
+        <v>12.51</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4385,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>5.34</v>
+        <v>5.3</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -4408,7 +4420,7 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>0.184</t>
+          <t>0.1895</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
@@ -4469,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>6.52</v>
+        <v>6.47</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -4549,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1.71</v>
+        <v>1.61</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -4629,7 +4641,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>10.79</v>
+        <v>10.83</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -4652,7 +4664,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.1244</t>
+          <t>0.1246</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -4664,9 +4676,13 @@
         <v>7.15</v>
       </c>
       <c r="P52" t="n">
-        <v>12.54</v>
-      </c>
-      <c r="Q52" t="inlineStr"/>
+        <v>12.38</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>1.980256</t>
+        </is>
+      </c>
       <c r="R52" t="inlineStr">
         <is>
           <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 0.37, 'earningsLow': 0.32, 'earningsHigh': 0.42, 'revenueAverage': 50600000, 'revenueLow': 39500000, 'revenueHigh': 59100000}</t>
@@ -4709,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>18.72</v>
+        <v>18.5</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4789,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>4.33</v>
+        <v>4.34</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -4812,7 +4828,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>0.13859999</t>
+          <t>0.1382</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -4873,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>5.8401</v>
+        <v>5.87</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -4957,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>19.83</v>
+        <v>19.96</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -4980,7 +4996,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>0.1299</t>
+          <t>0.1311</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -5041,7 +5057,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>9.17</v>
+        <v>9.08</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5125,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>7.815</v>
+        <v>7.92</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5205,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>7.43</v>
+        <v>8.1</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5228,7 +5244,7 @@
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>0.2171</t>
+          <t>0.21530001</t>
         </is>
       </c>
       <c r="N59" t="inlineStr">
@@ -5289,7 +5305,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>10.03</v>
+        <v>10.2</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -5373,10 +5389,10 @@
         <v>369</v>
       </c>
       <c r="G61" t="n">
-        <v>5.65</v>
+        <v>5.54</v>
       </c>
       <c r="H61" t="n">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="I61" t="n">
         <v>4.8</v>
@@ -5457,7 +5473,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>3.04</v>
+        <v>3.02</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -5480,7 +5496,7 @@
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>0.1373</t>
+          <t>0.1368</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
@@ -5541,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>13.52</v>
+        <v>13.47</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -5564,7 +5580,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>0.41279998</t>
+          <t>0.42900002</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
@@ -5621,7 +5637,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>7.18</v>
+        <v>7.21</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -5644,7 +5660,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>0.0686</t>
+          <t>0.0696</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -5705,7 +5721,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>20.81</v>
+        <v>20.7</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -5728,7 +5744,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>0.1336</t>
+          <t>0.1333</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -5785,7 +5801,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>7.04</v>
+        <v>7.33</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -5865,7 +5881,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>7.76</v>
+        <v>7.78</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -5888,7 +5904,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>0.0856</t>
+          <t>0.0825</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -5949,7 +5965,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>3.48</v>
+        <v>3.4</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -5972,7 +5988,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.134</t>
+          <t>0.1494</t>
         </is>
       </c>
       <c r="N68" t="inlineStr">
@@ -5984,7 +6000,7 @@
         <v>2.985</v>
       </c>
       <c r="P68" t="n">
-        <v>5.12</v>
+        <v>5.105</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
@@ -6033,10 +6049,10 @@
         <v>1263.55</v>
       </c>
       <c r="G69" t="n">
-        <v>18.28</v>
+        <v>18.54</v>
       </c>
       <c r="H69" t="n">
-        <v>1352.72</v>
+        <v>1371.96</v>
       </c>
       <c r="I69" t="n">
         <v>17.05</v>
@@ -6113,7 +6129,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>10.47</v>
+        <v>10.56</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -6136,7 +6152,7 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.1242</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
@@ -6197,7 +6213,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>36.55</v>
+        <v>38.04</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -6281,7 +6297,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>9.5</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -6349,7 +6365,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>11.43</v>
+        <v>11.32</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -6429,7 +6445,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>14.12</v>
+        <v>14.17</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -6532,7 +6548,7 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>0.1399</t>
+          <t>0.1341</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
@@ -6593,10 +6609,10 @@
         <v>281.915</v>
       </c>
       <c r="G76" t="n">
-        <v>253.86</v>
+        <v>251.45</v>
       </c>
       <c r="H76" t="n">
-        <v>253.86</v>
+        <v>251.45</v>
       </c>
       <c r="I76" t="n">
         <v>103.85</v>
@@ -6661,7 +6677,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>13.57</v>
+        <v>13.71</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -6745,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>9.91</v>
+        <v>10.13</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -6768,7 +6784,7 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>0.1417</t>
+          <t>0.1442</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
@@ -6780,7 +6796,7 @@
         <v>7</v>
       </c>
       <c r="P78" t="n">
-        <v>15.84</v>
+        <v>15.8</v>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
@@ -6789,7 +6805,7 @@
       </c>
       <c r="R78" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-07', '2023-08-14'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 5330000, 'revenueLow': 5330000, 'revenueHigh': 5330000}</t>
+          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 5330000, 'revenueLow': 5330000, 'revenueHigh': 5330000}</t>
         </is>
       </c>
       <c r="S78" t="inlineStr">
@@ -6829,7 +6845,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>15.04</v>
+        <v>14.5</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
feat: update target prices
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T79"/>
+  <dimension ref="A1:U79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,11 @@
           <t>yahoo_finance_url</t>
         </is>
       </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>long_name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -561,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>6.93</v>
+        <v>6.95</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -618,6 +623,11 @@
           <t>https://finance.yahoo.com/quote/ACP?p=ACP</t>
         </is>
       </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>ACP-Aberdeen Income Credit Strategi</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -645,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>10.06</v>
+        <v>10.145</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -702,6 +712,11 @@
           <t>https://finance.yahoo.com/quote/ACRE?p=ACRE</t>
         </is>
       </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>ACRE-Ares Commercial Real Estate Cor</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -729,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>13.07</v>
+        <v>13.2454</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -782,6 +797,11 @@
           <t>https://finance.yahoo.com/quote/AFCG?p=AFCG</t>
         </is>
       </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>AFCG-AFC Gamma, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -866,6 +886,11 @@
           <t>https://finance.yahoo.com/quote/AFSIA?p=AFSIA</t>
         </is>
       </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AFSIA-AMTRUST FINANCIAL SERVICES INC </t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -893,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>9.99</v>
+        <v>10.0599</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -950,6 +975,11 @@
           <t>https://finance.yahoo.com/quote/AGNC?p=AGNC</t>
         </is>
       </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>AGNC-AGNC Investment Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -977,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>6.61</v>
+        <v>6.675</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1034,6 +1064,11 @@
           <t>https://finance.yahoo.com/quote/AJX?p=AJX</t>
         </is>
       </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>AJX-Great Ajax Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1061,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>9.390000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1118,6 +1153,11 @@
           <t>https://finance.yahoo.com/quote/AMKBY?p=AMKBY</t>
         </is>
       </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>AMKBY-A.P. MOLLER - MAERSK UNSP ADR E</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1145,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>133.14</v>
+        <v>134.23</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1173,7 +1213,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.54, 'earningsLow': 0.41, 'earningsHigh': 0.66, 'revenueAverage': 130982000000, 'revenueLow': 127829000000, 'revenueHigh': 132640000000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.58, 'earningsLow': 0.44, 'earningsHigh': 0.71, 'revenueAverage': 141403000000, 'revenueLow': 138000000000, 'revenueHigh': 143193000000}</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1184,6 +1224,11 @@
       <c r="T9" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/AMZN?p=AMZN</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>AMZN-Amazon.com, Inc.</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>9.140000000000001</v>
+        <v>9.31</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1266,6 +1311,11 @@
           <t>https://finance.yahoo.com/quote/AOMR?p=AOMR</t>
         </is>
       </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>AOMR-Angel Oak Mortgage REIT, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1293,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>10.71</v>
+        <v>10.83</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1350,6 +1400,11 @@
           <t>https://finance.yahoo.com/quote/ARI?p=ARI</t>
         </is>
       </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>ARI-Apollo Commercial Real Estate F</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1377,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>20.13</v>
+        <v>20.158</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1430,6 +1485,11 @@
           <t>https://finance.yahoo.com/quote/ARLP?p=ARLP</t>
         </is>
       </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>ARLP-Alliance Resource Partners, L.P</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1457,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>5.02</v>
+        <v>5.04</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1514,6 +1574,11 @@
           <t>https://finance.yahoo.com/quote/ARR?p=ARR</t>
         </is>
       </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>ARR-ARMOUR Residential REIT, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1541,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>10</v>
+        <v>9.875</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1594,6 +1659,11 @@
           <t>https://finance.yahoo.com/quote/AVACF?p=AVACF</t>
         </is>
       </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>AVACF-AVANCE GAS HOLDING LIMITED</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1621,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>9.220000000000001</v>
+        <v>9.27</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1678,6 +1748,11 @@
           <t>https://finance.yahoo.com/quote/BBDC?p=BBDC</t>
         </is>
       </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>BBDC-Barings BDC, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1705,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>4.83</v>
+        <v>4.94</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1762,6 +1837,11 @@
           <t>https://finance.yahoo.com/quote/BDN?p=BDN</t>
         </is>
       </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>BDN-Brandywine Realty Trust</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1789,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>6.28</v>
+        <v>7.9204</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1829,7 +1909,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-29'], 'earningsAverage': -4.12, 'earningsLow': -4.59, 'earningsHigh': -3.65, 'revenueAverage': 1100770000, 'revenueLow': 1093100000, 'revenueHigh': 1107940000}</t>
+          <t>{'earningsDate': ['2023-08-29'], 'earningsAverage': -4.12, 'earningsLow': -4.59, 'earningsHigh': -3.65, 'revenueAverage': 1100980000, 'revenueLow': 1093100000, 'revenueHigh': 1107940000}</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -1840,6 +1920,11 @@
       <c r="T17" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/BIG?p=BIG</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>BIG-Big Lots, Inc.</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>8.42</v>
+        <v>8.435</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1922,6 +2007,11 @@
           <t>https://finance.yahoo.com/quote/BRY?p=BRY</t>
         </is>
       </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>BRY-Berry Corporation (bry)</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1949,10 +2039,10 @@
         <v>1446.798</v>
       </c>
       <c r="G19" t="n">
-        <v>3.94</v>
+        <v>3.965</v>
       </c>
       <c r="H19" t="n">
-        <v>1442.04</v>
+        <v>1451.19</v>
       </c>
       <c r="I19" t="n">
         <v>4.14</v>
@@ -2006,6 +2096,11 @@
           <t>https://finance.yahoo.com/quote/CHMI?p=CHMI</t>
         </is>
       </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>CHMI-Cherry Hill Mortgage Investment</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2033,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>5.95</v>
+        <v>5.965</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2090,6 +2185,11 @@
           <t>https://finance.yahoo.com/quote/CIM?p=CIM</t>
         </is>
       </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>CIM-Chimera Investment Corporation</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2117,7 +2217,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>10.8</v>
+        <v>10.83</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2166,6 +2266,11 @@
           <t>https://finance.yahoo.com/quote/CION?p=CION</t>
         </is>
       </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>CION-CION Investment Corporation</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2193,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>11.06</v>
+        <v>11.135</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2242,6 +2347,11 @@
           <t>https://finance.yahoo.com/quote/CMTG?p=CMTG</t>
         </is>
       </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>CMTG-Claros Mortgage Trust, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2269,7 +2379,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>7.98</v>
+        <v>7.985</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2326,6 +2436,11 @@
           <t>https://finance.yahoo.com/quote/CRF?p=CRF</t>
         </is>
       </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>CRF-33138</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2353,7 +2468,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>3.84</v>
+        <v>3.85</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2410,6 +2525,11 @@
           <t>https://finance.yahoo.com/quote/CUBA?p=CUBA</t>
         </is>
       </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>CUBA-The Herzfeld Caribbean Basin Fu</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2424,7 +2544,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2437,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>3.57</v>
+        <v>3.635</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2486,6 +2606,11 @@
           <t>https://finance.yahoo.com/quote/DSX?p=DSX</t>
         </is>
       </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>DSX-Diana Shipping inc.</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2513,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>6.64</v>
+        <v>6.69</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2570,6 +2695,11 @@
           <t>https://finance.yahoo.com/quote/EARN?p=EARN</t>
         </is>
       </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EARN-Ellington Residential Mortgage </t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2597,10 +2727,10 @@
         <v>153.75</v>
       </c>
       <c r="G27" t="n">
-        <v>10.28</v>
+        <v>10.292</v>
       </c>
       <c r="H27" t="n">
-        <v>154.2</v>
+        <v>154.38</v>
       </c>
       <c r="I27" t="n">
         <v>10.12</v>
@@ -2654,6 +2784,11 @@
           <t>https://finance.yahoo.com/quote/ECC?p=ECC</t>
         </is>
       </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>ECC-Eagle Point Credit Company Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2681,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>13.32</v>
+        <v>13.41</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -2738,6 +2873,11 @@
           <t>https://finance.yahoo.com/quote/EFC?p=EFC</t>
         </is>
       </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>EFC-Ellington Financial Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2765,10 +2905,10 @@
         <v>42</v>
       </c>
       <c r="G29" t="n">
-        <v>41.7</v>
+        <v>43.145</v>
       </c>
       <c r="H29" t="n">
-        <v>41.7</v>
+        <v>43.145</v>
       </c>
       <c r="I29" t="n">
         <v>39.28</v>
@@ -2818,6 +2958,11 @@
           <t>https://finance.yahoo.com/quote/EGLE?p=EGLE</t>
         </is>
       </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>EGLE-Eagle Bulk Shipping Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2845,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>5.97</v>
+        <v>6.01</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2902,6 +3047,11 @@
           <t>https://finance.yahoo.com/quote/FCO?p=FCO</t>
         </is>
       </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>FCO-17210</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2929,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>18.14</v>
+        <v>18.41</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2982,6 +3132,11 @@
           <t>https://finance.yahoo.com/quote/FRO?p=FRO</t>
         </is>
       </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>FRO-Frontline Plc</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3009,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>20.14</v>
+        <v>20.2126</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3066,6 +3221,11 @@
           <t>https://finance.yahoo.com/quote/FSK?p=FSK</t>
         </is>
       </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>FSK-FS KKR Capital Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3093,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>10.25</v>
+        <v>10.23</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3150,6 +3310,11 @@
           <t>https://finance.yahoo.com/quote/GECC?p=GECC</t>
         </is>
       </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>GECC-Great Elm Capital Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3177,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>5.15</v>
+        <v>5.2282</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3221,7 +3386,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.26, 'earningsLow': 0.24, 'earningsHigh': 0.27, 'revenueAverage': 4064920000, 'revenueLow': 4064920000, 'revenueHigh': 4064920000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.26, 'earningsLow': 0.24, 'earningsHigh': 0.28, 'revenueAverage': 4073180000, 'revenueLow': 4073180000, 'revenueHigh': 4073180000}</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -3232,6 +3397,11 @@
       <c r="T34" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/GGB?p=GGB</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>GGB-Gerdau S.A.</t>
         </is>
       </c>
     </row>
@@ -3261,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>6.03</v>
+        <v>6.0741</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -3318,6 +3488,11 @@
           <t>https://finance.yahoo.com/quote/GGT?p=GGT</t>
         </is>
       </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>GGT-Gabelli Multi-Media Trust, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3345,10 +3520,10 @@
         <v>70.75</v>
       </c>
       <c r="G36" t="n">
-        <v>13.61</v>
+        <v>13.88</v>
       </c>
       <c r="H36" t="n">
-        <v>68.05</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="I36" t="n">
         <v>12.41</v>
@@ -3398,6 +3573,11 @@
           <t>https://finance.yahoo.com/quote/GNK?p=GNK</t>
         </is>
       </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>GNK-Genco Shipping &amp; Trading Limite</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3425,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>10.95</v>
+        <v>11.0577</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3482,6 +3662,11 @@
           <t>https://finance.yahoo.com/quote/GNL?p=GNL</t>
         </is>
       </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>GNL-Global Net Lease, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3496,7 +3681,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -3509,10 +3694,10 @@
         <v>1023.26</v>
       </c>
       <c r="G38" t="n">
-        <v>6.9</v>
+        <v>7.22</v>
       </c>
       <c r="H38" t="n">
-        <v>966</v>
+        <v>1010.8</v>
       </c>
       <c r="I38" t="n">
         <v>7.06</v>
@@ -3562,6 +3747,11 @@
           <t>https://finance.yahoo.com/quote/GOGL?p=GOGL</t>
         </is>
       </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>GOGL-Golden Ocean Group Limited</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3576,23 +3766,23 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
         <v>104.747</v>
       </c>
       <c r="F39" t="n">
-        <v>418.988</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>131.01</v>
+        <v>134.445</v>
       </c>
       <c r="H39" t="n">
-        <v>524.04</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
         <v>85.01000000000001</v>
@@ -3608,7 +3798,7 @@
         <v>83.34</v>
       </c>
       <c r="P39" t="n">
-        <v>134.25</v>
+        <v>134.74</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
@@ -3617,7 +3807,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.33, 'earningsLow': 1.18, 'earningsHigh': 1.44, 'revenueAverage': 70297200000, 'revenueLow': 67493000000, 'revenueHigh': 72179800000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.44, 'earningsLow': 1.27, 'earningsHigh': 1.55, 'revenueAverage': 75890300000, 'revenueLow': 72863000000, 'revenueHigh': 77922700000}</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -3628,6 +3818,11 @@
       <c r="T39" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/GOOGL?p=GOOGL</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>GOOGL-Alphabet Inc.</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>5.27</v>
+        <v>5.31</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -3714,6 +3909,11 @@
           <t>https://finance.yahoo.com/quote/GPMT?p=GPMT</t>
         </is>
       </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>GPMT-Granite Point Mortgage Trust In</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3741,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>8.01</v>
+        <v>8.17</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -3794,6 +3994,11 @@
           <t>https://finance.yahoo.com/quote/GRIN?p=GRIN</t>
         </is>
       </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>GRIN-Grindrod Shipping Holdings Ltd.</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3821,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>6.49</v>
+        <v>6.805</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -3878,6 +4083,11 @@
           <t>https://finance.yahoo.com/quote/HPP?p=HPP</t>
         </is>
       </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>HPP-Hudson Pacific Properties, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3962,6 +4172,11 @@
           <t>https://finance.yahoo.com/quote/ICMB?p=ICMB</t>
         </is>
       </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>ICMB-Investcorp Credit Management BD</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3989,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>19.45</v>
+        <v>19.76</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4046,6 +4261,11 @@
           <t>https://finance.yahoo.com/quote/IEP?p=IEP</t>
         </is>
       </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>IEP-Icahn Enterprises L.P. - Deposi</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4073,7 +4293,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>11.14</v>
+        <v>11.3</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4130,6 +4350,11 @@
           <t>https://finance.yahoo.com/quote/IVR?p=IVR</t>
         </is>
       </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>IVR-INVESCO MORTGAGE CAPITAL INC</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4157,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>1.16</v>
+        <v>1.018</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4197,7 +4422,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-28'], 'earningsAverage': -1.15, 'earningsLow': -1.33, 'earningsHigh': -0.87, 'revenueAverage': 437440000, 'revenueLow': 427000000, 'revenueHigh': 447100000}</t>
+          <t>{'earningsDate': ['2023-08-28'], 'earningsAverage': -0.21, 'earningsLow': -0.38, 'earningsHigh': -0.07, 'revenueAverage': 539720000, 'revenueLow': 530000000, 'revenueHigh': 547200000}</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4208,6 +4433,11 @@
       <c r="T46" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/JOAN?p=JOAN</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>JOAN-JOANN, Inc.</t>
         </is>
       </c>
     </row>
@@ -4237,10 +4467,10 @@
         <v>1647.513</v>
       </c>
       <c r="G47" t="n">
-        <v>23.86</v>
+        <v>24.03</v>
       </c>
       <c r="H47" t="n">
-        <v>1646.34</v>
+        <v>1658.07</v>
       </c>
       <c r="I47" t="n">
         <v>23.01</v>
@@ -4290,6 +4520,11 @@
           <t>https://finance.yahoo.com/quote/KEN?p=KEN</t>
         </is>
       </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>KEN-Kenon Holdings Ltd.</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4317,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>12.11</v>
+        <v>12.2369</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4374,6 +4609,11 @@
           <t>https://finance.yahoo.com/quote/KREF?p=KREF</t>
         </is>
       </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>KREF-KKR Real Estate Finance Trust I</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4401,7 +4641,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>5.03</v>
+        <v>5.035</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -4458,6 +4698,11 @@
           <t>https://finance.yahoo.com/quote/LND?p=LND</t>
         </is>
       </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>LND-Brasilagro Brazilian Agric Real</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4485,7 +4730,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>6.58</v>
+        <v>6.698</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -4538,6 +4783,11 @@
           <t>https://finance.yahoo.com/quote/LOMA?p=LOMA</t>
         </is>
       </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LOMA-Loma Negra Compania Industrial </t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4565,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1.19</v>
+        <v>1.275</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -4618,6 +4868,11 @@
           <t>https://finance.yahoo.com/quote/LU?p=LU</t>
         </is>
       </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>LU-Lufax Holding Ltd</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4645,7 +4900,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>10.86</v>
+        <v>10.96</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -4702,6 +4957,11 @@
           <t>https://finance.yahoo.com/quote/MFA?p=MFA</t>
         </is>
       </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>MFA-MFA Financial, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4729,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>19.14</v>
+        <v>18.9827</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -4782,6 +5042,11 @@
           <t>https://finance.yahoo.com/quote/MSB?p=MSB</t>
         </is>
       </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>MSB-Mesabi Trust</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4809,7 +5074,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>3.97</v>
+        <v>4.09</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -4853,7 +5118,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-28', '2023-12-04'], 'earningsAverage': 0.14, 'earningsLow': 0.1, 'earningsHigh': 0.16, 'revenueAverage': 68320000, 'revenueLow': 60540000, 'revenueHigh': 73000000}</t>
+          <t>{'earningsDate': ['2023-11-28', '2023-12-04'], 'earningsAverage': 0.13, 'earningsLow': 0.1, 'earningsHigh': 0.16, 'revenueAverage': 74360000, 'revenueLow': 60540000, 'revenueHigh': 99100000}</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
@@ -4864,6 +5129,11 @@
       <c r="T54" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/NAT?p=NAT</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>NAT-Nordic American Tankers Limited</t>
         </is>
       </c>
     </row>
@@ -4893,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>5.32</v>
+        <v>5.41</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -4950,6 +5220,11 @@
           <t>https://finance.yahoo.com/quote/NHTC?p=NHTC</t>
         </is>
       </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>NHTC-Natural Health Trends Corp. - C</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4977,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>20.26</v>
+        <v>20.3824</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -5034,6 +5309,11 @@
           <t>https://finance.yahoo.com/quote/NLY?p=NLY</t>
         </is>
       </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>NLY-Annaly Capital Management Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5061,7 +5341,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>9.460000000000001</v>
+        <v>9.545</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5118,6 +5398,11 @@
           <t>https://finance.yahoo.com/quote/NYMT?p=NYMT</t>
         </is>
       </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>NYMT-New York Mortgage Trust, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5145,10 +5430,10 @@
         <v>3243.66</v>
       </c>
       <c r="G58" t="n">
-        <v>8.09</v>
+        <v>8.1099</v>
       </c>
       <c r="H58" t="n">
-        <v>3397.8</v>
+        <v>3406.158</v>
       </c>
       <c r="I58" t="n">
         <v>8.01</v>
@@ -5198,6 +5483,11 @@
           <t>https://finance.yahoo.com/quote/OCCI?p=OCCI</t>
         </is>
       </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>OCCI-OFS Credit Company, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5225,7 +5515,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>7.24</v>
+        <v>7.375</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5282,6 +5572,11 @@
           <t>https://finance.yahoo.com/quote/OPI?p=OPI</t>
         </is>
       </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>OPI-Office Properties Income Trust</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5296,7 +5591,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -5309,10 +5604,10 @@
         <v>599.6799999999999</v>
       </c>
       <c r="G60" t="n">
-        <v>9.75</v>
+        <v>9.82</v>
       </c>
       <c r="H60" t="n">
-        <v>624</v>
+        <v>628.48</v>
       </c>
       <c r="I60" t="n">
         <v>9.5</v>
@@ -5366,6 +5661,11 @@
           <t>https://finance.yahoo.com/quote/ORC?p=ORC</t>
         </is>
       </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>ORC-Orchid Island Capital, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5393,10 +5693,10 @@
         <v>369</v>
       </c>
       <c r="G61" t="n">
-        <v>5.01</v>
+        <v>4.9999</v>
       </c>
       <c r="H61" t="n">
-        <v>501</v>
+        <v>499.99</v>
       </c>
       <c r="I61" t="n">
         <v>4.8</v>
@@ -5450,6 +5750,11 @@
           <t>https://finance.yahoo.com/quote/OXLC?p=OXLC</t>
         </is>
       </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>OXLC-Oxford Lane Capital Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5477,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>3.15</v>
+        <v>3.23</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -5534,6 +5839,11 @@
           <t>https://finance.yahoo.com/quote/OXSQ?p=OXSQ</t>
         </is>
       </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>OXSQ-Oxford Square Capital Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5561,7 +5871,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>14.5</v>
+        <v>14.5609</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -5618,6 +5928,11 @@
           <t>https://finance.yahoo.com/quote/PBR?p=PBR</t>
         </is>
       </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>PBR-Petroleo Brasileiro S.A.- Petro</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5645,7 +5960,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>6.57</v>
+        <v>6.7</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -5702,6 +6017,11 @@
           <t>https://finance.yahoo.com/quote/PDM?p=PDM</t>
         </is>
       </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>PDM-Piedmont Office Realty Trust, I</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5716,7 +6036,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -5729,7 +6049,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>19.26</v>
+        <v>19.495</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -5786,6 +6106,11 @@
           <t>https://finance.yahoo.com/quote/PTMN?p=PTMN</t>
         </is>
       </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>PTMN-Portman Ridge Finance Corporati</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5813,7 +6138,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>7.22</v>
+        <v>7.32</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -5870,6 +6195,11 @@
           <t>https://finance.yahoo.com/quote/RTL?p=RTL</t>
         </is>
       </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>RTL-The Necessity Retail REIT, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5897,7 +6227,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>7.99</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -5954,6 +6284,11 @@
           <t>https://finance.yahoo.com/quote/RWT?p=RWT</t>
         </is>
       </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>RWT-Redwood Trust, Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5981,7 +6316,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>3.48</v>
+        <v>3.53</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -6038,6 +6373,11 @@
           <t>https://finance.yahoo.com/quote/SACH?p=SACH</t>
         </is>
       </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>SACH-Sachem Capital Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6065,10 +6405,10 @@
         <v>1263.55</v>
       </c>
       <c r="G69" t="n">
-        <v>17.08</v>
+        <v>17.48</v>
       </c>
       <c r="H69" t="n">
-        <v>1263.92</v>
+        <v>1293.52</v>
       </c>
       <c r="I69" t="n">
         <v>17.05</v>
@@ -6118,6 +6458,11 @@
           <t>https://finance.yahoo.com/quote/SBLK?p=SBLK</t>
         </is>
       </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>SBLK-Star Bulk Carriers Corp.</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6145,7 +6490,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>10.83</v>
+        <v>10.8676</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -6202,6 +6547,11 @@
           <t>https://finance.yahoo.com/quote/SEVN?p=SEVN</t>
         </is>
       </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>SEVN-Seven Hills Realty Trust</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6229,7 +6579,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>37.15</v>
+        <v>38.6</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -6286,6 +6636,11 @@
           <t>https://finance.yahoo.com/quote/SLG?p=SLG</t>
         </is>
       </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>SLG-SL Green Realty Corp</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6313,7 +6668,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>8.23</v>
+        <v>8.56</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -6341,7 +6696,7 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': -0.07, 'earningsLow': -0.1, 'earningsHigh': 0.0, 'revenueAverage': 508310000, 'revenueLow': 460050000, 'revenueHigh': 529700000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': -0.07, 'earningsLow': -0.1, 'earningsHigh': 0.0, 'revenueAverage': 508270000, 'revenueLow': 460050000, 'revenueHigh': 529700000}</t>
         </is>
       </c>
       <c r="S72" t="inlineStr">
@@ -6352,6 +6707,11 @@
       <c r="T72" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/SOFI?p=SOFI</t>
+        </is>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>SOFI-SoFi Technologies, Inc.</t>
         </is>
       </c>
     </row>
@@ -6381,7 +6741,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>10.98</v>
+        <v>11.0668</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -6438,6 +6798,11 @@
           <t>https://finance.yahoo.com/quote/TPVG?p=TPVG</t>
         </is>
       </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TPVG-TriplePoint Venture Growth BDC </t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -6465,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>14.48</v>
+        <v>14.565</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -6518,6 +6883,11 @@
           <t>https://finance.yahoo.com/quote/TRIN?p=TRIN</t>
         </is>
       </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>TRIN-Trinity Capital Inc.</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -6545,7 +6915,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>7.27</v>
+        <v>7.399</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -6589,7 +6959,7 @@
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': -0.13, 'earningsLow': -0.33, 'earningsHigh': 0.18, 'revenueAverage': 26670000, 'revenueLow': 24000000, 'revenueHigh': 30500000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': -0.18, 'earningsLow': -0.33, 'earningsHigh': 0.12, 'revenueAverage': 26340000, 'revenueLow': 24000000, 'revenueHigh': 30500000}</t>
         </is>
       </c>
       <c r="S75" t="inlineStr">
@@ -6600,6 +6970,11 @@
       <c r="T75" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/TRTX?p=TRTX</t>
+        </is>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>TRTX-TPG RE Finance Trust, Inc.</t>
         </is>
       </c>
     </row>
@@ -6629,10 +7004,10 @@
         <v>281.915</v>
       </c>
       <c r="G76" t="n">
-        <v>238.82</v>
+        <v>250.3501</v>
       </c>
       <c r="H76" t="n">
-        <v>238.82</v>
+        <v>250.3501</v>
       </c>
       <c r="I76" t="n">
         <v>103.85</v>
@@ -6657,7 +7032,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.75, 'earningsLow': 0.6, 'earningsHigh': 0.94, 'revenueAverage': 22891400000, 'revenueLow': 18776100000, 'revenueHigh': 25273200000}</t>
+          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.81, 'earningsLow': 0.65, 'earningsHigh': 1.02, 'revenueAverage': 24712700000, 'revenueLow': 20270000000, 'revenueHigh': 27284000000}</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -6668,6 +7043,11 @@
       <c r="T76" t="inlineStr">
         <is>
           <t>https://finance.yahoo.com/quote/TSLA?p=TSLA</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>TSLA-Tesla, Inc.</t>
         </is>
       </c>
     </row>
@@ -6697,7 +7077,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>13.61</v>
+        <v>13.705</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -6754,6 +7134,11 @@
           <t>https://finance.yahoo.com/quote/TWO?p=TWO</t>
         </is>
       </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>TWO-Two Harbors Investment Corp</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -6781,7 +7166,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>10.68</v>
+        <v>10.825</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -6838,6 +7223,11 @@
           <t>https://finance.yahoo.com/quote/WMC?p=WMC</t>
         </is>
       </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WMC-Western Asset Mortgage Capital </t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -6852,7 +7242,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -6865,7 +7255,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>11.8</v>
+        <v>12.08</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -6914,6 +7304,11 @@
           <t>https://finance.yahoo.com/quote/ZIM?p=ZIM</t>
         </is>
       </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>ZIM-ZIM Integrated Shipping Service</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: ex dividend analysis
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>148.2</v>
+        <v>146.1</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>102.85</v>
+        <v>100.88</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7</v>
+        <v>7.01</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>10.36</v>
+        <v>10.35</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>79.79000000000001</v>
+        <v>78.88</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>255.75</v>
+        <v>252.85</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>13.23</v>
+        <v>13.03</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>74.77</v>
+        <v>74.2</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.960000000000001</v>
+        <v>9.76</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6.75</v>
+        <v>6.7</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>200.26</v>
+        <v>200.8</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 3.86, 'earningsLow': 2.23, 'earningsHigh': 5.29, 'revenueAverage': 2590960000, 'revenueLow': 2070000000, 'revenueHigh': 2952100000}</t>
+          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 4.05, 'earningsLow': 2.23, 'earningsHigh': 8.18, 'revenueAverage': 2576080000, 'revenueLow': 2070000000, 'revenueHigh': 2952100000}</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9.779999999999999</v>
+        <v>9.48</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>9.154999999999999</v>
+        <v>8.93</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>138.12</v>
+        <v>137.27</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>9.26</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-06', '2023-11-11'], 'earningsAverage': 0.14, 'earningsLow': 0.06, 'earningsHigh': 0.22, 'revenueAverage': 8610000, 'revenueLow': 7300000, 'revenueHigh': 9800000}</t>
+          <t>{'earningsDate': ['2023-11-06', '2023-11-11'], 'earningsAverage': 0.15, 'earningsLow': 0.06, 'earningsHigh': 0.22, 'revenueAverage': 8610000, 'revenueLow': 7300000, 'revenueHigh': 9800000}</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>73.56999999999999</v>
+        <v>71.94</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>298.02</v>
+        <v>292.7</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>10.93</v>
+        <v>10.7</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>19.91</v>
+        <v>19.74</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2360,7 +2360,7 @@
         <v>17.05</v>
       </c>
       <c r="P21" t="n">
-        <v>26.88</v>
+        <v>26.1</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>4.93</v>
+        <v>4.87</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>115.47</v>
+        <v>112.22</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>10.015</v>
+        <v>11.1</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2638,7 +2638,7 @@
         <v>4.5</v>
       </c>
       <c r="P24" t="n">
-        <v>10.28</v>
+        <v>11.26</v>
       </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2693,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>9.34</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2787,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>5.1</v>
+        <v>4.97</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2881,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>278.46</v>
+        <v>272.88</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>26.87</v>
+        <v>26.13</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -3069,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>6.4</v>
+        <v>5.99</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-29', '2023-12-04'], 'earningsAverage': -4.64, 'earningsLow': -5.1, 'earningsHigh': -4.13, 'revenueAverage': 1032680000, 'revenueLow': 1025000000, 'revenueHigh': 1054000000}</t>
+          <t>{'earningsDate': ['2023-11-29', '2023-12-04'], 'earningsAverage': -4.65, 'earningsLow': -5.1, 'earningsHigh': -4.13, 'revenueAverage': 1033910000, 'revenueLow': 1025000000, 'revenueHigh': 1054000000}</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -3159,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>74.2</v>
+        <v>72.5</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3253,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.789999999999999</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>87.58</v>
+        <v>86.91</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3441,7 +3441,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>203.29</v>
+        <v>200.06</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>96.26000000000001</v>
+        <v>95.17</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3629,10 +3629,10 @@
         <v>1446.798</v>
       </c>
       <c r="G35" t="n">
-        <v>4.04</v>
+        <v>3.96</v>
       </c>
       <c r="H35" t="n">
-        <v>1478.64</v>
+        <v>1449.36</v>
       </c>
       <c r="I35" t="n">
         <v>4.14</v>
@@ -3723,7 +3723,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>88.34999999999999</v>
+        <v>88.65000000000001</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3758,7 +3758,7 @@
         <v>86.59999999999999</v>
       </c>
       <c r="P36" t="n">
-        <v>114.98</v>
+        <v>114.89</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
@@ -3817,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>6.09</v>
+        <v>5.9</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3911,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>106.48</v>
+        <v>105.06</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -4005,7 +4005,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>10.66</v>
+        <v>10.49</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -4091,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>73.27</v>
+        <v>72.78</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -4185,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>155.24</v>
+        <v>153.46</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>11.5</v>
+        <v>11.34</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>8.210000000000001</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -4459,7 +4459,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>505.26</v>
+        <v>496.74</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4540,7 +4540,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -4553,7 +4553,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>3.71</v>
+        <v>3.6077</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>164.3</v>
+        <v>166.46</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4741,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>148.7</v>
+        <v>143.78</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.62</v>
+        <v>3.58</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4921,7 +4921,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>6.54</v>
+        <v>6.46</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -5015,10 +5015,10 @@
         <v>153.75</v>
       </c>
       <c r="G50" t="n">
-        <v>10.37</v>
+        <v>10.41</v>
       </c>
       <c r="H50" t="n">
-        <v>155.55</v>
+        <v>156.15</v>
       </c>
       <c r="I50" t="n">
         <v>10.12</v>
@@ -5109,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>182.7</v>
+        <v>182.09</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -5203,7 +5203,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>88.34999999999999</v>
+        <v>86.51000000000001</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -5297,7 +5297,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>13.37</v>
+        <v>13.22</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-06', '2023-11-10'], 'earningsAverage': 0.41, 'earningsLow': 0.4, 'earningsHigh': 0.42, 'revenueAverage': 35700000, 'revenueLow': 35700000, 'revenueHigh': 35700000}</t>
+          <t>{'earningsDate': ['2023-11-06', '2023-11-10'], 'earningsAverage': 0.42, 'earningsLow': 0.4, 'earningsHigh': 0.43, 'revenueAverage': 57900000, 'revenueLow': 35700000, 'revenueHigh': 80100000}</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
@@ -5391,10 +5391,10 @@
         <v>42</v>
       </c>
       <c r="G54" t="n">
-        <v>44.03</v>
+        <v>43.74</v>
       </c>
       <c r="H54" t="n">
-        <v>44.03</v>
+        <v>43.74</v>
       </c>
       <c r="I54" t="n">
         <v>39.28</v>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>98.92</v>
+        <v>97.88</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -5575,7 +5575,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>237.52</v>
+        <v>235.79</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -5669,7 +5669,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>116.37</v>
+        <v>115.56</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5763,7 +5763,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>5.8668</v>
+        <v>5.85</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5857,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>17.48</v>
+        <v>16.57</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5947,7 +5947,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>98.06</v>
+        <v>96.54000000000001</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -6041,7 +6041,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>20.59</v>
+        <v>20.43</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -6135,7 +6135,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>226.37</v>
+        <v>223.33</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -6229,7 +6229,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>9.970000000000001</v>
+        <v>9.9</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -6323,7 +6323,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>5.25</v>
+        <v>5.14</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.27, 'revenueAverage': 3927690000, 'revenueLow': 3927690000, 'revenueHigh': 3927690000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.26, 'revenueAverage': 3909940000, 'revenueLow': 3909940000, 'revenueHigh': 3909940000}</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6417,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>6.52</v>
+        <v>6.4</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -6511,10 +6511,10 @@
         <v>70.75</v>
       </c>
       <c r="G66" t="n">
-        <v>13.81</v>
+        <v>13.55</v>
       </c>
       <c r="H66" t="n">
-        <v>69.05</v>
+        <v>67.75</v>
       </c>
       <c r="I66" t="n">
         <v>12.41</v>
@@ -6601,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>10.92</v>
+        <v>10.77</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -6718,7 +6718,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.1034</t>
+          <t>0.102299996</t>
         </is>
       </c>
       <c r="N68" t="inlineStr"/>
@@ -6730,12 +6730,12 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>1.279528</t>
+          <t>1.291147</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-30'], 'earningsAverage': 0.27, 'earningsLow': 0.08, 'earningsHigh': 0.62, 'revenueAverage': 181560000, 'revenueLow': 141120000, 'revenueHigh': 270000000}</t>
+          <t>{'earningsDate': ['2023-11-30'], 'earningsAverage': 0.26, 'earningsLow': 0.08, 'earningsHigh': 0.62, 'revenueAverage': 181560000, 'revenueLow': 141120000, 'revenueHigh': 270000000}</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
@@ -6785,7 +6785,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>135.66</v>
+        <v>135.77</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -6863,7 +6863,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>155.08</v>
+        <v>152.34</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -7051,7 +7051,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>7.8</v>
+        <v>7.99</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -7091,7 +7091,7 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-05'], 'earningsAverage': -0.21, 'earningsLow': -0.21, 'earningsHigh': -0.21, 'revenueAverage': 37100000, 'revenueLow': 37100000, 'revenueHigh': 37100000}</t>
+          <t>{'earningsDate': ['2023-11-14', '2023-11-20'], 'earningsAverage': -0.21, 'earningsLow': -0.21, 'earningsHigh': -0.21, 'revenueAverage': 37100000, 'revenueLow': 37100000, 'revenueHigh': 37100000}</t>
         </is>
       </c>
       <c r="S72" t="inlineStr">
@@ -7141,7 +7141,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>710.78</v>
+        <v>693.01</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -7235,7 +7235,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>7.02</v>
+        <v>7.11</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -7316,7 +7316,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -7329,7 +7329,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>38.4</v>
+        <v>37.65</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7361,7 +7361,7 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>37.78</v>
+        <v>37.64</v>
       </c>
       <c r="P75" t="n">
         <v>49.73</v>
@@ -7423,7 +7423,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>147.94</v>
+        <v>148.13</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -7517,7 +7517,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>4.06</v>
+        <v>4.1</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -7611,7 +7611,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>20.22</v>
+        <v>19.85</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -7705,7 +7705,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>247.37</v>
+        <v>242.35</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -7799,7 +7799,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>11.29</v>
+        <v>10.92</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -7893,7 +7893,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>160.48</v>
+        <v>160.68</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -7937,7 +7937,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.51, 'earningsLow': 2.4, 'earningsHigh': 2.58, 'revenueAverage': 21085500000, 'revenueLow': 20888000000, 'revenueHigh': 21356000000}</t>
+          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.51, 'earningsLow': 2.4, 'earningsHigh': 2.58, 'revenueAverage': 21082500000, 'revenueLow': 20888000000, 'revenueHigh': 21356000000}</t>
         </is>
       </c>
       <c r="S81" t="inlineStr">
@@ -7987,7 +7987,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>1.04</v>
+        <v>1.06</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -8077,10 +8077,10 @@
         <v>1647.513</v>
       </c>
       <c r="G83" t="n">
-        <v>24.02</v>
+        <v>24.52</v>
       </c>
       <c r="H83" t="n">
-        <v>1657.38</v>
+        <v>1691.88</v>
       </c>
       <c r="I83" t="n">
         <v>23.01</v>
@@ -8163,7 +8163,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>127.46</v>
+        <v>127.02</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -8257,7 +8257,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>59.31</v>
+        <v>58.82</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -8351,7 +8351,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>12.61</v>
+        <v>12.37</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -8432,7 +8432,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -8445,7 +8445,7 @@
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>28.29</v>
+        <v>27.11</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -8477,7 +8477,7 @@
         </is>
       </c>
       <c r="O87" t="n">
-        <v>27.22</v>
+        <v>27.11</v>
       </c>
       <c r="P87" t="n">
         <v>39.64</v>
@@ -8539,7 +8539,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>388.91</v>
+        <v>381.6</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -8578,7 +8578,7 @@
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>0.85071</t>
+          <t>0.862033</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -8633,7 +8633,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>4.93</v>
+        <v>4.95</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -8727,7 +8727,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>6.46</v>
+        <v>6.27</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -8767,7 +8767,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 187520000, 'revenueLow': 155800000, 'revenueHigh': 209400000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 185890000, 'revenueLow': 154440000, 'revenueHigh': 207570000}</t>
         </is>
       </c>
       <c r="S90" t="inlineStr">
@@ -8817,7 +8817,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>232.51</v>
+        <v>230.43</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -8911,7 +8911,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1.3</v>
+        <v>1.23</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -8942,7 +8942,7 @@
         <v>1.15</v>
       </c>
       <c r="P92" t="n">
-        <v>4.08</v>
+        <v>4.06</v>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
@@ -9001,7 +9001,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>280.94</v>
+        <v>279.16</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -9095,7 +9095,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>82.13</v>
+        <v>80.2</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -9189,7 +9189,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>10.94</v>
+        <v>10.89</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -9283,7 +9283,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>80.45999999999999</v>
+        <v>80.48999999999999</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -9377,7 +9377,7 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>106.95</v>
+        <v>106.85</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -9471,7 +9471,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>19.51</v>
+        <v>19.44</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -9561,7 +9561,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>3.92</v>
+        <v>3.81</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -9605,7 +9605,7 @@
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-28', '2023-12-04'], 'earningsAverage': 0.06, 'earningsLow': 0.04, 'earningsHigh': 0.08, 'revenueAverage': 59890000, 'revenueLow': 51000000, 'revenueHigh': 78600000}</t>
+          <t>{'earningsDate': ['2023-11-28', '2023-12-04'], 'earningsAverage': 0.06, 'earningsLow': 0.04, 'earningsHigh': 0.08, 'revenueAverage': 62850000, 'revenueLow': 52820000, 'revenueHigh': 78600000}</t>
         </is>
       </c>
       <c r="S99" t="inlineStr">
@@ -9655,7 +9655,7 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>245.51</v>
+        <v>240.6</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -9749,7 +9749,7 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>66.87</v>
+        <v>66.2</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -9781,7 +9781,7 @@
         </is>
       </c>
       <c r="O101" t="n">
-        <v>66.45</v>
+        <v>65.80500000000001</v>
       </c>
       <c r="P101" t="n">
         <v>91.06</v>
@@ -9843,7 +9843,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>5.4</v>
+        <v>5.4091</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -9937,7 +9937,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>20.36</v>
+        <v>20.09</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -9972,7 +9972,7 @@
         <v>15.11</v>
       </c>
       <c r="P103" t="n">
-        <v>27.04</v>
+        <v>26.92</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
@@ -10031,7 +10031,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>172.58</v>
+        <v>170.24</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -10125,7 +10125,7 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>9.57</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -10219,7 +10219,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>56.2</v>
+        <v>55.25</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -10251,7 +10251,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>55.5</v>
+        <v>55.23</v>
       </c>
       <c r="P106" t="n">
         <v>68.84999999999999</v>
@@ -10300,7 +10300,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -10313,10 +10313,10 @@
         <v>2432.64</v>
       </c>
       <c r="G107" t="n">
-        <v>8.039999999999999</v>
+        <v>8.31</v>
       </c>
       <c r="H107" t="n">
-        <v>2572.8</v>
+        <v>2659.2</v>
       </c>
       <c r="I107" t="n">
         <v>8.01</v>
@@ -10331,7 +10331,7 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>2023-06-13</t>
+          <t>2023-09-14</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
@@ -10344,7 +10344,7 @@
         <v>7.71</v>
       </c>
       <c r="P107" t="n">
-        <v>10.98</v>
+        <v>10.8</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>7.33</v>
+        <v>6.48</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -10497,7 +10497,7 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>9.51</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -10532,7 +10532,7 @@
         <v>7.95</v>
       </c>
       <c r="P109" t="n">
-        <v>12.95</v>
+        <v>12.85</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
@@ -10685,7 +10685,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3.11</v>
+        <v>3.08</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -10779,7 +10779,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>14.49</v>
+        <v>14.8</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -10873,7 +10873,7 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>7.01</v>
+        <v>6.94</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -10967,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>175.32</v>
+        <v>174.16</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -11061,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>154.51</v>
+        <v>152.44</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -11155,7 +11155,7 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>70.95999999999999</v>
+        <v>68.97</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -11249,7 +11249,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>142.01</v>
+        <v>136.47</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -11330,7 +11330,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -11343,7 +11343,7 @@
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>19.56</v>
+        <v>19.31</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -11437,7 +11437,7 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>499.54</v>
+        <v>493.39</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -11531,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>6.81</v>
+        <v>6.95</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -11625,7 +11625,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>8.220000000000001</v>
+        <v>7.88</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -11719,7 +11719,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>3.48</v>
+        <v>3.52</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -11800,7 +11800,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -11813,10 +11813,10 @@
         <v>1263.55</v>
       </c>
       <c r="G123" t="n">
-        <v>17.62</v>
+        <v>17.42</v>
       </c>
       <c r="H123" t="n">
-        <v>1303.88</v>
+        <v>1289.08</v>
       </c>
       <c r="I123" t="n">
         <v>17.05</v>
@@ -11903,7 +11903,7 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>10.78</v>
+        <v>10.74</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -11997,7 +11997,7 @@
         <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>274.82</v>
+        <v>269.59</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -12091,7 +12091,7 @@
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>142.49</v>
+        <v>143.01</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -12185,7 +12185,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>39.11</v>
+        <v>38.13</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -12279,7 +12279,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>8.789999999999999</v>
+        <v>8.75</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -12357,7 +12357,7 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>394.24</v>
+        <v>393.55</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -12451,7 +12451,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>94.45</v>
+        <v>92.64</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -12490,7 +12490,7 @@
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>1.355732</t>
+          <t>1.367911</t>
         </is>
       </c>
       <c r="R130" t="inlineStr">
@@ -12532,7 +12532,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -12545,7 +12545,7 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>70.29000000000001</v>
+        <v>68.66</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -12577,7 +12577,7 @@
         </is>
       </c>
       <c r="O131" t="n">
-        <v>69.22</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="P131" t="n">
         <v>87.41</v>
@@ -12626,7 +12626,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -12639,7 +12639,7 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>125.52</v>
+        <v>125.19</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -12733,7 +12733,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>11.17</v>
+        <v>11.14</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -12827,7 +12827,7 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>14.55</v>
+        <v>14.31</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>112.9</v>
+        <v>111.81</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -13011,7 +13011,7 @@
         <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>7.54</v>
+        <v>7.43</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -13105,10 +13105,10 @@
         <v>281.915</v>
       </c>
       <c r="G137" t="n">
-        <v>245.01</v>
+        <v>256.49</v>
       </c>
       <c r="H137" t="n">
-        <v>245.01</v>
+        <v>256.49</v>
       </c>
       <c r="I137" t="n">
         <v>103.85</v>
@@ -13183,7 +13183,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>13.81</v>
+        <v>13.54</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -13277,7 +13277,7 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>23.43</v>
+        <v>22.73</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -13309,7 +13309,7 @@
         </is>
       </c>
       <c r="O139" t="n">
-        <v>23.39</v>
+        <v>22.69</v>
       </c>
       <c r="P139" t="n">
         <v>42.29</v>
@@ -13371,7 +13371,7 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>10.66</v>
+        <v>10.43</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -13465,7 +13465,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>161.57</v>
+        <v>160.27</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -13559,7 +13559,7 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>407.69</v>
+        <v>403.67</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -13653,7 +13653,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>113.52</v>
+        <v>113.53</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -13734,7 +13734,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -13747,7 +13747,7 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>12.24</v>
+        <v>11.69</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -13771,10 +13771,10 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="n">
-        <v>11.72</v>
+        <v>11.65</v>
       </c>
       <c r="P144" t="n">
-        <v>34.64</v>
+        <v>34.14</v>
       </c>
       <c r="Q144" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
chore: update portfolio and notebook
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>146.1</v>
+        <v>145.61</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>100.88</v>
+        <v>101.56</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7.01</v>
+        <v>7.1</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -782,7 +782,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.1714</t>
+          <t>0.1712</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>10.35</v>
+        <v>10.29</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>78.88</v>
+        <v>77.45999999999999</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -970,7 +970,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.0226</t>
+          <t>0.0228</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>252.85</v>
+        <v>251.05</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 2.03, 'earningsLow': 1.97, 'earningsHigh': 2.21, 'revenueAverage': 4523980000, 'revenueLow': 4456000000, 'revenueHigh': 4630650000}</t>
+          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 2.04, 'earningsLow': 1.97, 'earningsHigh': 2.21, 'revenueAverage': 4520980000, 'revenueLow': 4456000000, 'revenueHigh': 4630650000}</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>13.03</v>
+        <v>12.95</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-06', '2023-11-10'], 'earningsAverage': 0.52, 'earningsLow': 0.5, 'earningsHigh': 0.55, 'revenueAverage': 18730000, 'revenueLow': 16650000, 'revenueHigh': 23850000}</t>
+          <t>{'earningsDate': ['2023-11-06', '2023-11-10'], 'earningsAverage': 0.49, 'earningsLow': 0.4, 'earningsHigh': 0.55, 'revenueAverage': 17840000, 'revenueLow': 14290000, 'revenueHigh': 23850000}</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>74.2</v>
+        <v>74.23</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.0225</t>
+          <t>0.0226</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.46, 'earningsLow': 1.4, 'earningsHigh': 1.5, 'revenueAverage': 4389680000, 'revenueLow': 4212910000, 'revenueHigh': 4615000000}</t>
+          <t>{'earningsDate': ['2023-11-01'], 'earningsAverage': 1.46, 'earningsLow': 1.4, 'earningsHigh': 1.5, 'revenueAverage': 4389680000, 'revenueLow': 4212910000, 'revenueHigh': 4615000000}</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>12.46</v>
+        <v>12.45</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.1308</t>
+          <t>0.1354</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.76</v>
+        <v>9.68</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.1454</t>
+          <t>0.1446</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6.7</v>
+        <v>6.64</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.1185</t>
+          <t>0.119399995</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>200.8</v>
+        <v>189.83</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 4.05, 'earningsLow': 2.23, 'earningsHigh': 8.18, 'revenueAverage': 2576080000, 'revenueLow': 2070000000, 'revenueHigh': 2952100000}</t>
+          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 4.07, 'earningsLow': 2.23, 'earningsHigh': 8.18, 'revenueAverage': 2590960000, 'revenueLow': 2070000000, 'revenueHigh': 2952100000}</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9.48</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>8.93</v>
+        <v>9.098000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>137.27</v>
+        <v>135.36</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>9.039999999999999</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>71.94</v>
+        <v>71.84999999999999</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>292.7</v>
+        <v>293.35</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>10.7</v>
+        <v>10.56</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>19.74</v>
+        <v>19.37</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>4.87</v>
+        <v>4.88</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2023-10-13</t>
+          <t>2023-09-14</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>112.22</v>
+        <v>112.27</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>0.0256</t>
+          <t>0.026400002</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-07', '2023-11-13'], 'earningsAverage': 0.71, 'earningsLow': 0.64, 'earningsHigh': 0.8, 'revenueAverage': 978050000, 'revenueLow': 841000000, 'revenueHigh': 1150160000}</t>
+          <t>{'earningsDate': ['2023-11-07', '2023-11-13'], 'earningsAverage': 0.7, 'earningsLow': 0.64, 'earningsHigh': 0.76, 'revenueAverage': 968050000, 'revenueLow': 841000000, 'revenueHigh': 1150160000}</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>11.1</v>
+        <v>11.3991</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.1997</t>
+          <t>0.17549999</t>
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
@@ -2638,9 +2638,13 @@
         <v>4.5</v>
       </c>
       <c r="P24" t="n">
-        <v>11.26</v>
-      </c>
-      <c r="Q24" t="inlineStr"/>
+        <v>11.47</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>1.209834</t>
+        </is>
+      </c>
       <c r="R24" t="inlineStr">
         <is>
           <t>{'earningsDate': [], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
@@ -2693,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>8.890000000000001</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2716,7 +2720,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.1113</t>
+          <t>0.117</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2787,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>4.97</v>
+        <v>5.05</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2881,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>272.88</v>
+        <v>266.64</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2975,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>26.13</v>
+        <v>26.11</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -3069,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>5.99</v>
+        <v>6.1</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -3159,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>72.5</v>
+        <v>72.73</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3253,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.699999999999999</v>
+        <v>8.57</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3347,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>86.91</v>
+        <v>87.25</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3441,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>200.06</v>
+        <v>201.94</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3535,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>95.17</v>
+        <v>94.12</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3558,7 +3562,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>0.0113</t>
+          <t>0.0115</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -3629,10 +3633,10 @@
         <v>1446.798</v>
       </c>
       <c r="G35" t="n">
-        <v>3.96</v>
+        <v>3.93</v>
       </c>
       <c r="H35" t="n">
-        <v>1449.36</v>
+        <v>1438.38</v>
       </c>
       <c r="I35" t="n">
         <v>4.14</v>
@@ -3710,7 +3714,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -3723,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>88.65000000000001</v>
+        <v>87.38</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3817,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.9</v>
+        <v>5.88</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3911,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>105.06</v>
+        <v>104.52</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -4005,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>10.49</v>
+        <v>10.48</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -4091,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>72.78</v>
+        <v>72.31999999999999</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -4185,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>153.46</v>
+        <v>153.6</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -4279,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>11.34</v>
+        <v>11.29</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -4365,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>8.289999999999999</v>
+        <v>8.27</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -4388,7 +4392,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>0.1714</t>
+          <t>0.1702</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -4459,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>496.74</v>
+        <v>495.73</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4482,7 +4486,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.0107</t>
+          <t>0.0109</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4553,7 +4557,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>3.6077</v>
+        <v>3.56</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4647,7 +4651,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>166.46</v>
+        <v>166.63</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4670,7 +4674,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>0.0368</t>
+          <t>0.0363</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -4741,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>143.78</v>
+        <v>143.86</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4764,7 +4768,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>0.0137</t>
+          <t>0.014199999</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -4835,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.58</v>
+        <v>3.56</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4912,25 +4916,25 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>6.47</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>647</v>
       </c>
       <c r="G49" t="n">
-        <v>6.46</v>
+        <v>6.28</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>628</v>
       </c>
       <c r="I49" t="n">
         <v>6.77</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>7.12</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -5015,10 +5019,10 @@
         <v>153.75</v>
       </c>
       <c r="G50" t="n">
-        <v>10.41</v>
+        <v>10.39</v>
       </c>
       <c r="H50" t="n">
-        <v>156.15</v>
+        <v>155.85</v>
       </c>
       <c r="I50" t="n">
         <v>10.12</v>
@@ -5038,7 +5042,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>0.162</t>
+          <t>0.16139999</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -5109,7 +5113,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>182.09</v>
+        <v>181.62</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -5203,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>86.51000000000001</v>
+        <v>86.8</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -5226,7 +5230,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.0367</t>
+          <t>0.0375</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -5247,7 +5251,7 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 1.67, 'earningsLow': 1.35, 'earningsHigh': 1.85, 'revenueAverage': 3972370000, 'revenueLow': 3852170000, 'revenueHigh': 4113330000}</t>
+          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 1.66, 'earningsLow': 1.35, 'earningsHigh': 1.85, 'revenueAverage': 3896010000, 'revenueLow': 3540450000, 'revenueHigh': 4113330000}</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
@@ -5297,7 +5301,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>13.22</v>
+        <v>13.16</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -5391,10 +5395,10 @@
         <v>42</v>
       </c>
       <c r="G54" t="n">
-        <v>43.74</v>
+        <v>43.73</v>
       </c>
       <c r="H54" t="n">
-        <v>43.74</v>
+        <v>43.73</v>
       </c>
       <c r="I54" t="n">
         <v>39.28</v>
@@ -5481,7 +5485,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>97.88</v>
+        <v>98.67</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -5504,7 +5508,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>0.021</t>
+          <t>0.0211</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -5575,7 +5579,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>235.79</v>
+        <v>236.41</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -5669,7 +5673,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>115.56</v>
+        <v>115.59</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5763,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>5.85</v>
+        <v>5.96</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5786,7 +5790,7 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>0.1432</t>
+          <t>0.1409</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
@@ -5857,7 +5861,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>16.57</v>
+        <v>16.45</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5947,7 +5951,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>96.54000000000001</v>
+        <v>97.23999999999999</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -5991,7 +5995,7 @@
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.67, 'earningsLow': 0.65, 'earningsHigh': 0.7, 'revenueAverage': 284120000, 'revenueLow': 279380000, 'revenueHigh': 288000000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.67, 'earningsLow': 0.65, 'earningsHigh': 0.7, 'revenueAverage': 283920000, 'revenueLow': 279380000, 'revenueHigh': 288000000}</t>
         </is>
       </c>
       <c r="S60" t="inlineStr">
@@ -6041,7 +6045,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>20.43</v>
+        <v>20.31</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -6064,7 +6068,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>0.136</t>
+          <t>0.1371</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -6135,7 +6139,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>223.33</v>
+        <v>218.05</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -6229,7 +6233,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>9.9</v>
+        <v>9.7753</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -6323,7 +6327,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>5.14</v>
+        <v>5.07</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -6346,7 +6350,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>0.116000004</t>
+          <t>0.1185</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -6367,7 +6371,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.26, 'revenueAverage': 3909940000, 'revenueLow': 3909940000, 'revenueHigh': 3909940000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.27, 'revenueAverage': 3941690000, 'revenueLow': 3941690000, 'revenueHigh': 3941690000}</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6417,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>6.4</v>
+        <v>6.43</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -6511,10 +6515,10 @@
         <v>70.75</v>
       </c>
       <c r="G66" t="n">
-        <v>13.55</v>
+        <v>13.59</v>
       </c>
       <c r="H66" t="n">
-        <v>67.75</v>
+        <v>67.95</v>
       </c>
       <c r="I66" t="n">
         <v>12.41</v>
@@ -6601,7 +6605,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>10.77</v>
+        <v>10.92</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -6695,10 +6699,10 @@
         <v>1023.26</v>
       </c>
       <c r="G68" t="n">
-        <v>7.33</v>
+        <v>7.45</v>
       </c>
       <c r="H68" t="n">
-        <v>1026.2</v>
+        <v>1043</v>
       </c>
       <c r="I68" t="n">
         <v>7.06</v>
@@ -6735,7 +6739,7 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-30'], 'earningsAverage': 0.26, 'earningsLow': 0.08, 'earningsHigh': 0.62, 'revenueAverage': 181560000, 'revenueLow': 141120000, 'revenueHigh': 270000000}</t>
+          <t>{'earningsDate': ['2023-11-30'], 'earningsAverage': 0.14, 'earningsLow': 0.08, 'earningsHigh': 0.19, 'revenueAverage': 150710000, 'revenueLow': 141120000, 'revenueHigh': 162000000}</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
@@ -6785,7 +6789,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>135.77</v>
+        <v>134.46</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -6863,7 +6867,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>152.34</v>
+        <v>151.78</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -6957,7 +6961,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>5.38</v>
+        <v>5.29</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -7051,7 +7055,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>7.99</v>
+        <v>7.62</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -7091,7 +7095,7 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-14', '2023-11-20'], 'earningsAverage': -0.21, 'earningsLow': -0.21, 'earningsHigh': -0.21, 'revenueAverage': 37100000, 'revenueLow': 37100000, 'revenueHigh': 37100000}</t>
+          <t>{'earningsDate': ['2023-11-14', '2023-11-20'], 'earningsAverage': 0.22, 'earningsLow': 0.22, 'earningsHigh': 0.22, 'revenueAverage': 47880000, 'revenueLow': 47880000, 'revenueHigh': 47880000}</t>
         </is>
       </c>
       <c r="S72" t="inlineStr">
@@ -7141,7 +7145,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>693.01</v>
+        <v>693.54</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -7164,7 +7168,7 @@
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>0.0105</t>
+          <t>0.0107</t>
         </is>
       </c>
       <c r="N73" t="inlineStr">
@@ -7235,7 +7239,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>7.11</v>
+        <v>7.21</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -7329,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>37.65</v>
+        <v>37.25</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7361,7 +7365,7 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>37.64</v>
+        <v>37.235</v>
       </c>
       <c r="P75" t="n">
         <v>49.73</v>
@@ -7423,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>148.13</v>
+        <v>148.06</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -7446,7 +7450,7 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>0.044899996</t>
+          <t>0.0448</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -7517,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>4.1</v>
+        <v>4.075</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -7611,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>19.85</v>
+        <v>20.01</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -7705,7 +7709,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>242.35</v>
+        <v>244.2</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -7799,7 +7803,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>10.92</v>
+        <v>10.81</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -7893,7 +7897,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>160.68</v>
+        <v>158.01</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -7916,7 +7920,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>0.0297</t>
+          <t>0.0296</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -7987,7 +7991,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>1.06</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -8018,7 +8022,7 @@
         <v>0.79</v>
       </c>
       <c r="P82" t="n">
-        <v>9.029999999999999</v>
+        <v>8.84</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
@@ -8064,7 +8068,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -8077,10 +8081,10 @@
         <v>1647.513</v>
       </c>
       <c r="G83" t="n">
-        <v>24.52</v>
+        <v>23.3</v>
       </c>
       <c r="H83" t="n">
-        <v>1691.88</v>
+        <v>1607.7</v>
       </c>
       <c r="I83" t="n">
         <v>23.01</v>
@@ -8163,7 +8167,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>127.02</v>
+        <v>126.59</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -8257,7 +8261,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>58.82</v>
+        <v>58.78</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -8351,7 +8355,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>12.37</v>
+        <v>12.25</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -8374,7 +8378,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>0.1375</t>
+          <t>0.139</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -8395,7 +8399,7 @@
       </c>
       <c r="R86" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.14, 'earningsLow': -0.34, 'earningsHigh': 0.47, 'revenueAverage': 43370000, 'revenueLow': 41000000, 'revenueHigh': 47200000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.22, 'earningsLow': -0.34, 'earningsHigh': 0.47, 'revenueAverage': 42870000, 'revenueLow': 41000000, 'revenueHigh': 47200000}</t>
         </is>
       </c>
       <c r="S86" t="inlineStr">
@@ -8432,29 +8436,29 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>27.11</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>569.3099999999999</v>
       </c>
       <c r="G87" t="n">
-        <v>27.11</v>
+        <v>27.03</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>567.63</v>
       </c>
       <c r="I87" t="n">
         <v>27.44</v>
       </c>
       <c r="J87" t="n">
-        <v>0</v>
+        <v>29.82</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
@@ -8477,7 +8481,7 @@
         </is>
       </c>
       <c r="O87" t="n">
-        <v>27.11</v>
+        <v>26.59</v>
       </c>
       <c r="P87" t="n">
         <v>39.64</v>
@@ -8539,7 +8543,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>381.6</v>
+        <v>383.29</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -8562,7 +8566,7 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>0.013099999</t>
+          <t>0.013300001</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
@@ -8633,7 +8637,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>4.95</v>
+        <v>5.11</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -8727,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>6.27</v>
+        <v>6</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -8767,7 +8771,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 185890000, 'revenueLow': 154440000, 'revenueHigh': 207570000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 187130000, 'revenueLow': 155470000, 'revenueHigh': 208960000}</t>
         </is>
       </c>
       <c r="S90" t="inlineStr">
@@ -8817,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>230.43</v>
+        <v>229.61</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -8911,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1.23</v>
+        <v>1.21</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -9001,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>279.16</v>
+        <v>275.44</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -9024,7 +9028,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>0.0216</t>
+          <t>0.0221</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -9095,7 +9099,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>80.2</v>
+        <v>80.70999999999999</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -9189,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>10.89</v>
+        <v>10.77</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -9283,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>80.48999999999999</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -9327,7 +9331,7 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-04', '2023-10-09'], 'earningsAverage': 0.65, 'earningsLow': 0.64, 'earningsHigh': 0.67, 'revenueAverage': 1696620000, 'revenueLow': 1671000000, 'revenueHigh': 1719000000}</t>
+          <t>{'earningsDate': ['2023-10-03'], 'earningsAverage': 0.65, 'earningsLow': 0.64, 'earningsHigh': 0.67, 'revenueAverage': 1696400000, 'revenueLow': 1671000000, 'revenueHigh': 1719000000}</t>
         </is>
       </c>
       <c r="S96" t="inlineStr">
@@ -9377,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>106.85</v>
+        <v>106.37</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -9471,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>19.44</v>
+        <v>19.41</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -9561,7 +9565,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>3.81</v>
+        <v>3.82</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -9655,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>240.6</v>
+        <v>239.55</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -9678,7 +9682,7 @@
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>0.0111</t>
+          <t>0.0113</t>
         </is>
       </c>
       <c r="N100" t="inlineStr">
@@ -9749,7 +9753,7 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>66.2</v>
+        <v>65.69</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -9772,7 +9776,7 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>0.027999999</t>
+          <t>0.028199999</t>
         </is>
       </c>
       <c r="N101" t="inlineStr">
@@ -9781,7 +9785,7 @@
         </is>
       </c>
       <c r="O101" t="n">
-        <v>65.80500000000001</v>
+        <v>65.355</v>
       </c>
       <c r="P101" t="n">
         <v>91.06</v>
@@ -9843,7 +9847,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>5.4091</v>
+        <v>5.31</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -9937,7 +9941,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>20.09</v>
+        <v>19.89</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -10031,7 +10035,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>170.24</v>
+        <v>168.6</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -10125,7 +10129,7 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>9.300000000000001</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -10219,7 +10223,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>55.25</v>
+        <v>54.99</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -10242,7 +10246,7 @@
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>0.0546</t>
+          <t>0.0555</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -10251,7 +10255,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>55.23</v>
+        <v>54.76</v>
       </c>
       <c r="P106" t="n">
         <v>68.84999999999999</v>
@@ -10300,7 +10304,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -10313,10 +10317,10 @@
         <v>2432.64</v>
       </c>
       <c r="G107" t="n">
-        <v>8.31</v>
+        <v>8.18</v>
       </c>
       <c r="H107" t="n">
-        <v>2659.2</v>
+        <v>2617.6</v>
       </c>
       <c r="I107" t="n">
         <v>8.01</v>
@@ -10336,7 +10340,7 @@
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>0.2752</t>
+          <t>0.2736</t>
         </is>
       </c>
       <c r="N107" t="inlineStr"/>
@@ -10344,7 +10348,7 @@
         <v>7.71</v>
       </c>
       <c r="P107" t="n">
-        <v>10.8</v>
+        <v>10.69</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
@@ -10353,7 +10357,7 @@
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-07', '2023-09-11'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 7510000, 'revenueLow': 7510000, 'revenueHigh': 7510000}</t>
+          <t>{'earningsDate': ['2023-09-07', '2023-09-10'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 7510000, 'revenueLow': 7510000, 'revenueHigh': 7510000}</t>
         </is>
       </c>
       <c r="S107" t="inlineStr">
@@ -10403,7 +10407,7 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>6.48</v>
+        <v>6.195</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -10497,7 +10501,7 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>9.289999999999999</v>
+        <v>9.24</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -10591,10 +10595,10 @@
         <v>369</v>
       </c>
       <c r="G110" t="n">
-        <v>5.19</v>
+        <v>5.2</v>
       </c>
       <c r="H110" t="n">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="I110" t="n">
         <v>4.8</v>
@@ -10685,7 +10689,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3.08</v>
+        <v>3.11</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -10708,7 +10712,7 @@
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>0.1355</t>
+          <t>0.1364</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
@@ -10779,7 +10783,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>14.8</v>
+        <v>14.93</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -10873,7 +10877,7 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>6.94</v>
+        <v>6.87</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -10896,7 +10900,7 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>0.0713</t>
+          <t>0.072</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
@@ -10967,7 +10971,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>174.16</v>
+        <v>174.73</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -11061,7 +11065,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>152.44</v>
+        <v>152.14</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -11155,7 +11159,7 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>68.97</v>
+        <v>69.63</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -11249,7 +11253,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>136.47</v>
+        <v>137.05</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -11272,7 +11276,7 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>0.0183</t>
+          <t>0.0191</t>
         </is>
       </c>
       <c r="N117" t="inlineStr">
@@ -11343,7 +11347,7 @@
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>19.31</v>
+        <v>19.33</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -11366,7 +11370,7 @@
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>0.1397</t>
+          <t>0.1429</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
@@ -11437,7 +11441,7 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>493.39</v>
+        <v>495</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -11531,7 +11535,7 @@
         <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>6.95</v>
+        <v>7.14</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -11625,7 +11629,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>7.88</v>
+        <v>7.79</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -11719,7 +11723,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>3.52</v>
+        <v>3.46</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -11800,7 +11804,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -11813,10 +11817,10 @@
         <v>1263.55</v>
       </c>
       <c r="G123" t="n">
-        <v>17.42</v>
+        <v>17.61</v>
       </c>
       <c r="H123" t="n">
-        <v>1289.08</v>
+        <v>1303.14</v>
       </c>
       <c r="I123" t="n">
         <v>17.05</v>
@@ -11836,7 +11840,7 @@
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>0.1447</t>
+          <t>0.14479999</t>
         </is>
       </c>
       <c r="N123" t="inlineStr"/>
@@ -11903,7 +11907,7 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>10.74</v>
+        <v>10.7</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -11997,7 +12001,7 @@
         <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>269.59</v>
+        <v>269.07</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -12020,7 +12024,7 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>0.0088</t>
+          <t>0.009</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
@@ -12091,7 +12095,7 @@
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>143.01</v>
+        <v>141.13</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -12135,7 +12139,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.52, 'revenueAverage': 1938990000, 'revenueLow': 1913390000, 'revenueHigh': 1959000000}</t>
+          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.44, 'earningsLow': 2.21, 'earningsHigh': 2.52, 'revenueAverage': 1938990000, 'revenueLow': 1913390000, 'revenueHigh': 1959000000}</t>
         </is>
       </c>
       <c r="S126" t="inlineStr">
@@ -12185,7 +12189,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>38.13</v>
+        <v>38.82</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -12208,7 +12212,7 @@
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>0.0828</t>
+          <t>0.085200004</t>
         </is>
       </c>
       <c r="N127" t="inlineStr">
@@ -12279,7 +12283,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>8.75</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -12357,7 +12361,7 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>393.55</v>
+        <v>394.15</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -12451,7 +12455,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>92.64</v>
+        <v>93.7</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -12474,7 +12478,7 @@
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>0.0343</t>
+          <t>0.035</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
@@ -12545,7 +12549,7 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>68.66</v>
+        <v>68.45</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -12639,7 +12643,7 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>125.19</v>
+        <v>123.71</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -12662,7 +12666,7 @@
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>0.0346</t>
+          <t>0.0347</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
@@ -12733,7 +12737,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>11.14</v>
+        <v>11.06</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -12827,7 +12831,7 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>14.31</v>
+        <v>14.23</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -12917,7 +12921,7 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>111.81</v>
+        <v>111.5</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -13105,10 +13109,10 @@
         <v>281.915</v>
       </c>
       <c r="G137" t="n">
-        <v>256.49</v>
+        <v>251.92</v>
       </c>
       <c r="H137" t="n">
-        <v>256.49</v>
+        <v>251.92</v>
       </c>
       <c r="I137" t="n">
         <v>103.85</v>
@@ -13183,7 +13187,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>13.54</v>
+        <v>13.39</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -13264,7 +13268,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -13277,7 +13281,7 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>22.73</v>
+        <v>22.64</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -13300,7 +13304,7 @@
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>0.0759</t>
+          <t>0.0848</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
@@ -13309,7 +13313,7 @@
         </is>
       </c>
       <c r="O139" t="n">
-        <v>22.69</v>
+        <v>22.31</v>
       </c>
       <c r="P139" t="n">
         <v>42.29</v>
@@ -13371,7 +13375,7 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>10.43</v>
+        <v>10.32</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -13406,7 +13410,7 @@
         <v>7</v>
       </c>
       <c r="P140" t="n">
-        <v>14.57</v>
+        <v>14.28</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
@@ -13465,7 +13469,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>160.27</v>
+        <v>161.47</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -13488,7 +13492,7 @@
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>0.014099999</t>
+          <t>0.014199999</t>
         </is>
       </c>
       <c r="N141" t="inlineStr">
@@ -13559,7 +13563,7 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>403.67</v>
+        <v>404.85</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -13653,7 +13657,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>113.53</v>
+        <v>114.51</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -13734,7 +13738,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -13747,7 +13751,7 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>11.69</v>
+        <v>11.7</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -13771,7 +13775,7 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="n">
-        <v>11.65</v>
+        <v>11.55</v>
       </c>
       <c r="P144" t="n">
         <v>34.14</v>

</xml_diff>

<commit_message>
feat(analysis): historical prices and machine learning
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>149.02</v>
+        <v>149.04</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -589,12 +589,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2023-07-13</t>
+          <t>2023-10-12</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.0398</t>
+          <t>0.0397</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>100.73</v>
+        <v>102.45</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -688,7 +688,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.020299999</t>
+          <t>0.0199</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7.05</v>
+        <v>7.06</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -782,7 +782,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0.1702</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>10.41</v>
+        <v>10.49</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -876,7 +876,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.1313</t>
+          <t>0.1306</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -888,7 +888,7 @@
         <v>7.52</v>
       </c>
       <c r="P5" t="n">
-        <v>13.62</v>
+        <v>13.42</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>78.81</v>
+        <v>78.73999999999999</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>249.37</v>
+        <v>248.2</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.0201</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>13.17</v>
+        <v>13.3</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>74.83</v>
+        <v>75.59</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.0225</t>
+          <t>0.0222</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.69</v>
+        <v>9.83</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.1488</t>
+          <t>0.14649999</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6.68</v>
+        <v>6.73</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.1205</t>
+          <t>0.1189</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>184.43</v>
+        <v>186.32</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.0085</t>
+          <t>0.0087</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9.25</v>
+        <v>9.43</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.053600002</t>
+          <t>0.053000003</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>8.779999999999999</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.3575</t>
+          <t>0.35029998</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>138.23</v>
+        <v>143.1</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.54, 'earningsLow': 0.41, 'earningsHigh': 0.66, 'revenueAverage': 131883000000, 'revenueLow': 128681000000, 'revenueHigh': 133523000000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.58, 'earningsLow': 0.44, 'earningsHigh': 0.71, 'revenueAverage': 141434000000, 'revenueLow': 138000000000, 'revenueHigh': 143193000000}</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>9.029999999999999</v>
+        <v>9.15</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>70.19</v>
+        <v>70.51000000000001</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.0167</t>
+          <t>0.017</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>298.51</v>
+        <v>302.8</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0.024</t>
+          <t>0.0234</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>10.69</v>
+        <v>10.75</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0.1322</t>
+          <t>0.131</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>19.675</v>
+        <v>19.84</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>4.83</v>
+        <v>4.9</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.9959</t>
+          <t>0.9796</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2454,7 +2454,7 @@
         <v>4.38</v>
       </c>
       <c r="P22" t="n">
-        <v>7.3</v>
+        <v>7.03</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>114.18</v>
+        <v>113.93</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>10.87</v>
+        <v>10.9</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.1728</t>
+          <t>0.1835</t>
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>8.9</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.1185</t>
+          <t>0.1159</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>4.96</v>
+        <v>4.78</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.1532</t>
+          <t>0.159</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2826,7 +2826,7 @@
         <v>3.42</v>
       </c>
       <c r="P26" t="n">
-        <v>8.609999999999999</v>
+        <v>8.49</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': -0.04, 'earningsLow': -0.04, 'earningsHigh': -0.04, 'revenueAverage': 129510000, 'revenueLow': 128340000, 'revenueHigh': 130150000}</t>
+          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': -0.06, 'earningsLow': -0.06, 'earningsHigh': -0.06, 'revenueAverage': 129510000, 'revenueLow': 128340000, 'revenueHigh': 130150000}</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>266.76</v>
+        <v>267.18</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-08', '2023-11-13'], 'earningsAverage': 3.43, 'earningsLow': 3.35, 'earningsHigh': 3.52, 'revenueAverage': 5022480000, 'revenueLow': 4998010000, 'revenueHigh': 5064000000}</t>
+          <t>{'earningsDate': ['2023-11-08', '2023-11-13'], 'earningsAverage': 3.43, 'earningsLow': 3.35, 'earningsHigh': 3.52, 'revenueAverage': 5022890000, 'revenueLow': 4998010000, 'revenueHigh': 5064000000}</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>25.93</v>
+        <v>25.96</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.0463</t>
+          <t>0.0462</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>5.64</v>
+        <v>5.89</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -3104,7 +3104,7 @@
         <v>4.78</v>
       </c>
       <c r="P29" t="n">
-        <v>24.09</v>
+        <v>22.8</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>73.12</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.49</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>0.1449</t>
+          <t>0.1498</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -3351,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>88.78</v>
+        <v>89.73</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0.0226</t>
+          <t>0.0223</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>204.67</v>
+        <v>206.35</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3539,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>95.67</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3633,10 +3633,10 @@
         <v>1446.798</v>
       </c>
       <c r="G35" t="n">
-        <v>3.92</v>
+        <v>3.99</v>
       </c>
       <c r="H35" t="n">
-        <v>1434.72</v>
+        <v>1460.34</v>
       </c>
       <c r="I35" t="n">
         <v>3.74</v>
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>86.31999999999999</v>
+        <v>86.55</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>0.028299998</t>
+          <t>0.028199999</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>85.22499999999999</v>
+        <v>85.23</v>
       </c>
       <c r="P36" t="n">
-        <v>114.57</v>
+        <v>112.89</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.85</v>
+        <v>5.97</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>0.123500004</t>
+          <t>0.123100005</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -3856,7 +3856,7 @@
         <v>4.48</v>
       </c>
       <c r="P37" t="n">
-        <v>8.41</v>
+        <v>8.25</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 0.16, 'earningsLow': 0.12, 'earningsHigh': 0.25, 'revenueAverage': 75010000, 'revenueLow': 69750000, 'revenueHigh': 84900000}</t>
+          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 0.16, 'earningsLow': 0.12, 'earningsHigh': 0.25, 'revenueAverage': 81210000, 'revenueLow': 69750000, 'revenueHigh': 99800000}</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -3915,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>105</v>
+        <v>105.91</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>0.0286</t>
+          <t>0.028299998</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -4009,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>10.65</v>
+        <v>10.76</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>0.0744</t>
+          <t>0.0725</t>
         </is>
       </c>
       <c r="N39" t="inlineStr"/>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>73.2</v>
+        <v>73.95</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>0.026199998</t>
+          <t>0.025999999</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.75, 'earningsLow': 0.73, 'earningsHigh': 0.77, 'revenueAverage': 4488870000, 'revenueLow': 4401260000, 'revenueHigh': 4671300000}</t>
+          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.8, 'earningsLow': 0.78, 'earningsHigh': 0.83, 'revenueAverage': 4813960000, 'revenueLow': 4720000000, 'revenueHigh': 5009600000}</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>154.7</v>
+        <v>154.26</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>0.031</t>
+          <t>0.0311</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>11.49</v>
+        <v>11.57</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>8.25</v>
+        <v>8.31</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -4404,7 +4404,7 @@
         <v>6.86</v>
       </c>
       <c r="P43" t="n">
-        <v>10.06</v>
+        <v>9.9</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>495.13</v>
+        <v>497.85</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.0109</t>
+          <t>0.0108</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-26', '2023-10-02'], 'earningsAverage': 3.65, 'earningsLow': 3.43, 'earningsHigh': 3.8, 'revenueAverage': 2329960000, 'revenueLow': 2308200000, 'revenueHigh': 2344000000}</t>
+          <t>{'earningsDate': ['2023-09-26', '2023-10-02'], 'earningsAverage': 3.66, 'earningsLow': 3.43, 'earningsHigh': 3.8, 'revenueAverage': 2329960000, 'revenueLow': 2308200000, 'revenueHigh': 2344000000}</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -4544,7 +4544,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -4557,7 +4557,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>3.5</v>
+        <v>3.51</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>167.21</v>
+        <v>163.76</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4670,7 +4670,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>0.0361</t>
+          <t>0.0369</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -4741,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>142.11</v>
+        <v>140.22</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4764,7 +4764,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>0.014400001</t>
+          <t>0.0145000005</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 2.33, 'earningsLow': 2.25, 'earningsHigh': 2.43, 'revenueAverage': 2216080000, 'revenueLow': 2079000000, 'revenueHigh': 2289360000}</t>
+          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 2.33, 'earningsLow': 2.25, 'earningsHigh': 2.43, 'revenueAverage': 2229310000, 'revenueLow': 2147000000, 'revenueHigh': 2289360000}</t>
         </is>
       </c>
       <c r="S47" t="inlineStr">
@@ -4822,7 +4822,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.56</v>
+        <v>3.48</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4858,7 +4858,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>0.17809999</t>
+          <t>0.17959999</t>
         </is>
       </c>
       <c r="N48" t="inlineStr"/>
@@ -5015,10 +5015,10 @@
         <v>153.75</v>
       </c>
       <c r="G50" t="n">
-        <v>10.2</v>
+        <v>10.13</v>
       </c>
       <c r="H50" t="n">
-        <v>153</v>
+        <v>151.95</v>
       </c>
       <c r="I50" t="n">
         <v>10.12</v>
@@ -5033,12 +5033,12 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2023-09-08</t>
+          <t>2023-10-10</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>0.1617</t>
+          <t>0.16469999</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -5050,7 +5050,7 @@
         <v>9.960000000000001</v>
       </c>
       <c r="P50" t="n">
-        <v>11.84</v>
+        <v>11.79</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
@@ -5109,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>182.06</v>
+        <v>183.85</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -5132,7 +5132,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>0.0117</t>
+          <t>0.0116</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -5203,7 +5203,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>89.25</v>
+        <v>89.73</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.0366</t>
+          <t>0.0361</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -5238,7 +5238,7 @@
         <v>78.09999999999999</v>
       </c>
       <c r="P52" t="n">
-        <v>102.21</v>
+        <v>101.39</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -5297,7 +5297,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>13.19</v>
+        <v>13.33</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -5315,12 +5315,12 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2023-08-30</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>0.1373</t>
+          <t>0.135</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -5332,7 +5332,7 @@
         <v>10.81</v>
       </c>
       <c r="P53" t="n">
-        <v>14.98</v>
+        <v>14.79</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
@@ -5391,10 +5391,10 @@
         <v>42</v>
       </c>
       <c r="G54" t="n">
-        <v>43.6</v>
+        <v>42.44</v>
       </c>
       <c r="H54" t="n">
-        <v>43.6</v>
+        <v>42.44</v>
       </c>
       <c r="I54" t="n">
         <v>39.28</v>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>98.95</v>
+        <v>100.12</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>0.0209</t>
+          <t>0.0208</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -5516,7 +5516,7 @@
         <v>72.41</v>
       </c>
       <c r="P55" t="n">
-        <v>99.65000000000001</v>
+        <v>100.56</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.3, 'earningsLow': 1.27, 'earningsHigh': 1.4, 'revenueAverage': 4190850000, 'revenueLow': 4078000000, 'revenueHigh': 4275900000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.3, 'earningsLow': 1.27, 'earningsHigh': 1.4, 'revenueAverage': 4194400000, 'revenueLow': 4078000000, 'revenueHigh': 4275900000}</t>
         </is>
       </c>
       <c r="S55" t="inlineStr">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -5575,7 +5575,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>225.29</v>
+        <v>224.07</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -5593,12 +5593,12 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2023-06-29</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.040999997</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -5610,7 +5610,7 @@
         <v>195.03</v>
       </c>
       <c r="P56" t="n">
-        <v>279.96</v>
+        <v>274.61</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -5669,7 +5669,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>114.73</v>
+        <v>116.22</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5692,7 +5692,7 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>0.0119</t>
+          <t>0.012</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
@@ -5763,7 +5763,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>5.94</v>
+        <v>5.8502</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>0.1409</t>
+          <t>0.1417</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
@@ -5857,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>17.2</v>
+        <v>16.71</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5880,7 +5880,7 @@
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>0.1559</t>
+          <t>0.1538</t>
         </is>
       </c>
       <c r="N59" t="inlineStr"/>
@@ -5947,7 +5947,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>97.61</v>
+        <v>97.31999999999999</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>0.0448</t>
+          <t>0.044699997</t>
         </is>
       </c>
       <c r="N60" t="inlineStr">
@@ -6064,7 +6064,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>0.1379</t>
+          <t>0.1357</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -6076,7 +6076,7 @@
         <v>16.7</v>
       </c>
       <c r="P61" t="n">
-        <v>21.87</v>
+        <v>20.81</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -6135,7 +6135,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>217.87</v>
+        <v>216.27</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -6229,7 +6229,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>9.869999999999999</v>
+        <v>10.06</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -6252,7 +6252,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>0.1534</t>
+          <t>0.152</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
@@ -6323,7 +6323,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>5.04</v>
+        <v>5.15</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -6346,7 +6346,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>0.1223</t>
+          <t>0.1182</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -6367,7 +6367,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.27, 'revenueAverage': 3968830000, 'revenueLow': 3968830000, 'revenueHigh': 3968830000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.27, 'revenueAverage': 3964070000, 'revenueLow': 3964070000, 'revenueHigh': 3964070000}</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6417,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>6.34</v>
+        <v>6.56</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -6440,7 +6440,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>0.1397</t>
+          <t>0.1341</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -6452,7 +6452,7 @@
         <v>5.1</v>
       </c>
       <c r="P65" t="n">
-        <v>7.94</v>
+        <v>7.87</v>
       </c>
       <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr">
@@ -6507,10 +6507,10 @@
         <v>70.75</v>
       </c>
       <c r="G66" t="n">
-        <v>13.82</v>
+        <v>13.6</v>
       </c>
       <c r="H66" t="n">
-        <v>69.09999999999999</v>
+        <v>68</v>
       </c>
       <c r="I66" t="n">
         <v>12.41</v>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>0.1163</t>
+          <t>0.114300005</t>
         </is>
       </c>
       <c r="N66" t="inlineStr"/>
@@ -6597,7 +6597,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>11.27</v>
+        <v>11.31</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>0.1432</t>
+          <t>0.142</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -6691,10 +6691,10 @@
         <v>1023.26</v>
       </c>
       <c r="G68" t="n">
-        <v>7.39</v>
+        <v>7.4</v>
       </c>
       <c r="H68" t="n">
-        <v>1034.6</v>
+        <v>1036</v>
       </c>
       <c r="I68" t="n">
         <v>6.9</v>
@@ -6714,7 +6714,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.1003</t>
+          <t>0.1014</t>
         </is>
       </c>
       <c r="N68" t="inlineStr"/>
@@ -6731,7 +6731,7 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-30'], 'earningsAverage': 0.14, 'earningsLow': 0.08, 'earningsHigh': 0.19, 'revenueAverage': 150710000, 'revenueLow': 141120000, 'revenueHigh': 162000000}</t>
+          <t>{'earningsDate': ['2023-11-30'], 'earningsAverage': 0.11, 'earningsLow': 0.02, 'earningsHigh': 0.19, 'revenueAverage': 148280000, 'revenueLow': 141000000, 'revenueHigh': 162000000}</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
@@ -6781,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>136.38</v>
+        <v>136.92</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>149.99</v>
+        <v>148.71</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -6882,7 +6882,7 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>0.025</t>
+          <t>0.0253</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
@@ -6953,7 +6953,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>5.36</v>
+        <v>5.39</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -6976,7 +6976,7 @@
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>0.1487</t>
+          <t>0.14930001</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
@@ -6988,7 +6988,7 @@
         <v>3.97</v>
       </c>
       <c r="P71" t="n">
-        <v>9.359999999999999</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
@@ -7070,7 +7070,7 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>0.17979999</t>
+          <t>0.17559999</t>
         </is>
       </c>
       <c r="N72" t="inlineStr"/>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -7137,7 +7137,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>689.9299999999999</v>
+        <v>691.99</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -7181,7 +7181,7 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26'], 'earningsAverage': 8.93, 'earningsLow': 8.61, 'earningsHigh': 9.29, 'revenueAverage': 4213280000, 'revenueLow': 4156000000, 'revenueHigh': 4272000000}</t>
+          <t>{'earningsDate': ['2023-10-26'], 'earningsAverage': 8.94, 'earningsLow': 8.61, 'earningsHigh': 9.29, 'revenueAverage': 4213790000, 'revenueLow': 4156000000, 'revenueHigh': 4272000000}</t>
         </is>
       </c>
       <c r="S73" t="inlineStr">
@@ -7231,7 +7231,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>7.21</v>
+        <v>7.18</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>0.069299996</t>
+          <t>0.067600004</t>
         </is>
       </c>
       <c r="N74" t="inlineStr">
@@ -7266,7 +7266,7 @@
         <v>4.05</v>
       </c>
       <c r="P74" t="n">
-        <v>14.57</v>
+        <v>14.27</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -7325,7 +7325,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>37.12</v>
+        <v>37.36</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7348,7 +7348,7 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>0.0295</t>
+          <t>0.0296</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
@@ -7357,7 +7357,7 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>36.775</v>
+        <v>36.78</v>
       </c>
       <c r="P75" t="n">
         <v>49.73</v>
@@ -7419,7 +7419,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>147.68</v>
+        <v>148.38</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -7442,7 +7442,7 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>0.045</t>
+          <t>0.044699997</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -7463,7 +7463,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.0, 'earningsLow': 1.95, 'earningsHigh': 2.1, 'revenueAverage': 13794200000, 'revenueLow': 13696500000, 'revenueHigh': 13982400000}</t>
+          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.15, 'earningsLow': 2.09, 'earningsHigh': 2.25, 'revenueAverage': 14793200000, 'revenueLow': 14688400000, 'revenueHigh': 14995000000}</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -7513,7 +7513,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>4.1116</v>
+        <v>4.05</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -7536,7 +7536,7 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>0.1268</t>
+          <t>0.1265</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
@@ -7607,7 +7607,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>20.99</v>
+        <v>21.83</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>0.2015</t>
+          <t>0.1906</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
@@ -7701,7 +7701,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>238.45</v>
+        <v>238.04</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -7724,7 +7724,7 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>0.0229</t>
+          <t>0.0235</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
@@ -7795,7 +7795,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>10.8</v>
+        <v>10.88</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -7830,7 +7830,7 @@
         <v>9.48</v>
       </c>
       <c r="P80" t="n">
-        <v>16.11</v>
+        <v>15.68</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7889,7 +7889,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>160.56</v>
+        <v>162.66</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -7912,7 +7912,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>0.0297</t>
+          <t>0.0293</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -7933,7 +7933,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.34, 'earningsLow': 2.24, 'earningsHigh': 2.41, 'revenueAverage': 19658800000, 'revenueLow': 19477400000, 'revenueHigh': 19913800000}</t>
+          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.5, 'earningsLow': 2.4, 'earningsHigh': 2.58, 'revenueAverage': 21079700000, 'revenueLow': 20888000000, 'revenueHigh': 21356000000}</t>
         </is>
       </c>
       <c r="S81" t="inlineStr">
@@ -7983,7 +7983,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.9152</v>
+        <v>0.9202</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -8006,7 +8006,7 @@
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.48650002</t>
         </is>
       </c>
       <c r="N82" t="inlineStr"/>
@@ -8014,7 +8014,7 @@
         <v>0.79</v>
       </c>
       <c r="P82" t="n">
-        <v>8.800000000000001</v>
+        <v>8.57</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
@@ -8023,7 +8023,7 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-28'], 'earningsAverage': -0.21, 'earningsLow': -0.38, 'earningsHigh': -0.04, 'revenueAverage': 547200000, 'revenueLow': 535600000, 'revenueHigh': 554800000}</t>
+          <t>{'earningsDate': ['2023-12-11', '2023-12-15'], 'earningsAverage': -0.21, 'earningsLow': -0.38, 'earningsHigh': -0.04, 'revenueAverage': 547200000, 'revenueLow': 535600000, 'revenueHigh': 554800000}</t>
         </is>
       </c>
       <c r="S82" t="inlineStr">
@@ -8060,7 +8060,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -8073,10 +8073,10 @@
         <v>1647.513</v>
       </c>
       <c r="G83" t="n">
-        <v>23.13</v>
+        <v>23.76</v>
       </c>
       <c r="H83" t="n">
-        <v>1595.97</v>
+        <v>1639.44</v>
       </c>
       <c r="I83" t="n">
         <v>23.01</v>
@@ -8104,7 +8104,7 @@
         <v>22.85</v>
       </c>
       <c r="P83" t="n">
-        <v>42.24</v>
+        <v>41.93</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
@@ -8163,7 +8163,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>127.48</v>
+        <v>128.05</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>0.0373</t>
+          <t>0.037</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
@@ -8257,7 +8257,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>58.33</v>
+        <v>58.88</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -8301,7 +8301,7 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.65, 'earningsLow': 0.63, 'earningsHigh': 0.67, 'revenueAverage': 10691000000, 'revenueLow': 10551300000, 'revenueHigh': 10945300000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.7, 'earningsLow': 0.68, 'earningsHigh': 0.72, 'revenueAverage': 11465300000, 'revenueLow': 11315400000, 'revenueHigh': 11738000000}</t>
         </is>
       </c>
       <c r="S85" t="inlineStr">
@@ -8351,7 +8351,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>12.45</v>
+        <v>12.61</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -8374,7 +8374,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>0.14039999</t>
+          <t>0.1364</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -8386,7 +8386,7 @@
         <v>9.94</v>
       </c>
       <c r="P86" t="n">
-        <v>19.99</v>
+        <v>19.75</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
@@ -8445,10 +8445,10 @@
         <v>569.3099999999999</v>
       </c>
       <c r="G87" t="n">
-        <v>26.71</v>
+        <v>26.85</v>
       </c>
       <c r="H87" t="n">
-        <v>560.91</v>
+        <v>563.85</v>
       </c>
       <c r="I87" t="n">
         <v>26.71</v>
@@ -8468,7 +8468,7 @@
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>0.0671</t>
+          <t>0.0674</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
@@ -8480,7 +8480,7 @@
         <v>26.35</v>
       </c>
       <c r="P87" t="n">
-        <v>39.64</v>
+        <v>38.55</v>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
@@ -8539,7 +8539,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>386.81</v>
+        <v>389.35</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -8562,7 +8562,7 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>0.013200001</t>
+          <t>0.013099999</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
@@ -8633,7 +8633,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>5.25</v>
+        <v>5.49</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -8723,7 +8723,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>5.9</v>
+        <v>5.91</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="n">
-        <v>5.82</v>
+        <v>5.78</v>
       </c>
       <c r="P90" t="n">
         <v>7.95</v>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 187130000, 'revenueLow': 155470000, 'revenueHigh': 208960000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 187390000, 'revenueLow': 155690000, 'revenueHigh': 209250000}</t>
         </is>
       </c>
       <c r="S90" t="inlineStr">
@@ -8813,7 +8813,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>231.29</v>
+        <v>231.91</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -8836,7 +8836,7 @@
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>0.0188</t>
+          <t>0.019</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
@@ -8857,7 +8857,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-21'], 'earningsAverage': 3.14, 'earningsLow': 3.04, 'earningsHigh': 3.37, 'revenueAverage': 21207200000, 'revenueLow': 20810000000, 'revenueHigh': 22583600000}</t>
+          <t>{'earningsDate': ['2023-11-21'], 'earningsAverage': 3.14, 'earningsLow': 3.04, 'earningsHigh': 3.37, 'revenueAverage': 21207600000, 'revenueLow': 20810000000, 'revenueHigh': 22583600000}</t>
         </is>
       </c>
       <c r="S91" t="inlineStr">
@@ -8894,7 +8894,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -8907,7 +8907,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1.17</v>
+        <v>1.21</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -8938,7 +8938,7 @@
         <v>1.125</v>
       </c>
       <c r="P92" t="n">
-        <v>4.06</v>
+        <v>3.965</v>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
@@ -8997,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>279.22</v>
+        <v>279.76</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -9020,7 +9020,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>0.0218</t>
+          <t>0.0217</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -9041,7 +9041,7 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 2.79, 'earningsLow': 2.65, 'earningsHigh': 3.05, 'revenueAverage': 6118640000, 'revenueLow': 5920530000, 'revenueHigh': 6295570000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 2.99, 'earningsLow': 2.84, 'earningsHigh': 3.27, 'revenueAverage': 6561760000, 'revenueLow': 6349300000, 'revenueHigh': 6751500000}</t>
         </is>
       </c>
       <c r="S93" t="inlineStr">
@@ -9091,7 +9091,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>79.95999999999999</v>
+        <v>81.40000000000001</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -9114,7 +9114,7 @@
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>0.0345</t>
+          <t>0.0339</t>
         </is>
       </c>
       <c r="N94" t="inlineStr">
@@ -9126,7 +9126,7 @@
         <v>75.77</v>
       </c>
       <c r="P94" t="n">
-        <v>92.39</v>
+        <v>92.02</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
@@ -9185,7 +9185,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>10.82</v>
+        <v>10.86</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -9279,7 +9279,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>80.7</v>
+        <v>81.75</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -9302,7 +9302,7 @@
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>0.0195</t>
+          <t>0.019299999</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
@@ -9373,7 +9373,7 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>106.24</v>
+        <v>107.89</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -9396,7 +9396,7 @@
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>0.056399997</t>
+          <t>0.0556</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
@@ -9417,7 +9417,7 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.21, 'earningsLow': 2.14, 'earningsHigh': 2.27, 'revenueAverage': 7514420000, 'revenueLow': 7490440000, 'revenueHigh': 7563260000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.36, 'earningsLow': 2.29, 'earningsHigh': 2.43, 'revenueAverage': 8056380000, 'revenueLow': 8032900000, 'revenueHigh': 8111000000}</t>
         </is>
       </c>
       <c r="S97" t="inlineStr">
@@ -9467,7 +9467,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>19.62</v>
+        <v>19.55</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -9507,7 +9507,7 @@
       </c>
       <c r="R98" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-11', '2023-09-15'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
+          <t>{'earningsDate': ['2023-09-12', '2023-09-15'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
         </is>
       </c>
       <c r="S98" t="inlineStr">
@@ -9557,7 +9557,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>3.92</v>
+        <v>3.84</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>0.1361</t>
+          <t>0.13270001</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
@@ -9651,7 +9651,7 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>232.8</v>
+        <v>234.87</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -9745,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>66.83</v>
+        <v>67.53</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -9768,7 +9768,7 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>0.028199999</t>
+          <t>0.0277</t>
         </is>
       </c>
       <c r="N101" t="inlineStr">
@@ -9780,7 +9780,7 @@
         <v>65.36</v>
       </c>
       <c r="P101" t="n">
-        <v>90.84999999999999</v>
+        <v>90.47</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
@@ -9826,7 +9826,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -9839,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>5.22</v>
+        <v>5.26</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -9857,12 +9857,12 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>2023-05-15</t>
+          <t>2023-08-14</t>
         </is>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>0.1481</t>
+          <t>0.1533</t>
         </is>
       </c>
       <c r="N102" t="inlineStr">
@@ -9878,7 +9878,7 @@
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>0.791825</t>
+          <t>0.784923</t>
         </is>
       </c>
       <c r="R102" t="inlineStr">
@@ -9920,7 +9920,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -9933,7 +9933,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>19.89</v>
+        <v>20.17</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -9951,7 +9951,7 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>2023-06-29</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="M103" t="inlineStr">
@@ -9968,7 +9968,7 @@
         <v>15.11</v>
       </c>
       <c r="P103" t="n">
-        <v>26.92</v>
+        <v>26.28</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
@@ -10027,7 +10027,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>164.94</v>
+        <v>163.17</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -10050,7 +10050,7 @@
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>0.012</t>
+          <t>0.0123000005</t>
         </is>
       </c>
       <c r="N104" t="inlineStr">
@@ -10071,7 +10071,7 @@
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 4.75, 'earningsLow': 4.19, 'earningsHigh': 5.57, 'revenueAverage': 8820360000, 'revenueLow': 8181000000, 'revenueHigh': 9235000000}</t>
+          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 4.67, 'earningsLow': 4.19, 'earningsHigh': 5.29, 'revenueAverage': 8715560000, 'revenueLow': 8181000000, 'revenueHigh': 9154570000}</t>
         </is>
       </c>
       <c r="S104" t="inlineStr">
@@ -10121,7 +10121,7 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>9.210000000000001</v>
+        <v>9.25</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -10144,7 +10144,7 @@
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>0.1261</t>
+          <t>0.1304</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
@@ -10160,7 +10160,7 @@
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>1.824038</t>
+          <t>1.826417</t>
         </is>
       </c>
       <c r="R105" t="inlineStr">
@@ -10202,7 +10202,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -10215,7 +10215,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>55.32</v>
+        <v>55.17</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -10238,7 +10238,7 @@
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>0.0557</t>
+          <t>0.0556</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -10296,7 +10296,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -10309,10 +10309,10 @@
         <v>2432.64</v>
       </c>
       <c r="G107" t="n">
-        <v>7.92</v>
+        <v>8.06</v>
       </c>
       <c r="H107" t="n">
-        <v>2534.4</v>
+        <v>2579.2</v>
       </c>
       <c r="I107" t="n">
         <v>7.76</v>
@@ -10342,14 +10342,10 @@
       <c r="P107" t="n">
         <v>10.5</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>1.367198</t>
-        </is>
-      </c>
+      <c r="Q107" t="inlineStr"/>
       <c r="R107" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-08'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 7510000, 'revenueLow': 7510000, 'revenueHigh': 7510000}</t>
+          <t>{'earningsDate': ['2023-12-11', '2023-12-15'], 'earningsAverage': 0.29, 'earningsLow': 0.29, 'earningsHigh': 0.29, 'revenueAverage': 6800000, 'revenueLow': 6800000, 'revenueHigh': 6800000}</t>
         </is>
       </c>
       <c r="S107" t="inlineStr">
@@ -10399,7 +10395,7 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>5.89</v>
+        <v>5.94</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -10422,7 +10418,7 @@
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>0.2583</t>
+          <t>0.2716</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -10434,7 +10430,7 @@
         <v>5.65</v>
       </c>
       <c r="P108" t="n">
-        <v>18.49</v>
+        <v>18.18</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
@@ -10493,7 +10489,7 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>9.26</v>
+        <v>9.34</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -10516,7 +10512,7 @@
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>0.2082</t>
+          <t>0.2056</t>
         </is>
       </c>
       <c r="N109" t="inlineStr">
@@ -10528,7 +10524,7 @@
         <v>7.95</v>
       </c>
       <c r="P109" t="n">
-        <v>12.85</v>
+        <v>12.66</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
@@ -10587,10 +10583,10 @@
         <v>369</v>
       </c>
       <c r="G110" t="n">
-        <v>5.2</v>
+        <v>5.18</v>
       </c>
       <c r="H110" t="n">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I110" t="n">
         <v>4.8</v>
@@ -10610,7 +10606,7 @@
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>0.1792</t>
+          <t>0.17879999</t>
         </is>
       </c>
       <c r="N110" t="inlineStr">
@@ -10681,7 +10677,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3.13</v>
+        <v>3.15</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -10704,7 +10700,7 @@
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>0.135</t>
+          <t>0.1342</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
@@ -10716,7 +10712,7 @@
         <v>2.6</v>
       </c>
       <c r="P111" t="n">
-        <v>3.95</v>
+        <v>3.9</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
@@ -10775,7 +10771,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>14.68</v>
+        <v>14.74</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -10798,7 +10794,7 @@
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>0.2522</t>
+          <t>0.25010002</t>
         </is>
       </c>
       <c r="N112" t="inlineStr">
@@ -10869,7 +10865,7 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>6.79</v>
+        <v>6.47</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -10892,7 +10888,7 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>0.074</t>
+          <t>0.0773</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
@@ -10904,7 +10900,7 @@
         <v>5.99</v>
       </c>
       <c r="P113" t="n">
-        <v>12.7</v>
+        <v>12.47</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
@@ -10913,7 +10909,7 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.0, 'earningsLow': 0.0, 'earningsHigh': 0.0, 'revenueAverage': 143590000, 'revenueLow': 143190000, 'revenueHigh': 144000000}</t>
+          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': -0.04, 'earningsLow': -0.04, 'earningsHigh': -0.04, 'revenueAverage': 143590000, 'revenueLow': 143190000, 'revenueHigh': 144000000}</t>
         </is>
       </c>
       <c r="S113" t="inlineStr">
@@ -10963,7 +10959,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>176.27</v>
+        <v>178.93</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -10986,7 +10982,7 @@
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>0.0274</t>
+          <t>0.027</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
@@ -11007,7 +11003,7 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-10', '2023-10-16'], 'earningsAverage': 2.01, 'earningsLow': 1.94, 'earningsHigh': 2.06, 'revenueAverage': 21849000000, 'revenueLow': 21265900000, 'revenueHigh': 22003500000}</t>
+          <t>{'earningsDate': ['2023-10-10', '2023-10-16'], 'earningsAverage': 2.15, 'earningsLow': 2.08, 'earningsHigh': 2.21, 'revenueAverage': 23431300000, 'revenueLow': 22806000000, 'revenueHigh': 23597000000}</t>
         </is>
       </c>
       <c r="S114" t="inlineStr">
@@ -11057,7 +11053,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>152.93</v>
+        <v>154.75</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -11080,7 +11076,7 @@
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>0.024600001</t>
+          <t>0.024300002</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">
@@ -11101,7 +11097,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.6, 'earningsLow': 1.55, 'earningsHigh': 1.66, 'revenueAverage': 20080700000, 'revenueLow': 19759000000, 'revenueHigh': 20558200000}</t>
+          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.71, 'earningsLow': 1.66, 'earningsHigh': 1.78, 'revenueAverage': 21543000000, 'revenueLow': 21190000000, 'revenueHigh': 22047000000}</t>
         </is>
       </c>
       <c r="S115" t="inlineStr">
@@ -11151,7 +11147,7 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>68.08</v>
+        <v>68.8</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -11174,7 +11170,7 @@
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>0.0127</t>
+          <t>0.0128999995</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
@@ -11245,7 +11241,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>135.7</v>
+        <v>136.35</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -11362,7 +11358,7 @@
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>0.1428</t>
+          <t>0.1419</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
@@ -11433,7 +11429,7 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>491.51</v>
+        <v>497.86</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -11456,7 +11452,7 @@
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>0.0055</t>
+          <t>0.0056</t>
         </is>
       </c>
       <c r="N119" t="inlineStr">
@@ -11477,7 +11473,7 @@
       </c>
       <c r="R119" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 4.2, 'earningsLow': 4.16, 'earningsHigh': 4.26, 'revenueAverage': 1536780000, 'revenueLow': 1508000000, 'revenueHigh': 1556300000}</t>
+          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 4.2, 'earningsLow': 4.16, 'earningsHigh': 4.26, 'revenueAverage': 1539290000, 'revenueLow': 1508000000, 'revenueHigh': 1572000000}</t>
         </is>
       </c>
       <c r="S119" t="inlineStr">
@@ -11527,7 +11523,7 @@
         <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>7.53</v>
+        <v>7.61</v>
       </c>
       <c r="H120" t="n">
         <v>0</v>
@@ -11550,7 +11546,7 @@
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>0.114700004</t>
+          <t>0.1129</t>
         </is>
       </c>
       <c r="N120" t="inlineStr">
@@ -11562,7 +11558,7 @@
         <v>4.45</v>
       </c>
       <c r="P120" t="n">
-        <v>7.63</v>
+        <v>7.66</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
@@ -11621,7 +11617,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>7.64</v>
+        <v>7.75</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -11644,7 +11640,7 @@
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>0.0829</t>
+          <t>0.0838</t>
         </is>
       </c>
       <c r="N121" t="inlineStr">
@@ -11715,7 +11711,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>3.54</v>
+        <v>3.61</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -11750,7 +11746,7 @@
         <v>2.985</v>
       </c>
       <c r="P122" t="n">
-        <v>4.476</v>
+        <v>4.4</v>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
@@ -11809,10 +11805,10 @@
         <v>1263.55</v>
       </c>
       <c r="G123" t="n">
-        <v>17.64</v>
+        <v>17.54</v>
       </c>
       <c r="H123" t="n">
-        <v>1305.36</v>
+        <v>1297.96</v>
       </c>
       <c r="I123" t="n">
         <v>16.91</v>
@@ -11832,7 +11828,7 @@
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>0.14479999</t>
+          <t>0.1454</t>
         </is>
       </c>
       <c r="N123" t="inlineStr"/>
@@ -11899,7 +11895,7 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>10.9</v>
+        <v>10.91</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -11922,7 +11918,7 @@
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>0.119399995</t>
+          <t>0.1193</t>
         </is>
       </c>
       <c r="N124" t="inlineStr">
@@ -11993,7 +11989,7 @@
         <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>271.45</v>
+        <v>273.65</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -12016,7 +12012,7 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>0.0089</t>
+          <t>0.0088</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
@@ -12087,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>141.58</v>
+        <v>131.66</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -12110,7 +12106,7 @@
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>0.030199999</t>
+          <t>0.0322</t>
         </is>
       </c>
       <c r="N126" t="inlineStr">
@@ -12119,7 +12115,7 @@
         </is>
       </c>
       <c r="O126" t="n">
-        <v>135.44</v>
+        <v>129</v>
       </c>
       <c r="P126" t="n">
         <v>163.07</v>
@@ -12131,7 +12127,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.52, 'revenueAverage': 1938990000, 'revenueLow': 1913390000, 'revenueHigh': 1959000000}</t>
+          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.52, 'revenueAverage': 1940630000, 'revenueLow': 1913390000, 'revenueHigh': 1959000000}</t>
         </is>
       </c>
       <c r="S126" t="inlineStr">
@@ -12181,7 +12177,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>40.4</v>
+        <v>40.56</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -12204,7 +12200,7 @@
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>0.082100004</t>
+          <t>0.0801</t>
         </is>
       </c>
       <c r="N127" t="inlineStr">
@@ -12216,7 +12212,7 @@
         <v>19.06</v>
       </c>
       <c r="P127" t="n">
-        <v>49.83</v>
+        <v>47.89</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
@@ -12275,7 +12271,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>8.550000000000001</v>
+        <v>8.9</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -12353,7 +12349,7 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>390.71</v>
+        <v>389.36</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -12376,7 +12372,7 @@
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>0.0091</t>
+          <t>0.0092</t>
         </is>
       </c>
       <c r="N129" t="inlineStr">
@@ -12397,7 +12393,7 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 3.07, 'earningsLow': 2.95, 'earningsHigh': 3.22, 'revenueAverage': 3033260000, 'revenueLow': 2956390000, 'revenueHigh': 3099880000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 3.07, 'earningsLow': 2.97, 'earningsHigh': 3.22, 'revenueAverage': 3033260000, 'revenueLow': 2956390000, 'revenueHigh': 3099880000}</t>
         </is>
       </c>
       <c r="S129" t="inlineStr">
@@ -12447,7 +12443,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>90.98999999999999</v>
+        <v>90.95</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -12470,7 +12466,7 @@
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>0.035099998</t>
+          <t>0.0356</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
@@ -12541,7 +12537,7 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>69.95</v>
+        <v>70.17</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -12564,7 +12560,7 @@
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>0.028900001</t>
+          <t>0.0286</t>
         </is>
       </c>
       <c r="N131" t="inlineStr">
@@ -12635,7 +12631,7 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>123.69</v>
+        <v>122.67</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -12658,7 +12654,7 @@
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>0.0349</t>
+          <t>0.0354</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
@@ -12729,7 +12725,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>11.15</v>
+        <v>11.16</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -12764,7 +12760,7 @@
         <v>9.41</v>
       </c>
       <c r="P133" t="n">
-        <v>13.64</v>
+        <v>13.47</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
@@ -12823,7 +12819,7 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>14.26</v>
+        <v>14.33</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -12846,7 +12842,7 @@
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>0.1447</t>
+          <t>0.1438</t>
         </is>
       </c>
       <c r="N134" t="inlineStr"/>
@@ -12913,7 +12909,7 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>109.24</v>
+        <v>110.1</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -12936,7 +12932,7 @@
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>0.0444</t>
+          <t>0.044699997</t>
         </is>
       </c>
       <c r="N135" t="inlineStr">
@@ -13007,7 +13003,7 @@
         <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>7.52</v>
+        <v>7.72</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -13042,7 +13038,7 @@
         <v>5.14</v>
       </c>
       <c r="P136" t="n">
-        <v>9.300000000000001</v>
+        <v>9.255000000000001</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
@@ -13101,10 +13097,10 @@
         <v>281.915</v>
       </c>
       <c r="G137" t="n">
-        <v>248.5</v>
+        <v>273.58</v>
       </c>
       <c r="H137" t="n">
-        <v>248.5</v>
+        <v>273.58</v>
       </c>
       <c r="I137" t="n">
         <v>103.85</v>
@@ -13129,7 +13125,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.75, 'earningsLow': 0.61, 'earningsHigh': 0.95, 'revenueAverage': 23005900000, 'revenueLow': 18901200000, 'revenueHigh': 25441500000}</t>
+          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.8, 'earningsLow': 0.65, 'earningsHigh': 1.02, 'revenueAverage': 24666900000, 'revenueLow': 20270000000, 'revenueHigh': 27284000000}</t>
         </is>
       </c>
       <c r="S137" t="inlineStr">
@@ -13179,7 +13175,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>13.44</v>
+        <v>13.57</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -13202,7 +13198,7 @@
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>0.1339</t>
+          <t>0.13260001</t>
         </is>
       </c>
       <c r="N138" t="inlineStr">
@@ -13214,7 +13210,7 @@
         <v>11.57</v>
       </c>
       <c r="P138" t="n">
-        <v>20.16</v>
+        <v>19.88</v>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
@@ -13273,7 +13269,7 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>21.99</v>
+        <v>21.43</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -13296,7 +13292,7 @@
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>0.0871</t>
+          <t>0.087299995</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
@@ -13305,7 +13301,7 @@
         </is>
       </c>
       <c r="O139" t="n">
-        <v>21.92</v>
+        <v>21.39</v>
       </c>
       <c r="P139" t="n">
         <v>42.29</v>
@@ -13317,7 +13313,7 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-11', '2023-10-16'], 'earningsAverage': 0.65, 'earningsLow': 0.63, 'earningsHigh': 0.67, 'revenueAverage': 32395100000, 'revenueLow': 31643400000, 'revenueHigh': 33349500000}</t>
+          <t>{'earningsDate': ['2023-10-11', '2023-10-16'], 'earningsAverage': 0.69, 'earningsLow': 0.68, 'earningsHigh': 0.72, 'revenueAverage': 34741200000, 'revenueLow': 33935000000, 'revenueHigh': 35764700000}</t>
         </is>
       </c>
       <c r="S139" t="inlineStr">
@@ -13367,7 +13363,7 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>10.55</v>
+        <v>10.52</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -13390,7 +13386,7 @@
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>0.1333</t>
+          <t>0.1331</t>
         </is>
       </c>
       <c r="N140" t="inlineStr">
@@ -13402,7 +13398,7 @@
         <v>7</v>
       </c>
       <c r="P140" t="n">
-        <v>14.28</v>
+        <v>14.12</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
@@ -13461,7 +13457,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>163.77</v>
+        <v>164.34</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -13496,7 +13492,7 @@
         <v>128.07</v>
       </c>
       <c r="P141" t="n">
-        <v>163.86</v>
+        <v>164.4806</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
@@ -13505,7 +13501,7 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-16'], 'earningsAverage': 1.4, 'earningsLow': 1.35, 'earningsHigh': 1.49, 'revenueAverage': 148132000000, 'revenueLow': 146360000000, 'revenueHigh': 150589000000}</t>
+          <t>{'earningsDate': ['2023-11-16'], 'earningsAverage': 1.5, 'earningsLow': 1.45, 'earningsHigh': 1.6, 'revenueAverage': 158860000000, 'revenueLow': 156959000000, 'revenueHigh': 161495000000}</t>
         </is>
       </c>
       <c r="S141" t="inlineStr">
@@ -13555,7 +13551,7 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>393.16</v>
+        <v>397.15</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -13649,7 +13645,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>115.61</v>
+        <v>114.16</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -13672,7 +13668,7 @@
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>0.0315</t>
+          <t>0.0319</t>
         </is>
       </c>
       <c r="N143" t="inlineStr">
@@ -13693,7 +13689,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.04, 'earningsLow': 1.82, 'earningsHigh': 2.43, 'revenueAverage': 75799500000, 'revenueLow': 55489700000, 'revenueHigh': 86385900000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.19, 'earningsLow': 1.95, 'earningsHigh': 2.61, 'revenueAverage': 81288900000, 'revenueLow': 59508300000, 'revenueHigh': 92642000000}</t>
         </is>
       </c>
       <c r="S143" t="inlineStr">
@@ -13743,7 +13739,7 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>11.44</v>
+        <v>11.43</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -13779,7 +13775,7 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': -1.08, 'earningsLow': -1.59, 'earningsHigh': -0.58, 'revenueAverage': 1365080000, 'revenueLow': 1230230000, 'revenueHigh': 1479000000}</t>
+          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': -1.14, 'earningsLow': -1.59, 'earningsHigh': -0.58, 'revenueAverage': 1345680000, 'revenueLow': 1230230000, 'revenueHigh': 1479000000}</t>
         </is>
       </c>
       <c r="S144" t="inlineStr">

</xml_diff>

<commit_message>
feat: analysis using machine learning
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>149.04</v>
+        <v>154.3</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -594,7 +594,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.0397</t>
+          <t>0.0385</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>102.45</v>
+        <v>102.659</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>7.06</v>
+        <v>7.065</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -782,7 +782,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.1702</t>
+          <t>0.16950001</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>10.49</v>
+        <v>10.35</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -876,7 +876,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.1306</t>
+          <t>0.132</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -888,7 +888,7 @@
         <v>7.52</v>
       </c>
       <c r="P5" t="n">
-        <v>13.42</v>
+        <v>13</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.21, 'earningsLow': 0.13, 'earningsHigh': 0.31, 'revenueAverage': 26190000, 'revenueLow': 23400000, 'revenueHigh': 29200000}</t>
+          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.21, 'earningsLow': 0.13, 'earningsHigh': 0.31, 'revenueAverage': 25450000, 'revenueLow': 21000000, 'revenueHigh': 29200000}</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>78.73999999999999</v>
+        <v>80.45999999999999</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -970,7 +970,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.0229</t>
+          <t>0.0226</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>248.2</v>
+        <v>247.93</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>13.3</v>
+        <v>12.83</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.1488</t>
+          <t>0.1515</t>
         </is>
       </c>
       <c r="N8" t="inlineStr"/>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>75.59</v>
+        <v>76.98</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.0222</t>
+          <t>0.022</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>12.45</v>
+        <v>12.65</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.1355</t>
+          <t>0.1378</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.83</v>
+        <v>10.055</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.14649999</t>
+          <t>0.145</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1494,7 +1494,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6.73</v>
+        <v>6.78</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.1189</t>
+          <t>0.1178</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>186.32</v>
+        <v>185.6799</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9.43</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.053000003</t>
+          <t>0.053200003</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>8.960000000000001</v>
+        <v>8.952500000000001</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>143.1</v>
+        <v>142.1405</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1898,7 +1898,7 @@
         <v>81.43000000000001</v>
       </c>
       <c r="P16" t="n">
-        <v>143.63</v>
+        <v>145.86</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.58, 'earningsLow': 0.44, 'earningsHigh': 0.71, 'revenueAverage': 141434000000, 'revenueLow': 138000000000, 'revenueHigh': 143193000000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.54, 'earningsLow': 0.41, 'earningsHigh': 0.66, 'revenueAverage': 131760000000, 'revenueLow': 128561000000, 'revenueHigh': 133399000000}</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>9.15</v>
+        <v>9.154999999999999</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.14220001</t>
+          <t>0.1399</t>
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>70.51000000000001</v>
+        <v>67.175</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.017</t>
+          <t>0.0176</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>302.8</v>
+        <v>306.8982</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0.0234</t>
+          <t>0.0229</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>10.75</v>
+        <v>10.77</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2253,12 +2253,12 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2023-06-29</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0.131</t>
+          <t>0.1294</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>19.84</v>
+        <v>20.735</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>0.1423</t>
+          <t>0.1361</t>
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
@@ -2360,7 +2360,7 @@
         <v>17.05</v>
       </c>
       <c r="P21" t="n">
-        <v>26.1</v>
+        <v>25.47</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>4.9</v>
+        <v>4.835</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0.9796</t>
+          <t>0.9836</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2454,7 +2454,7 @@
         <v>4.38</v>
       </c>
       <c r="P22" t="n">
-        <v>7.03</v>
+        <v>6.68</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>113.93</v>
+        <v>115.78</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>0.025999999</t>
+          <t>0.0257</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>10.9</v>
+        <v>10.72</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.1835</t>
+          <t>0.191</t>
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>8.970000000000001</v>
+        <v>8.9101</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.1159</t>
+          <t>0.1169</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2732,7 +2732,7 @@
         <v>6.96</v>
       </c>
       <c r="P25" t="n">
-        <v>9.779999999999999</v>
+        <v>9.68</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>4.78</v>
+        <v>5.005</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.159</t>
+          <t>0.1517</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2826,7 +2826,7 @@
         <v>3.42</v>
       </c>
       <c r="P26" t="n">
-        <v>8.49</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>267.18</v>
+        <v>263.675</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.0136</t>
+          <t>0.0138</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>25.96</v>
+        <v>26.36</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.0462</t>
+          <t>0.0458</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 0.62, 'earningsLow': 0.59, 'earningsHigh': 0.66, 'revenueAverage': 1589730000, 'revenueLow': 1482900000, 'revenueHigh': 1936000000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 0.61, 'earningsLow': 0.58, 'earningsHigh': 0.66, 'revenueAverage': 1587260000, 'revenueLow': 1482900000, 'revenueHigh': 1936000000}</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>5.89</v>
+        <v>5.425</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -3104,7 +3104,7 @@
         <v>4.78</v>
       </c>
       <c r="P29" t="n">
-        <v>22.8</v>
+        <v>20.91</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>73.40000000000001</v>
+        <v>73.09</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.210000000000001</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3351,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>89.73</v>
+        <v>87.645</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0.0223</t>
+          <t>0.0228</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>206.35</v>
+        <v>211.45</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3468,7 +3468,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>0.0168</t>
+          <t>0.0162</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -3526,7 +3526,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -3539,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>96.31999999999999</v>
+        <v>96.18000000000001</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3562,7 +3562,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>0.0113</t>
+          <t>0.0114</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -3633,10 +3633,10 @@
         <v>1446.798</v>
       </c>
       <c r="G35" t="n">
-        <v>3.99</v>
+        <v>4.01</v>
       </c>
       <c r="H35" t="n">
-        <v>1460.34</v>
+        <v>1467.66</v>
       </c>
       <c r="I35" t="n">
         <v>3.74</v>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>86.55</v>
+        <v>89.76690000000001</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>0.028199999</t>
+          <t>0.0271</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -3762,7 +3762,7 @@
         <v>85.23</v>
       </c>
       <c r="P36" t="n">
-        <v>112.89</v>
+        <v>108.05</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.97</v>
+        <v>6.045</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3856,7 +3856,7 @@
         <v>4.48</v>
       </c>
       <c r="P37" t="n">
-        <v>8.25</v>
+        <v>7.85</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3915,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>105.91</v>
+        <v>107.55</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>0.028299998</t>
+          <t>0.0277</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -4009,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>10.76</v>
+        <v>10.835</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>0.0725</t>
+          <t>0.0716</t>
         </is>
       </c>
       <c r="N39" t="inlineStr"/>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>73.95</v>
+        <v>73.61499999999999</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -4113,12 +4113,12 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2023-07-20</t>
+          <t>2023-10-20</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>0.025999999</t>
+          <t>0.026099999</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.8, 'earningsLow': 0.78, 'earningsHigh': 0.83, 'revenueAverage': 4813960000, 'revenueLow': 4720000000, 'revenueHigh': 5009600000}</t>
+          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.75, 'earningsLow': 0.73, 'earningsHigh': 0.77, 'revenueAverage': 4484690000, 'revenueLow': 4397150000, 'revenueHigh': 4666940000}</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>154.26</v>
+        <v>148.61</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>0.0311</t>
+          <t>0.0321</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>11.57</v>
+        <v>11.51</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>0.129</t>
+          <t>0.1301</t>
         </is>
       </c>
       <c r="N42" t="inlineStr"/>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>8.31</v>
+        <v>8.0212</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>0.1706</t>
+          <t>0.1702</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -4404,7 +4404,7 @@
         <v>6.86</v>
       </c>
       <c r="P43" t="n">
-        <v>9.9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>497.85</v>
+        <v>522.35</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.0108</t>
+          <t>0.0105</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4498,7 +4498,7 @@
         <v>370.93</v>
       </c>
       <c r="P44" t="n">
-        <v>518.71</v>
+        <v>524.76</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-26', '2023-10-02'], 'earningsAverage': 3.66, 'earningsLow': 3.43, 'earningsHigh': 3.8, 'revenueAverage': 2329960000, 'revenueLow': 2308200000, 'revenueHigh': 2344000000}</t>
+          <t>{'earningsDate': ['2023-09-26'], 'earningsAverage': 3.67, 'earningsLow': 3.43, 'earningsHigh': 3.95, 'revenueAverage': 2335620000, 'revenueLow': 2308200000, 'revenueHigh': 2396870000}</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -4580,7 +4580,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>0.1984</t>
+          <t>0.1967</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -4594,7 +4594,11 @@
       <c r="P45" t="n">
         <v>4.4</v>
       </c>
-      <c r="Q45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>1.394536</t>
+        </is>
+      </c>
       <c r="R45" t="inlineStr">
         <is>
           <t>{'earningsDate': [], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
@@ -4647,7 +4651,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>163.76</v>
+        <v>168.17</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4670,7 +4674,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>0.0369</t>
+          <t>0.0363</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -4691,7 +4695,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 3.28, 'earningsLow': 2.74, 'earningsHigh': 4.02, 'revenueAverage': 49214400000, 'revenueLow': 44069000000, 'revenueHigh': 56800000000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 3.06, 'earningsLow': 2.55, 'earningsHigh': 3.75, 'revenueAverage': 44183000000, 'revenueLow': 34192500000, 'revenueHigh': 52914900000}</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4741,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>140.22</v>
+        <v>144.44</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4764,7 +4768,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>0.0145000005</t>
+          <t>0.014400001</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -4835,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.48</v>
+        <v>3.56</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4858,7 +4862,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>0.17959999</t>
+          <t>0.18010001</t>
         </is>
       </c>
       <c r="N48" t="inlineStr"/>
@@ -4866,7 +4870,7 @@
         <v>3.36</v>
       </c>
       <c r="P48" t="n">
-        <v>5.14</v>
+        <v>4.85</v>
       </c>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr">
@@ -4921,10 +4925,10 @@
         <v>647</v>
       </c>
       <c r="G49" t="n">
-        <v>6.44</v>
+        <v>6.4999</v>
       </c>
       <c r="H49" t="n">
-        <v>644</v>
+        <v>649.99</v>
       </c>
       <c r="I49" t="n">
         <v>6.24</v>
@@ -5015,10 +5019,10 @@
         <v>153.75</v>
       </c>
       <c r="G50" t="n">
-        <v>10.13</v>
+        <v>10.19</v>
       </c>
       <c r="H50" t="n">
-        <v>151.95</v>
+        <v>152.85</v>
       </c>
       <c r="I50" t="n">
         <v>10.12</v>
@@ -5038,7 +5042,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>0.16469999</t>
+          <t>0.1658</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -5059,7 +5063,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': 0.32, 'earningsLow': 0.29, 'earningsHigh': 0.34, 'revenueAverage': 32650000, 'revenueLow': 31830000, 'revenueHigh': 33480000}</t>
+          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': 0.33, 'earningsLow': 0.29, 'earningsHigh': 0.36, 'revenueAverage': 33400000, 'revenueLow': 31830000, 'revenueHigh': 34900000}</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -5109,7 +5113,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>183.85</v>
+        <v>179.0825</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -5132,7 +5136,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>0.0116</t>
+          <t>0.0119</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -5190,7 +5194,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -5203,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>89.73</v>
+        <v>92.77500000000001</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -5226,7 +5230,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.0361</t>
+          <t>0.0354</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -5238,7 +5242,7 @@
         <v>78.09999999999999</v>
       </c>
       <c r="P52" t="n">
-        <v>101.39</v>
+        <v>100.92</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -5297,7 +5301,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>13.33</v>
+        <v>13.445</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -5320,7 +5324,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>0.135</t>
+          <t>0.1356</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -5332,7 +5336,7 @@
         <v>10.81</v>
       </c>
       <c r="P53" t="n">
-        <v>14.79</v>
+        <v>14.62</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
@@ -5378,7 +5382,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -5391,10 +5395,10 @@
         <v>42</v>
       </c>
       <c r="G54" t="n">
-        <v>42.44</v>
+        <v>42.56</v>
       </c>
       <c r="H54" t="n">
-        <v>42.44</v>
+        <v>42.56</v>
       </c>
       <c r="I54" t="n">
         <v>39.28</v>
@@ -5414,7 +5418,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>0.0706</t>
+          <t>0.0728</t>
         </is>
       </c>
       <c r="N54" t="inlineStr"/>
@@ -5431,7 +5435,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': -0.5, 'earningsLow': -1.12, 'earningsHigh': 0.11, 'revenueAverage': 80600000, 'revenueLow': 48700000, 'revenueHigh': 95580000}</t>
+          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': -0.46, 'earningsLow': -1.12, 'earningsHigh': 0.11, 'revenueAverage': 80600000, 'revenueLow': 48700000, 'revenueHigh': 95580000}</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
@@ -5481,7 +5485,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>100.12</v>
+        <v>99.52</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -5504,7 +5508,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>0.0208</t>
+          <t>0.021300001</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -5516,7 +5520,7 @@
         <v>72.41</v>
       </c>
       <c r="P55" t="n">
-        <v>100.56</v>
+        <v>100.62</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -5610,7 +5614,7 @@
         <v>195.03</v>
       </c>
       <c r="P56" t="n">
-        <v>274.61</v>
+        <v>261.32</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -5669,7 +5673,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>116.22</v>
+        <v>118.23</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5692,7 +5696,7 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>0.012</t>
+          <t>0.0117</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
@@ -5763,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>5.8502</v>
+        <v>6.0306</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5786,7 +5790,7 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>0.1417</t>
+          <t>0.1436</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
@@ -5844,7 +5848,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -5857,7 +5861,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>16.71</v>
+        <v>16.2</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5947,7 +5951,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>97.31999999999999</v>
+        <v>99.25749999999999</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -5970,7 +5974,7 @@
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>0.044699997</t>
+          <t>0.0437</t>
         </is>
       </c>
       <c r="N60" t="inlineStr">
@@ -6028,7 +6032,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -6041,7 +6045,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>20.63</v>
+        <v>19.94</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -6059,12 +6063,12 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>2023-09-12</t>
+          <t>2023-11-14</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>0.1357</t>
+          <t>0.14060001</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -6076,7 +6080,7 @@
         <v>16.7</v>
       </c>
       <c r="P61" t="n">
-        <v>20.81</v>
+        <v>20.8</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -6135,7 +6139,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>216.27</v>
+        <v>222.275</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -6158,7 +6162,7 @@
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>0.0242</t>
+          <t>0.0238</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
@@ -6216,7 +6220,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -6229,7 +6233,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>10.06</v>
+        <v>9.4</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -6252,7 +6256,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>0.152</t>
+          <t>0.1463</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
@@ -6264,7 +6268,7 @@
         <v>7.51</v>
       </c>
       <c r="P63" t="n">
-        <v>12.25</v>
+        <v>11.35</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
@@ -6323,7 +6327,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>5.15</v>
+        <v>5.275</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -6346,7 +6350,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>0.1182</t>
+          <t>0.1155</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -6367,7 +6371,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.23, 'earningsHigh': 0.27, 'revenueAverage': 3964070000, 'revenueLow': 3964070000, 'revenueHigh': 3964070000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.25, 'earningsLow': 0.24, 'earningsHigh': 0.27, 'revenueAverage': 4036630000, 'revenueLow': 4036630000, 'revenueHigh': 4036630000}</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6404,7 +6408,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -6417,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>6.56</v>
+        <v>6.05</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -6440,7 +6444,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>0.1341</t>
+          <t>0.135</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -6452,9 +6456,13 @@
         <v>5.1</v>
       </c>
       <c r="P65" t="n">
-        <v>7.87</v>
-      </c>
-      <c r="Q65" t="inlineStr"/>
+        <v>7.45</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>1.260719</t>
+        </is>
+      </c>
       <c r="R65" t="inlineStr">
         <is>
           <t>{'earningsDate': [], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
@@ -6494,7 +6502,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -6507,10 +6515,10 @@
         <v>70.75</v>
       </c>
       <c r="G66" t="n">
-        <v>13.6</v>
+        <v>13.895</v>
       </c>
       <c r="H66" t="n">
-        <v>68</v>
+        <v>69.47499999999999</v>
       </c>
       <c r="I66" t="n">
         <v>12.41</v>
@@ -6530,7 +6538,7 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>0.114300005</t>
+          <t>0.118</t>
         </is>
       </c>
       <c r="N66" t="inlineStr"/>
@@ -6547,7 +6555,7 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-07', '2023-11-13'], 'earningsAverage': 0.01, 'earningsLow': -0.13, 'earningsHigh': 0.21, 'revenueAverage': 52300000, 'revenueLow': 48700000, 'revenueHigh': 61510000}</t>
+          <t>{'earningsDate': ['2023-11-07', '2023-11-13'], 'earningsAverage': 0.0, 'earningsLow': -0.13, 'earningsHigh': 0.21, 'revenueAverage': 51960000, 'revenueLow': 48700000, 'revenueHigh': 61510000}</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
@@ -6597,7 +6605,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>11.31</v>
+        <v>11.1395</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -6620,7 +6628,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>0.142</t>
+          <t>0.1401</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -6691,10 +6699,10 @@
         <v>1023.26</v>
       </c>
       <c r="G68" t="n">
-        <v>7.4</v>
+        <v>7.75</v>
       </c>
       <c r="H68" t="n">
-        <v>1036</v>
+        <v>1085</v>
       </c>
       <c r="I68" t="n">
         <v>6.9</v>
@@ -6714,7 +6722,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.1014</t>
+          <t>0.1008</t>
         </is>
       </c>
       <c r="N68" t="inlineStr"/>
@@ -6781,7 +6789,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>136.92</v>
+        <v>137.28</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -6800,7 +6808,7 @@
         <v>83.34</v>
       </c>
       <c r="P69" t="n">
-        <v>138</v>
+        <v>138.7</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
@@ -6859,7 +6867,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>148.71</v>
+        <v>149.64</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -6953,7 +6961,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>5.39</v>
+        <v>5.3427</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -6976,7 +6984,7 @@
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>0.14930001</t>
+          <t>0.1515</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
@@ -6988,7 +6996,7 @@
         <v>3.97</v>
       </c>
       <c r="P71" t="n">
-        <v>9.279999999999999</v>
+        <v>8.859999999999999</v>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
@@ -7047,7 +7055,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>7.8</v>
+        <v>8.06</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -7070,7 +7078,7 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>0.17559999</t>
+          <t>0.1685</t>
         </is>
       </c>
       <c r="N72" t="inlineStr"/>
@@ -7137,7 +7145,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>691.99</v>
+        <v>696.6</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -7160,7 +7168,7 @@
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>0.0108</t>
+          <t>0.0109</t>
         </is>
       </c>
       <c r="N73" t="inlineStr">
@@ -7181,7 +7189,7 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26'], 'earningsAverage': 8.94, 'earningsLow': 8.61, 'earningsHigh': 9.29, 'revenueAverage': 4213790000, 'revenueLow': 4156000000, 'revenueHigh': 4272000000}</t>
+          <t>{'earningsDate': ['2023-10-26'], 'earningsAverage': 8.94, 'earningsLow': 8.61, 'earningsHigh': 9.29, 'revenueAverage': 4215330000, 'revenueLow': 4165870000, 'revenueHigh': 4272000000}</t>
         </is>
       </c>
       <c r="S73" t="inlineStr">
@@ -7231,7 +7239,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>7.18</v>
+        <v>6.95</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -7254,7 +7262,7 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>0.067600004</t>
+          <t>0.0715</t>
         </is>
       </c>
       <c r="N74" t="inlineStr">
@@ -7266,7 +7274,7 @@
         <v>4.05</v>
       </c>
       <c r="P74" t="n">
-        <v>14.27</v>
+        <v>13.11</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
@@ -7312,7 +7320,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -7325,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>37.36</v>
+        <v>38.42</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7348,7 +7356,7 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>0.0296</t>
+          <t>0.0286</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
@@ -7419,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>148.38</v>
+        <v>147.72</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -7442,7 +7450,7 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>0.044699997</t>
+          <t>0.045300003</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -7463,7 +7471,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.15, 'earningsLow': 2.09, 'earningsHigh': 2.25, 'revenueAverage': 14793200000, 'revenueLow': 14688400000, 'revenueHigh': 14995000000}</t>
+          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.0, 'earningsLow': 1.95, 'earningsHigh': 2.1, 'revenueAverage': 13781300000, 'revenueLow': 13683700000, 'revenueHigh': 13969300000}</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -7513,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>4.05</v>
+        <v>4.252</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -7536,7 +7544,7 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>0.1265</t>
+          <t>0.1284</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
@@ -7607,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>21.83</v>
+        <v>20.63</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -7630,7 +7638,7 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>0.1906</t>
+          <t>0.1821</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
@@ -7701,7 +7709,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>238.04</v>
+        <v>239.38</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -7724,7 +7732,7 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>0.0235</t>
+          <t>0.0234</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
@@ -7745,7 +7753,7 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.46, 'earningsLow': 2.42, 'earningsHigh': 2.5, 'revenueAverage': 4108930000, 'revenueLow': 4031000000, 'revenueHigh': 4164000000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.46, 'earningsLow': 2.42, 'earningsHigh': 2.5, 'revenueAverage': 4109370000, 'revenueLow': 4031000000, 'revenueHigh': 4164000000}</t>
         </is>
       </c>
       <c r="S79" t="inlineStr">
@@ -7795,7 +7803,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>10.88</v>
+        <v>10.775</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -7818,7 +7826,7 @@
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>0.1491</t>
+          <t>0.14840001</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
@@ -7830,7 +7838,7 @@
         <v>9.48</v>
       </c>
       <c r="P80" t="n">
-        <v>15.68</v>
+        <v>15.56</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -7889,7 +7897,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>162.66</v>
+        <v>163.96</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -7912,7 +7920,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>0.0293</t>
+          <t>0.029000001</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -7933,7 +7941,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.5, 'earningsLow': 2.4, 'earningsHigh': 2.58, 'revenueAverage': 21079700000, 'revenueLow': 20888000000, 'revenueHigh': 21356000000}</t>
+          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.34, 'earningsLow': 2.24, 'earningsHigh': 2.4, 'revenueAverage': 19599800000, 'revenueLow': 19181700000, 'revenueHigh': 19895200000}</t>
         </is>
       </c>
       <c r="S81" t="inlineStr">
@@ -7983,7 +7991,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.9202</v>
+        <v>0.9101</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -8004,17 +8012,13 @@
           <t>2022-09-08</t>
         </is>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>0.48650002</t>
-        </is>
-      </c>
+      <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="n">
         <v>0.79</v>
       </c>
       <c r="P82" t="n">
-        <v>8.57</v>
+        <v>8.49</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
@@ -8096,7 +8100,7 @@
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>0.5655</t>
+          <t>0.5452</t>
         </is>
       </c>
       <c r="N83" t="inlineStr"/>
@@ -8104,7 +8108,7 @@
         <v>22.85</v>
       </c>
       <c r="P83" t="n">
-        <v>41.93</v>
+        <v>41.06</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
@@ -8113,7 +8117,7 @@
       </c>
       <c r="R83" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-28', '2023-12-04'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
+          <t>{'earningsDate': ['2023-11-28', '2023-12-04'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': 1607000000, 'revenueLow': 1607000000, 'revenueHigh': 1607000000}</t>
         </is>
       </c>
       <c r="S83" t="inlineStr">
@@ -8163,7 +8167,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>128.05</v>
+        <v>126.555</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -8186,7 +8190,7 @@
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>0.037</t>
+          <t>0.0375</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
@@ -8244,7 +8248,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -8257,7 +8261,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>58.88</v>
+        <v>58.5592</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -8301,7 +8305,7 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.7, 'earningsLow': 0.68, 'earningsHigh': 0.72, 'revenueAverage': 11465300000, 'revenueLow': 11315400000, 'revenueHigh': 11738000000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 0.65, 'earningsLow': 0.63, 'earningsHigh': 0.67, 'revenueAverage': 10681100000, 'revenueLow': 10541400000, 'revenueHigh': 10935100000}</t>
         </is>
       </c>
       <c r="S85" t="inlineStr">
@@ -8351,7 +8355,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>12.61</v>
+        <v>12.64</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -8374,7 +8378,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>0.1364</t>
+          <t>0.1362</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -8386,7 +8390,7 @@
         <v>9.94</v>
       </c>
       <c r="P86" t="n">
-        <v>19.75</v>
+        <v>19.41</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
@@ -8445,10 +8449,10 @@
         <v>569.3099999999999</v>
       </c>
       <c r="G87" t="n">
-        <v>26.85</v>
+        <v>26.9</v>
       </c>
       <c r="H87" t="n">
-        <v>563.85</v>
+        <v>564.9</v>
       </c>
       <c r="I87" t="n">
         <v>26.71</v>
@@ -8468,7 +8472,7 @@
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>0.0674</t>
+          <t>0.0671</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
@@ -8477,7 +8481,7 @@
         </is>
       </c>
       <c r="O87" t="n">
-        <v>26.35</v>
+        <v>26.08</v>
       </c>
       <c r="P87" t="n">
         <v>38.55</v>
@@ -8539,7 +8543,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>389.35</v>
+        <v>392.61</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -8562,7 +8566,7 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>0.013099999</t>
+          <t>0.013200001</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
@@ -8633,7 +8637,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>5.49</v>
+        <v>5.66</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -8656,7 +8660,7 @@
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>0.1981</t>
+          <t>0.1754</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
@@ -8670,7 +8674,11 @@
       <c r="P89" t="n">
         <v>6.48</v>
       </c>
-      <c r="Q89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>0.439162</t>
+        </is>
+      </c>
       <c r="R89" t="inlineStr">
         <is>
           <t>{'earningsDate': [], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
@@ -8723,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>5.91</v>
+        <v>6.02</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -8746,7 +8754,7 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>0.1356</t>
+          <t>0.1331</t>
         </is>
       </c>
       <c r="N90" t="inlineStr"/>
@@ -8763,7 +8771,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.04, 'earningsLow': 0.0, 'earningsHigh': 0.08, 'revenueAverage': 187390000, 'revenueLow': 155690000, 'revenueHigh': 209250000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.01, 'earningsLow': 0.01, 'earningsHigh': 0.01, 'revenueAverage': 194910000, 'revenueLow': 194910000, 'revenueHigh': 194910000}</t>
         </is>
       </c>
       <c r="S90" t="inlineStr">
@@ -8813,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>231.91</v>
+        <v>225</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -8836,7 +8844,7 @@
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>0.019</t>
+          <t>0.0191</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
@@ -8857,7 +8865,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-21'], 'earningsAverage': 3.14, 'earningsLow': 3.04, 'earningsHigh': 3.37, 'revenueAverage': 21207600000, 'revenueLow': 20810000000, 'revenueHigh': 22583600000}</t>
+          <t>{'earningsDate': ['2023-11-21'], 'earningsAverage': 3.13, 'earningsLow': 2.89, 'earningsHigh': 3.37, 'revenueAverage': 21207600000, 'revenueLow': 20810000000, 'revenueHigh': 22583600000}</t>
         </is>
       </c>
       <c r="S91" t="inlineStr">
@@ -8907,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1.21</v>
+        <v>1.19</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -8930,7 +8938,7 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>0.0761</t>
+          <t>0.0754</t>
         </is>
       </c>
       <c r="N92" t="inlineStr"/>
@@ -8938,7 +8946,7 @@
         <v>1.125</v>
       </c>
       <c r="P92" t="n">
-        <v>3.965</v>
+        <v>3.6</v>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
@@ -8947,7 +8955,7 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-21', '2023-11-27'], 'earningsAverage': 0.03, 'earningsLow': 0.02, 'earningsHigh': 0.03, 'revenueAverage': 1212340000, 'revenueLow': 1149490000, 'revenueHigh': 1275190000}</t>
+          <t>{'earningsDate': ['2023-11-21', '2023-11-27'], 'earningsAverage': 0.03, 'earningsLow': 0.02, 'earningsHigh': 0.03, 'revenueAverage': 1200680000, 'revenueLow': 1138430000, 'revenueHigh': 1262930000}</t>
         </is>
       </c>
       <c r="S92" t="inlineStr">
@@ -8997,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>279.76</v>
+        <v>282.77</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -9020,7 +9028,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>0.0217</t>
+          <t>0.0216</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -9041,7 +9049,7 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 2.99, 'earningsLow': 2.84, 'earningsHigh': 3.27, 'revenueAverage': 6561760000, 'revenueLow': 6349300000, 'revenueHigh': 6751500000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 2.79, 'earningsLow': 2.65, 'earningsHigh': 3.05, 'revenueAverage': 6112940000, 'revenueLow': 5915010000, 'revenueHigh': 6289700000}</t>
         </is>
       </c>
       <c r="S93" t="inlineStr">
@@ -9091,7 +9099,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>81.40000000000001</v>
+        <v>82.19499999999999</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -9185,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>10.86</v>
+        <v>10.84</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -9208,7 +9216,7 @@
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>0.1294</t>
+          <t>0.1308</t>
         </is>
       </c>
       <c r="N95" t="inlineStr">
@@ -9279,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>81.75</v>
+        <v>80.26000000000001</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -9323,7 +9331,7 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-03'], 'earningsAverage': 0.65, 'earningsLow': 0.64, 'earningsHigh': 0.67, 'revenueAverage': 1696400000, 'revenueLow': 1671000000, 'revenueHigh': 1719000000}</t>
+          <t>{'earningsDate': ['2023-10-03'], 'earningsAverage': 0.65, 'earningsLow': 0.63, 'earningsHigh': 0.67, 'revenueAverage': 1697590000, 'revenueLow': 1671000000, 'revenueHigh': 1719000000}</t>
         </is>
       </c>
       <c r="S96" t="inlineStr">
@@ -9373,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>107.89</v>
+        <v>101.86</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -9396,7 +9404,7 @@
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>0.0556</t>
+          <t>0.055999998</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
@@ -9417,7 +9425,7 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.36, 'earningsLow': 2.29, 'earningsHigh': 2.43, 'revenueAverage': 8056380000, 'revenueLow': 8032900000, 'revenueHigh': 8111000000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
         </is>
       </c>
       <c r="S97" t="inlineStr">
@@ -9467,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>19.55</v>
+        <v>20.36</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -9489,25 +9497,17 @@
         </is>
       </c>
       <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr">
-        <is>
-          <t>11.93</t>
-        </is>
-      </c>
+      <c r="N98" t="inlineStr"/>
       <c r="O98" t="n">
         <v>16.56</v>
       </c>
       <c r="P98" t="n">
         <v>29</v>
       </c>
-      <c r="Q98" t="inlineStr">
-        <is>
-          <t>0.969225</t>
-        </is>
-      </c>
+      <c r="Q98" t="inlineStr"/>
       <c r="R98" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-09-12', '2023-09-15'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
+          <t>{'earningsDate': ['2023-12-11', '2023-12-15'], 'earningsAverage': {}, 'earningsLow': {}, 'earningsHigh': {}, 'revenueAverage': {}, 'revenueLow': {}, 'revenueHigh': {}}</t>
         </is>
       </c>
       <c r="S98" t="inlineStr">
@@ -9544,7 +9544,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -9557,7 +9557,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>3.84</v>
+        <v>3.745</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>0.13270001</t>
+          <t>0.1376</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
@@ -9651,7 +9651,7 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>234.87</v>
+        <v>233.075</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -9695,7 +9695,7 @@
       </c>
       <c r="R100" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-08-22'], 'earningsAverage': 2.4, 'earningsLow': 2.35, 'earningsHigh': 2.44, 'revenueAverage': 707460000, 'revenueLow': 703200000, 'revenueHigh': 716000000}</t>
+          <t>{'earningsDate': ['2023-12-12', '2023-12-18'], 'earningsAverage': 2.4, 'earningsLow': 2.35, 'earningsHigh': 2.44, 'revenueAverage': 707460000, 'revenueLow': 703200000, 'revenueHigh': 716000000}</t>
         </is>
       </c>
       <c r="S100" t="inlineStr">
@@ -9732,7 +9732,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -9745,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>67.53</v>
+        <v>69.4036</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -9768,7 +9768,7 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>0.0277</t>
+          <t>0.0273</t>
         </is>
       </c>
       <c r="N101" t="inlineStr">
@@ -9780,7 +9780,7 @@
         <v>65.36</v>
       </c>
       <c r="P101" t="n">
-        <v>90.47</v>
+        <v>88.61</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
@@ -9826,7 +9826,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -9839,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>5.26</v>
+        <v>5.27</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -9862,7 +9862,7 @@
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>0.1533</t>
+          <t>0.1528</t>
         </is>
       </c>
       <c r="N102" t="inlineStr">
@@ -9933,7 +9933,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>20.17</v>
+        <v>20.53</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -9956,7 +9956,7 @@
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>0.13069999</t>
+          <t>0.1295</t>
         </is>
       </c>
       <c r="N103" t="inlineStr">
@@ -9968,7 +9968,7 @@
         <v>15.11</v>
       </c>
       <c r="P103" t="n">
-        <v>26.28</v>
+        <v>24.72</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
@@ -10027,7 +10027,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>163.17</v>
+        <v>161.165</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -10071,7 +10071,7 @@
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 4.67, 'earningsLow': 4.19, 'earningsHigh': 5.29, 'revenueAverage': 8715560000, 'revenueLow': 8181000000, 'revenueHigh': 9154570000}</t>
+          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 4.65, 'earningsLow': 4.19, 'earningsHigh': 4.96, 'revenueAverage': 8558290000, 'revenueLow': 7924000000, 'revenueHigh': 9154570000}</t>
         </is>
       </c>
       <c r="S104" t="inlineStr">
@@ -10108,7 +10108,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -10121,7 +10121,7 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>9.25</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -10139,12 +10139,12 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>2023-06-15</t>
+          <t>2023-09-20</t>
         </is>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>0.1304</t>
+          <t>0.1257</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
@@ -10215,7 +10215,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>55.17</v>
+        <v>54.6275</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -10233,12 +10233,12 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>2023-08-31</t>
+          <t>2023-09-29</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>0.0556</t>
+          <t>0.0558</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -10247,7 +10247,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>54.76</v>
+        <v>54.52</v>
       </c>
       <c r="P106" t="n">
         <v>68.84999999999999</v>
@@ -10296,7 +10296,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -10309,10 +10309,10 @@
         <v>2432.64</v>
       </c>
       <c r="G107" t="n">
-        <v>8.06</v>
+        <v>7.29</v>
       </c>
       <c r="H107" t="n">
-        <v>2579.2</v>
+        <v>2332.8</v>
       </c>
       <c r="I107" t="n">
         <v>7.76</v>
@@ -10337,7 +10337,7 @@
       </c>
       <c r="N107" t="inlineStr"/>
       <c r="O107" t="n">
-        <v>7.71</v>
+        <v>7.26</v>
       </c>
       <c r="P107" t="n">
         <v>10.5</v>
@@ -10395,7 +10395,7 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>5.94</v>
+        <v>5.99</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -10418,7 +10418,7 @@
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>0.2716</t>
+          <t>0.2593</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -10430,7 +10430,7 @@
         <v>5.65</v>
       </c>
       <c r="P108" t="n">
-        <v>18.18</v>
+        <v>18.1</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
@@ -10476,7 +10476,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D109" t="n">
@@ -10489,7 +10489,7 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>9.34</v>
+        <v>9.5092</v>
       </c>
       <c r="H109" t="n">
         <v>0</v>
@@ -10507,12 +10507,12 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>2023-08-30</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>0.2056</t>
+          <t>0.206</t>
         </is>
       </c>
       <c r="N109" t="inlineStr">
@@ -10583,10 +10583,10 @@
         <v>369</v>
       </c>
       <c r="G110" t="n">
-        <v>5.18</v>
+        <v>4.98</v>
       </c>
       <c r="H110" t="n">
-        <v>518</v>
+        <v>498.0000000000001</v>
       </c>
       <c r="I110" t="n">
         <v>4.8</v>
@@ -10664,7 +10664,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -10677,7 +10677,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3.15</v>
+        <v>3.05</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -10712,7 +10712,7 @@
         <v>2.6</v>
       </c>
       <c r="P111" t="n">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
@@ -10771,7 +10771,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>14.74</v>
+        <v>15.33</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -10794,7 +10794,7 @@
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>0.25010002</t>
+          <t>0.23889999</t>
         </is>
       </c>
       <c r="N112" t="inlineStr">
@@ -10815,7 +10815,7 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.78, 'earningsLow': 0.7, 'earningsHigh': 0.87, 'revenueAverage': 24764600000, 'revenueLow': 24028500000, 'revenueHigh': 25998000000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.78, 'earningsLow': 0.7, 'earningsHigh': 0.87, 'revenueAverage': 24710200000, 'revenueLow': 23920800000, 'revenueHigh': 25998000000}</t>
         </is>
       </c>
       <c r="S112" t="inlineStr">
@@ -10865,7 +10865,7 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>6.47</v>
+        <v>6.4</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -10888,7 +10888,7 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>0.0773</t>
+          <t>0.081199996</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
@@ -10900,7 +10900,7 @@
         <v>5.99</v>
       </c>
       <c r="P113" t="n">
-        <v>12.47</v>
+        <v>12.21</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
@@ -10959,7 +10959,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>178.93</v>
+        <v>181.33</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -10982,7 +10982,7 @@
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>0.027</t>
+          <t>0.0271</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
@@ -11003,7 +11003,7 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-10', '2023-10-16'], 'earningsAverage': 2.15, 'earningsLow': 2.08, 'earningsHigh': 2.21, 'revenueAverage': 23431300000, 'revenueLow': 22806000000, 'revenueHigh': 23597000000}</t>
+          <t>{'earningsDate': ['2023-10-10'], 'earningsAverage': 2.01, 'earningsLow': 1.94, 'earningsHigh': 2.06, 'revenueAverage': 21829200000, 'revenueLow': 21246100000, 'revenueHigh': 21983000000}</t>
         </is>
       </c>
       <c r="S114" t="inlineStr">
@@ -11053,7 +11053,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>154.75</v>
+        <v>155.25</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -11097,7 +11097,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.71, 'earningsLow': 1.66, 'earningsHigh': 1.78, 'revenueAverage': 21543000000, 'revenueLow': 21190000000, 'revenueHigh': 22047000000}</t>
+          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.59, 'earningsLow': 1.55, 'earningsHigh': 1.66, 'revenueAverage': 20069500000, 'revenueLow': 19740600000, 'revenueHigh': 20539000000}</t>
         </is>
       </c>
       <c r="S115" t="inlineStr">
@@ -11147,7 +11147,7 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>68.8</v>
+        <v>66.79000000000001</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -11241,7 +11241,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>136.35</v>
+        <v>135.49</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -11264,7 +11264,7 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>0.0191</t>
+          <t>0.0195</t>
         </is>
       </c>
       <c r="N117" t="inlineStr">
@@ -11322,7 +11322,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -11335,7 +11335,7 @@
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>19.45</v>
+        <v>19.06</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -11358,7 +11358,7 @@
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>0.1419</t>
+          <t>0.1449</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
@@ -11429,7 +11429,7 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>497.86</v>
+        <v>498.02</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -11558,7 +11558,7 @@
         <v>4.45</v>
       </c>
       <c r="P120" t="n">
-        <v>7.66</v>
+        <v>7.655</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
@@ -11617,7 +11617,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>7.75</v>
+        <v>7.86</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -11711,7 +11711,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>3.61</v>
+        <v>3.695</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -11746,7 +11746,7 @@
         <v>2.985</v>
       </c>
       <c r="P122" t="n">
-        <v>4.4</v>
+        <v>4.31</v>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
@@ -11805,10 +11805,10 @@
         <v>1263.55</v>
       </c>
       <c r="G123" t="n">
-        <v>17.54</v>
+        <v>18.285</v>
       </c>
       <c r="H123" t="n">
-        <v>1297.96</v>
+        <v>1353.09</v>
       </c>
       <c r="I123" t="n">
         <v>16.91</v>
@@ -11828,7 +11828,7 @@
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>0.1454</t>
+          <t>0.1462</t>
         </is>
       </c>
       <c r="N123" t="inlineStr"/>
@@ -11845,7 +11845,7 @@
       </c>
       <c r="R123" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-14', '2023-11-20'], 'earningsAverage': 0.31, 'earningsLow': 0.12, 'earningsHigh': 0.68, 'revenueAverage': 156740000, 'revenueLow': 140770000, 'revenueHigh': 191180000}</t>
+          <t>{'earningsDate': ['2023-11-14', '2023-11-20'], 'earningsAverage': 0.31, 'earningsLow': 0.12, 'earningsHigh': 0.68, 'revenueAverage': 157540000, 'revenueLow': 140770000, 'revenueHigh': 191180000}</t>
         </is>
       </c>
       <c r="S123" t="inlineStr">
@@ -11895,7 +11895,7 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>10.91</v>
+        <v>11</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -11989,7 +11989,7 @@
         <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>273.65</v>
+        <v>264.145</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -12012,7 +12012,7 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>0.0088</t>
+          <t>0.009</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
@@ -12070,7 +12070,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -12083,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>131.66</v>
+        <v>126.715</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -12106,7 +12106,7 @@
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>0.0322</t>
+          <t>0.0327</t>
         </is>
       </c>
       <c r="N126" t="inlineStr">
@@ -12115,7 +12115,7 @@
         </is>
       </c>
       <c r="O126" t="n">
-        <v>129</v>
+        <v>126.25</v>
       </c>
       <c r="P126" t="n">
         <v>163.07</v>
@@ -12127,7 +12127,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.52, 'revenueAverage': 1940630000, 'revenueLow': 1913390000, 'revenueHigh': 1959000000}</t>
+          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.52, 'revenueAverage': 1942970000, 'revenueLow': 1913390000, 'revenueHigh': 1978880000}</t>
         </is>
       </c>
       <c r="S126" t="inlineStr">
@@ -12177,7 +12177,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>40.56</v>
+        <v>40.66</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -12200,7 +12200,7 @@
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>0.0801</t>
+          <t>0.0794</t>
         </is>
       </c>
       <c r="N127" t="inlineStr">
@@ -12212,7 +12212,7 @@
         <v>19.06</v>
       </c>
       <c r="P127" t="n">
-        <v>47.89</v>
+        <v>47.32</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
@@ -12271,7 +12271,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>8.9</v>
+        <v>8.942600000000001</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -12349,7 +12349,7 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>389.36</v>
+        <v>392.52</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -12393,7 +12393,7 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 3.07, 'earningsLow': 2.97, 'earningsHigh': 3.22, 'revenueAverage': 3033260000, 'revenueLow': 2956390000, 'revenueHigh': 3099880000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 3.06, 'earningsLow': 2.97, 'earningsHigh': 3.22, 'revenueAverage': 3031600000, 'revenueLow': 2956390000, 'revenueHigh': 3099880000}</t>
         </is>
       </c>
       <c r="S129" t="inlineStr">
@@ -12443,7 +12443,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>90.95</v>
+        <v>87.05</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -12466,7 +12466,7 @@
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>0.0356</t>
+          <t>0.037100002</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
@@ -12524,7 +12524,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -12537,7 +12537,7 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>70.17</v>
+        <v>71.44</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -12631,7 +12631,7 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>122.67</v>
+        <v>124.27</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -12654,7 +12654,7 @@
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>0.0354</t>
+          <t>0.0353</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
@@ -12712,7 +12712,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -12725,7 +12725,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>11.16</v>
+        <v>10.9137</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -12748,7 +12748,7 @@
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>0.1435</t>
+          <t>0.1418</t>
         </is>
       </c>
       <c r="N133" t="inlineStr">
@@ -12806,7 +12806,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -12819,7 +12819,7 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>14.33</v>
+        <v>14.78</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -12837,12 +12837,12 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>2023-06-29</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>0.1438</t>
+          <t>0.1466</t>
         </is>
       </c>
       <c r="N134" t="inlineStr"/>
@@ -12896,7 +12896,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -12909,7 +12909,7 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>110.1</v>
+        <v>109.88</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -12953,7 +12953,7 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 1.83, 'earningsLow': 1.72, 'earningsHigh': 2.06, 'revenueAverage': 1636440000, 'revenueLow': 1577100000, 'revenueHigh': 1683400000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 1.83, 'earningsLow': 1.72, 'earningsHigh': 2.02, 'revenueAverage': 1636440000, 'revenueLow': 1577100000, 'revenueHigh': 1683400000}</t>
         </is>
       </c>
       <c r="S135" t="inlineStr">
@@ -13003,7 +13003,7 @@
         <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>7.72</v>
+        <v>7.61</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -13038,7 +13038,7 @@
         <v>5.14</v>
       </c>
       <c r="P136" t="n">
-        <v>9.255000000000001</v>
+        <v>9.228999999999999</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
@@ -13097,10 +13097,10 @@
         <v>281.915</v>
       </c>
       <c r="G137" t="n">
-        <v>273.58</v>
+        <v>272.721</v>
       </c>
       <c r="H137" t="n">
-        <v>273.58</v>
+        <v>272.721</v>
       </c>
       <c r="I137" t="n">
         <v>103.85</v>
@@ -13125,7 +13125,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.8, 'earningsLow': 0.65, 'earningsHigh': 1.02, 'revenueAverage': 24666900000, 'revenueLow': 20270000000, 'revenueHigh': 27284000000}</t>
+          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.75, 'earningsLow': 0.61, 'earningsHigh': 0.95, 'revenueAverage': 23174400000, 'revenueLow': 21622400000, 'revenueHigh': 25417800000}</t>
         </is>
       </c>
       <c r="S137" t="inlineStr">
@@ -13175,7 +13175,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>13.57</v>
+        <v>13.89</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -13210,7 +13210,7 @@
         <v>11.57</v>
       </c>
       <c r="P138" t="n">
-        <v>19.88</v>
+        <v>19.4</v>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
@@ -13256,7 +13256,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -13269,7 +13269,7 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>21.43</v>
+        <v>22.215</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -13292,7 +13292,7 @@
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>0.087299995</t>
+          <t>0.0877</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
@@ -13313,7 +13313,7 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-11', '2023-10-16'], 'earningsAverage': 0.69, 'earningsLow': 0.68, 'earningsHigh': 0.72, 'revenueAverage': 34741200000, 'revenueLow': 33935000000, 'revenueHigh': 35764700000}</t>
+          <t>{'earningsDate': ['2023-10-12'], 'earningsAverage': 0.65, 'earningsLow': 0.63, 'earningsHigh': 0.67, 'revenueAverage': 32364900000, 'revenueLow': 31613800000, 'revenueHigh': 33318400000}</t>
         </is>
       </c>
       <c r="S139" t="inlineStr">
@@ -13363,7 +13363,7 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>10.52</v>
+        <v>10.5078</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -13386,7 +13386,7 @@
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>0.1331</t>
+          <t>0.1344</t>
         </is>
       </c>
       <c r="N140" t="inlineStr">
@@ -13398,7 +13398,7 @@
         <v>7</v>
       </c>
       <c r="P140" t="n">
-        <v>14.12</v>
+        <v>13.67</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
@@ -13457,7 +13457,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>164.34</v>
+        <v>165.02</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -13492,7 +13492,7 @@
         <v>128.07</v>
       </c>
       <c r="P141" t="n">
-        <v>164.4806</v>
+        <v>165.85</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
@@ -13551,7 +13551,7 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>397.15</v>
+        <v>397.655</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -13632,7 +13632,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -13645,7 +13645,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>114.16</v>
+        <v>118.31</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -13668,7 +13668,7 @@
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>0.0319</t>
+          <t>0.0313</t>
         </is>
       </c>
       <c r="N143" t="inlineStr">
@@ -13689,7 +13689,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.19, 'earningsLow': 1.95, 'earningsHigh': 2.61, 'revenueAverage': 81288900000, 'revenueLow': 59508300000, 'revenueHigh': 92642000000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.05, 'earningsLow': 1.82, 'earningsHigh': 2.43, 'revenueAverage': 75728700000, 'revenueLow': 55437900000, 'revenueHigh': 86305300000}</t>
         </is>
       </c>
       <c r="S143" t="inlineStr">
@@ -13726,7 +13726,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -13739,7 +13739,7 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>11.43</v>
+        <v>11.1982</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -13763,10 +13763,10 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="n">
-        <v>11.16</v>
+        <v>11.15</v>
       </c>
       <c r="P144" t="n">
-        <v>34.14</v>
+        <v>29.98</v>
       </c>
       <c r="Q144" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
feat: trend and holders analysis
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>153.23</v>
+        <v>149.06</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -594,7 +594,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.0383</t>
+          <t>0.038900003</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.87, 'earningsLow': 2.78, 'earningsHigh': 2.95, 'revenueAverage': 13635700000, 'revenueLow': 13145000000, 'revenueHigh': 13811000000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.87, 'earningsLow': 2.78, 'earningsHigh': 2.97, 'revenueAverage': 13637900000, 'revenueLow': 13145000000, 'revenueHigh': 13811000000}</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>96.11</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -688,12 +688,12 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.0212</t>
+          <t>0.0211</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1.54</t>
+          <t>1.55</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -709,7 +709,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 1.03, 'earningsLow': 1.0, 'earningsHigh': 1.04, 'revenueAverage': 9261620000, 'revenueLow': 9151550000, 'revenueHigh': 9545260000}</t>
+          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.09, 'earningsLow': 1.06, 'earningsHigh': 1.1, 'revenueAverage': 9809580000, 'revenueLow': 9693000000, 'revenueHigh': 10110000000}</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>6.805</v>
+        <v>6.8</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -782,7 +782,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.1765</t>
+          <t>0.1762</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -840,7 +840,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>9.74</v>
+        <v>9.52</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -876,7 +876,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.1377</t>
+          <t>0.1375</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>76.28</v>
+        <v>75.42</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -970,7 +970,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.0228</t>
+          <t>0.023599999</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.55, 'earningsLow': 1.4, 'earningsHigh': 1.71, 'revenueAverage': 24168200000, 'revenueLow': 22968000000, 'revenueHigh': 25287600000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.54, 'earningsLow': 1.4, 'earningsHigh': 1.71, 'revenueAverage': 24168200000, 'revenueLow': 22968000000, 'revenueHigh': 25287600000}</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>241.3532</v>
+        <v>240.58</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.0211</t>
+          <t>0.020499999</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 2.02, 'earningsLow': 1.97, 'earningsHigh': 2.12, 'revenueAverage': 4512160000, 'revenueLow': 4456000000, 'revenueHigh': 4554000000}</t>
+          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.02, 'earningsLow': 1.97, 'earningsHigh': 2.12, 'revenueAverage': 4512160000, 'revenueLow': 4456000000, 'revenueHigh': 4554000000}</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>12.385</v>
+        <v>11.74</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.15359999</t>
+          <t>0.1649</t>
         </is>
       </c>
       <c r="N8" t="inlineStr"/>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>76.31999999999999</v>
+        <v>76.75</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.0221</t>
+          <t>0.0216</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>56.04</v>
+        <v>56.12</v>
       </c>
       <c r="P9" t="n">
         <v>78.43000000000001</v>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>12.41</v>
+        <v>12.51</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.1329</t>
+          <t>0.136</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1413,13 +1413,13 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.414999999999999</v>
+        <v>9.44</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>9.19</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -1436,12 +1436,12 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.1524</t>
+          <t>0.1526</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>12.09</t>
+          <t>12.15</t>
         </is>
       </c>
       <c r="O11" t="n">
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6.318</v>
+        <v>6.44</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.1233</t>
+          <t>0.123100005</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1601,13 +1601,13 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>162.84</v>
+        <v>170.04</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>172.91</v>
+        <v>162.63</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.0098</t>
+          <t>0.0093</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1695,13 +1695,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9</v>
+        <v>9.16</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>9.15</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1718,12 +1718,12 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.0538</t>
+          <t>0.0535</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>9</v>
+        <v>8.94</v>
       </c>
       <c r="P14" t="n">
         <v>12.78</v>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>8.800000000000001</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1808,12 +1808,12 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.35909998</t>
+          <t>0.35029998</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>7.84</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="O15" t="n">
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>124.28</v>
+        <v>127.12</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.55, 'earningsLow': 0.42, 'earningsHigh': 0.67, 'revenueAverage': 133599000000, 'revenueLow': 130291000000, 'revenueHigh': 135194000000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 0.58, 'earningsLow': 0.44, 'earningsHigh': 0.71, 'revenueAverage': 141503000000, 'revenueLow': 138000000000, 'revenueHigh': 143193000000}</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>8.550000000000001</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.1427</t>
+          <t>0.1513</t>
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
@@ -1988,7 +1988,7 @@
         <v>4.43</v>
       </c>
       <c r="P17" t="n">
-        <v>13.18</v>
+        <v>12.47</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>65.95999999999999</v>
+        <v>66.13</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2070,12 +2070,12 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0.0183</t>
+          <t>0.018099999</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>1.77</t>
+          <t>1.78</t>
         </is>
       </c>
       <c r="O18" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -2141,13 +2141,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>286.37</v>
+        <v>283.4</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>229.32</v>
+        <v>266.94</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0.024400001</t>
+          <t>0.024500001</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>10.42</v>
+        <v>10.13</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2258,12 +2258,12 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0.1349</t>
+          <t>0.1382</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>12.19</t>
+          <t>12.25</t>
         </is>
       </c>
       <c r="O20" t="n">
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>21.75</v>
+        <v>22.53</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>0.1299</t>
+          <t>0.122</t>
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -2419,13 +2419,13 @@
         <v>2103.093</v>
       </c>
       <c r="G22" t="n">
-        <v>4.2917</v>
+        <v>4.25</v>
       </c>
       <c r="H22" t="n">
-        <v>2047.1409</v>
+        <v>2027.25</v>
       </c>
       <c r="I22" t="n">
-        <v>4.59</v>
+        <v>4.21</v>
       </c>
       <c r="J22" t="n">
         <v>4.85</v>
@@ -2442,16 +2442,16 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>1.0667</t>
+          <t>1.1401</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>15.27</t>
+          <t>15.52</t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>4.28</v>
+        <v>4.13</v>
       </c>
       <c r="P22" t="n">
         <v>6.68</v>
@@ -2513,13 +2513,13 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>107.07</v>
+        <v>105.93</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>106.52</v>
+        <v>105.91</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>0.026500002</t>
+          <t>0.0279</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>10.45</v>
+        <v>10.88</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2630,12 +2630,12 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0.18040001</t>
+          <t>0.1876</t>
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>4.5</v>
+        <v>5.12</v>
       </c>
       <c r="P24" t="n">
         <v>11.75</v>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>8.741300000000001</v>
+        <v>8.91</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0.118999995</t>
+          <t>0.1167</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>4.335</v>
+        <v>4.54</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.1379</t>
+          <t>0.1364</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>258.89</v>
+        <v>258.53</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>24.31</v>
+        <v>24.58</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.0481</t>
+          <t>0.049099997</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -3060,7 +3060,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -3073,13 +3073,13 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>4.61</v>
+        <v>5.11</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>4.87</v>
+        <v>4.52</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>4.54</v>
+        <v>4.39</v>
       </c>
       <c r="P29" t="n">
         <v>20.91</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>70.67</v>
+        <v>69.84</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>0.0064</t>
+          <t>0.0064999997</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.445</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>0.1456</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>5.66</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="O31" t="n">
@@ -3351,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>87.77</v>
+        <v>86.81999999999999</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0.0224</t>
+          <t>0.0227</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>209.84</v>
+        <v>208.18</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3477,7 +3477,7 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>177.48</v>
+        <v>181.23</v>
       </c>
       <c r="P33" t="n">
         <v>231.37</v>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-07-26'], 'earningsAverage': 4.24, 'earningsLow': 3.56, 'earningsHigh': 5.05, 'revenueAverage': 11619800000, 'revenueLow': 11421000000, 'revenueHigh': 11752000000}</t>
+          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': 4.24, 'earningsLow': 3.56, 'earningsHigh': 5.05, 'revenueAverage': 11619800000, 'revenueLow': 11421000000, 'revenueHigh': 11752000000}</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3539,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>92.535</v>
+        <v>91.63</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3562,7 +3562,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>0.0116</t>
+          <t>0.0119</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.68, 'earningsLow': 0.66, 'earningsHigh': 0.79, 'revenueAverage': 1428230000, 'revenueLow': 1420870000, 'revenueHigh': 1445800000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.68, 'earningsLow': 0.66, 'earningsHigh': 0.75, 'revenueAverage': 1428230000, 'revenueLow': 1420870000, 'revenueHigh': 1445800000}</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -3633,13 +3633,13 @@
         <v>1446.798</v>
       </c>
       <c r="G35" t="n">
-        <v>3.955</v>
+        <v>3.72</v>
       </c>
       <c r="H35" t="n">
-        <v>1447.53</v>
+        <v>1361.52</v>
       </c>
       <c r="I35" t="n">
-        <v>3.74</v>
+        <v>3.72</v>
       </c>
       <c r="J35" t="n">
         <v>4.35</v>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>0.1489</t>
+          <t>0.1604</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -3665,7 +3665,7 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>3.7</v>
+        <v>3.65</v>
       </c>
       <c r="P35" t="n">
         <v>7.24</v>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -3727,13 +3727,13 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>85.22</v>
+        <v>86.13</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>86.19</v>
+        <v>84.95</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>0.0287</t>
+          <t>0.027999999</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.86, 'earningsLow': 0.68, 'earningsHigh': 0.99, 'revenueAverage': 4384500000, 'revenueLow': 4165100000, 'revenueHigh': 4557000000}</t>
+          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.86, 'earningsLow': 0.68, 'earningsHigh': 0.99, 'revenueAverage': 4384560000, 'revenueLow': 4165100000, 'revenueHigh': 4557000000}</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.705</v>
+        <v>5.46</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3844,12 +3844,12 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>0.1254</t>
+          <t>0.13430001</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>13.56</t>
         </is>
       </c>
       <c r="O37" t="n">
@@ -3915,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>104.66</v>
+        <v>102.29</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>0.028099999</t>
+          <t>0.028499998</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -3947,7 +3947,7 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>89.36</v>
+        <v>89.62</v>
       </c>
       <c r="P38" t="n">
         <v>130.66</v>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -4009,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>10.48</v>
+        <v>10.57</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2023-09-28</t>
+          <t>2023-12-28</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>0.0735</t>
+          <t>0.0744</t>
         </is>
       </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>8.08</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="P39" t="n">
         <v>11.75</v>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>71.375</v>
+        <v>71.11</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -4118,12 +4118,12 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>0.026600001</t>
+          <t>0.027</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>2.38</t>
+          <t>2.39</t>
         </is>
       </c>
       <c r="O40" t="n">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.76, 'earningsLow': 0.74, 'earningsHigh': 0.78, 'revenueAverage': 4545050000, 'revenueLow': 4456340000, 'revenueHigh': 4729760000}</t>
+          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.8, 'earningsLow': 0.78, 'earningsHigh': 0.83, 'revenueAverage': 4813960000, 'revenueLow': 4720000000, 'revenueHigh': 5009600000}</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4189,13 +4189,13 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>129.82</v>
+        <v>131.06</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>136.46</v>
+        <v>128.62</v>
       </c>
       <c r="J41" t="n">
         <v>0</v>
@@ -4212,12 +4212,12 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>0.036</t>
+          <t>0.0363</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>2.65</t>
+          <t>2.67</t>
         </is>
       </c>
       <c r="O41" t="n">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.37, 'earningsLow': 1.21, 'earningsHigh': 1.49, 'revenueAverage': 1802690000, 'revenueLow': 1747150000, 'revenueHigh': 1840000000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.36, 'earningsLow': 1.21, 'earningsHigh': 1.49, 'revenueAverage': 1802690000, 'revenueLow': 1747150000, 'revenueHigh': 1840000000}</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>11</v>
+        <v>11.08</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>0.089499995</t>
+          <t>0.090299994</t>
         </is>
       </c>
       <c r="N42" t="inlineStr"/>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>7.715</v>
+        <v>7.99</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -4392,12 +4392,12 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>0.18280001</t>
+          <t>0.1762</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>20.69</t>
+          <t>20.68</t>
         </is>
       </c>
       <c r="O43" t="n">
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>477.51</v>
+        <v>481.01</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.0113</t>
+          <t>0.0112</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4500,10 +4500,14 @@
       <c r="P44" t="n">
         <v>524.76</v>
       </c>
-      <c r="Q44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>1.301867</t>
+        </is>
+      </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-12-19', '2023-12-26'], 'earningsAverage': 3.49, 'earningsLow': 3.41, 'earningsHigh': 3.69, 'revenueAverage': 2339710000, 'revenueLow': 2325990000, 'revenueHigh': 2399290000}</t>
+          <t>{'earningsDate': ['2023-12-19', '2023-12-26'], 'earningsAverage': 3.49, 'earningsLow': 3.42, 'earningsHigh': 3.69, 'revenueAverage': 2340160000, 'revenueLow': 2328600000, 'revenueHigh': 2357410000}</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -4553,13 +4557,13 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>3.3553</v>
+        <v>3.34</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>3.47</v>
+        <v>3.31</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
@@ -4576,12 +4580,12 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>0.206</t>
+          <t>0.2079</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>15.11</t>
+          <t>15.42</t>
         </is>
       </c>
       <c r="O45" t="n">
@@ -4647,7 +4651,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>170.195</v>
+        <v>168.62</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4679,7 +4683,7 @@
         </is>
       </c>
       <c r="O46" t="n">
-        <v>141.4</v>
+        <v>148.3</v>
       </c>
       <c r="P46" t="n">
         <v>189.68</v>
@@ -4691,7 +4695,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 3.11, 'earningsLow': 2.58, 'earningsHigh': 3.8, 'revenueAverage': 44777700000, 'revenueLow': 34652800000, 'revenueHigh': 53627100000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 3.33, 'earningsLow': 2.74, 'earningsHigh': 4.02, 'revenueAverage': 49265100000, 'revenueLow': 36703000000, 'revenueHigh': 62131400000}</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4728,7 +4732,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -4741,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>140.39</v>
+        <v>139.51</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4769,7 +4773,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>1.66</t>
+          <t>1.65</t>
         </is>
       </c>
       <c r="O47" t="n">
@@ -4785,7 +4789,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 2.33, 'earningsLow': 2.25, 'earningsHigh': 2.43, 'revenueAverage': 2229310000, 'revenueLow': 2147000000, 'revenueHigh': 2289360000}</t>
+          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 2.33, 'earningsLow': 2.25, 'earningsHigh': 2.43, 'revenueAverage': 2230930000, 'revenueLow': 2147000000, 'revenueHigh': 2289360000}</t>
         </is>
       </c>
       <c r="S47" t="inlineStr">
@@ -4835,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.5</v>
+        <v>3.47</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4858,7 +4862,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>0.18010001</t>
+          <t>0.17909999</t>
         </is>
       </c>
       <c r="N48" t="inlineStr"/>
@@ -4868,7 +4872,11 @@
       <c r="P48" t="n">
         <v>4.85</v>
       </c>
-      <c r="Q48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>1.155601</t>
+        </is>
+      </c>
       <c r="R48" t="inlineStr">
         <is>
           <t>{'earningsDate': ['2023-11-15', '2023-11-20'], 'earningsAverage': 0.06, 'earningsLow': 0.05, 'earningsHigh': 0.07, 'revenueAverage': 62270000, 'revenueLow': 59000000, 'revenueHigh': 64570000}</t>
@@ -4921,13 +4929,13 @@
         <v>647</v>
       </c>
       <c r="G49" t="n">
-        <v>6.3499</v>
+        <v>6.21</v>
       </c>
       <c r="H49" t="n">
-        <v>634.99</v>
+        <v>621</v>
       </c>
       <c r="I49" t="n">
-        <v>6.24</v>
+        <v>6.2</v>
       </c>
       <c r="J49" t="n">
         <v>7.12</v>
@@ -4944,12 +4952,12 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>0.1529</t>
+          <t>0.1546</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>12.4</t>
+          <t>12.44</t>
         </is>
       </c>
       <c r="O49" t="n">
@@ -5002,7 +5010,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -5015,13 +5023,13 @@
         <v>153.75</v>
       </c>
       <c r="G50" t="n">
+        <v>10.15</v>
+      </c>
+      <c r="H50" t="n">
+        <v>152.25</v>
+      </c>
+      <c r="I50" t="n">
         <v>9.98</v>
-      </c>
-      <c r="H50" t="n">
-        <v>149.7</v>
-      </c>
-      <c r="I50" t="n">
-        <v>10.1</v>
       </c>
       <c r="J50" t="n">
         <v>11.28</v>
@@ -5038,7 +5046,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>0.1683</t>
+          <t>0.1657</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -5109,7 +5117,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>168.58</v>
+        <v>169.4</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -5132,7 +5140,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>0.0123000005</t>
+          <t>0.0125</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -5203,13 +5211,13 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>87.39</v>
+        <v>85.53</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>86.51000000000001</v>
+        <v>85.48999999999999</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
@@ -5226,7 +5234,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.0359</t>
+          <t>0.0369</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -5297,13 +5305,13 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>12.54</v>
+        <v>12.47</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>12.4</v>
+        <v>12.3</v>
       </c>
       <c r="J53" t="n">
         <v>13.34</v>
@@ -5320,12 +5328,12 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>0.1442</t>
+          <t>0.1443</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>11.17</t>
+          <t>11.24</t>
         </is>
       </c>
       <c r="O53" t="n">
@@ -5391,13 +5399,13 @@
         <v>42</v>
       </c>
       <c r="G54" t="n">
-        <v>42</v>
+        <v>42.03</v>
       </c>
       <c r="H54" t="n">
-        <v>42</v>
+        <v>42.03</v>
       </c>
       <c r="I54" t="n">
-        <v>39.28</v>
+        <v>39.27</v>
       </c>
       <c r="J54" t="n">
         <v>46.2</v>
@@ -5414,7 +5422,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>0.077199996</t>
+          <t>0.0733</t>
         </is>
       </c>
       <c r="N54" t="inlineStr"/>
@@ -5431,7 +5439,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': -0.46, 'earningsLow': -1.12, 'earningsHigh': 0.11, 'revenueAverage': 80600000, 'revenueLow': 48700000, 'revenueHigh': 95580000}</t>
+          <t>{'earningsDate': ['2023-11-02'], 'earningsAverage': -0.46, 'earningsLow': -1.12, 'earningsHigh': 0.11, 'revenueAverage': 80600000, 'revenueLow': 48700000, 'revenueHigh': 95580000}</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
@@ -5481,7 +5489,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>96.39</v>
+        <v>96.56999999999999</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -5504,7 +5512,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>0.0212</t>
+          <t>0.0218</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -5513,7 +5521,7 @@
         </is>
       </c>
       <c r="O55" t="n">
-        <v>73.03</v>
+        <v>73.94</v>
       </c>
       <c r="P55" t="n">
         <v>100.62</v>
@@ -5525,7 +5533,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.3, 'earningsLow': 1.27, 'earningsHigh': 1.4, 'revenueAverage': 4196380000, 'revenueLow': 4078000000, 'revenueHigh': 4275900000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.3, 'earningsLow': 1.27, 'earningsHigh': 1.4, 'revenueAverage': 4196370000, 'revenueLow': 4078000000, 'revenueHigh': 4275800000}</t>
         </is>
       </c>
       <c r="S55" t="inlineStr">
@@ -5562,7 +5570,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -5575,7 +5583,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>212.9</v>
+        <v>212.09</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -5598,7 +5606,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>0.0427</t>
+          <t>0.0438</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -5669,7 +5677,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>113.3</v>
+        <v>114.63</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5763,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>6.05</v>
+        <v>5.98</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5786,12 +5794,12 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>0.13949999</t>
+          <t>0.14050001</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>12.43</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="O58" t="n">
@@ -5857,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>18.495</v>
+        <v>18.78</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5880,7 +5888,7 @@
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0.138</t>
         </is>
       </c>
       <c r="N59" t="inlineStr"/>
@@ -5947,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>90.935</v>
+        <v>90.63</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -6041,7 +6049,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>19.865</v>
+        <v>19.69</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -6064,7 +6072,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>0.1421</t>
+          <t>0.1407</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -6073,7 +6081,7 @@
         </is>
       </c>
       <c r="O61" t="n">
-        <v>16.7</v>
+        <v>16.74</v>
       </c>
       <c r="P61" t="n">
         <v>20.8</v>
@@ -6135,7 +6143,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>220.3</v>
+        <v>220.97</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -6158,12 +6166,12 @@
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>0.0242</t>
+          <t>0.0239</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>2.36</t>
+          <t>2.37</t>
         </is>
       </c>
       <c r="O62" t="n">
@@ -6179,7 +6187,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 2.75, 'earningsLow': 2.66, 'earningsHigh': 2.97, 'revenueAverage': 9480200000, 'revenueLow': 9120390000, 'revenueHigh': 9989950000}</t>
+          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 2.91, 'earningsLow': 2.82, 'earningsHigh': 3.15, 'revenueAverage': 10035900000, 'revenueLow': 9660000000, 'revenueHigh': 10581000000}</t>
         </is>
       </c>
       <c r="S62" t="inlineStr">
@@ -6229,7 +6237,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>9.84</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -6252,12 +6260,12 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>0.1596</t>
+          <t>0.1523</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>18.74</t>
+          <t>18.83</t>
         </is>
       </c>
       <c r="O63" t="n">
@@ -6323,7 +6331,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>4.86</v>
+        <v>4.77</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -6346,16 +6354,16 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>0.12529999</t>
+          <t>0.1276</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>5.68</t>
+          <t>5.87</t>
         </is>
       </c>
       <c r="O64" t="n">
-        <v>4.085714</v>
+        <v>4.419048</v>
       </c>
       <c r="P64" t="n">
         <v>6.342857</v>
@@ -6367,7 +6375,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.23, 'earningsLow': 0.22, 'earningsHigh': 0.23, 'revenueAverage': 3570280000, 'revenueLow': 3570280000, 'revenueHigh': 3570280000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.22, 'earningsLow': 0.22, 'earningsHigh': 0.23, 'revenueAverage': 3524540000, 'revenueLow': 3524540000, 'revenueHigh': 3524540000}</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6417,7 +6425,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>6.15</v>
+        <v>5.89</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -6440,7 +6448,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>0.1408</t>
+          <t>0.1512</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -6511,10 +6519,10 @@
         <v>70.75</v>
       </c>
       <c r="G66" t="n">
-        <v>14.0091</v>
+        <v>13.99</v>
       </c>
       <c r="H66" t="n">
-        <v>70.0455</v>
+        <v>69.95</v>
       </c>
       <c r="I66" t="n">
         <v>12.41</v>
@@ -6534,12 +6542,12 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>0.1154</t>
+          <t>0.11359999</t>
         </is>
       </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="n">
-        <v>11.92</v>
+        <v>12.39</v>
       </c>
       <c r="P66" t="n">
         <v>19.842</v>
@@ -6588,7 +6596,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -6601,7 +6609,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>9.44</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -6624,7 +6632,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>0.15640001</t>
+          <t>0.1693</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -6695,7 +6703,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>7.905</v>
+        <v>7.88</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -6718,7 +6726,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.097200006</t>
+          <t>0.0949</t>
         </is>
       </c>
       <c r="N68" t="inlineStr"/>
@@ -6785,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>129.26</v>
+        <v>130.86</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -6813,7 +6821,7 @@
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.44, 'earningsLow': 1.27, 'earningsHigh': 1.55, 'revenueAverage': 75906700000, 'revenueLow': 72863000000, 'revenueHigh': 77922700000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.44, 'earningsLow': 1.27, 'earningsHigh': 1.55, 'revenueAverage': 75914400000, 'revenueLow': 72863000000, 'revenueHigh': 77922700000}</t>
         </is>
       </c>
       <c r="S69" t="inlineStr">
@@ -6850,7 +6858,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -6863,13 +6871,13 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>142.805</v>
+        <v>144.38</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
       </c>
       <c r="I70" t="n">
-        <v>147.28</v>
+        <v>142.31</v>
       </c>
       <c r="J70" t="n">
         <v>0</v>
@@ -6886,7 +6894,7 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>0.026600001</t>
+          <t>0.026500002</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
@@ -6895,7 +6903,7 @@
         </is>
       </c>
       <c r="O70" t="n">
-        <v>142.5601</v>
+        <v>141.58</v>
       </c>
       <c r="P70" t="n">
         <v>187.73</v>
@@ -6907,7 +6915,7 @@
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18', '2023-10-23'], 'earningsAverage': 2.41, 'earningsLow': 2.36, 'earningsHigh': 2.51, 'revenueAverage': 5921890000, 'revenueLow': 5834610000, 'revenueHigh': 6096050000}</t>
+          <t>{'earningsDate': ['2023-10-19'], 'earningsAverage': 2.41, 'earningsLow': 2.36, 'earningsHigh': 2.51, 'revenueAverage': 5921890000, 'revenueLow': 5834610000, 'revenueHigh': 6096050000}</t>
         </is>
       </c>
       <c r="S70" t="inlineStr">
@@ -6944,7 +6952,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -6957,7 +6965,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>4.96</v>
+        <v>4.88</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -7051,7 +7059,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>9.449999999999999</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -7074,7 +7082,7 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>0.1459</t>
+          <t>0.1445</t>
         </is>
       </c>
       <c r="N72" t="inlineStr"/>
@@ -7141,7 +7149,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>694.385</v>
+        <v>691.84</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -7164,16 +7172,16 @@
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>0.0109</t>
+          <t>0.0108</t>
         </is>
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>1.53</t>
+          <t>1.52</t>
         </is>
       </c>
       <c r="O73" t="n">
-        <v>483.59</v>
+        <v>488.24</v>
       </c>
       <c r="P73" t="n">
         <v>811.6</v>
@@ -7235,7 +7243,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>6.7</v>
+        <v>6.65</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -7275,7 +7283,7 @@
       </c>
       <c r="R74" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': -0.36, 'earningsLow': -0.4, 'earningsHigh': -0.33, 'revenueAverage': 236200000, 'revenueLow': 232920000, 'revenueHigh': 239640000}</t>
+          <t>{'earningsDate': ['2023-11-01'], 'earningsAverage': -0.38, 'earningsLow': -0.43, 'earningsHigh': -0.33, 'revenueAverage': 236200000, 'revenueLow': 232920000, 'revenueHigh': 239640000}</t>
         </is>
       </c>
       <c r="S74" t="inlineStr">
@@ -7312,7 +7320,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -7325,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>38.59</v>
+        <v>38.03</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7348,12 +7356,12 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>0.028299998</t>
+          <t>0.028900001</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>2.07</t>
+          <t>2.08</t>
         </is>
       </c>
       <c r="O75" t="n">
@@ -7419,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>142.795</v>
+        <v>140.3</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -7442,12 +7450,12 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>0.0464</t>
+          <t>0.0473</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>4.94</t>
+          <t>4.95</t>
         </is>
       </c>
       <c r="O76" t="n">
@@ -7463,7 +7471,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.02, 'earningsLow': 1.97, 'earningsHigh': 2.12, 'revenueAverage': 13966200000, 'revenueLow': 13867900000, 'revenueHigh': 14157400000}</t>
+          <t>{'earningsDate': ['2023-10-25'], 'earningsAverage': 2.14, 'earningsLow': 2.09, 'earningsHigh': 2.25, 'revenueAverage': 14792500000, 'revenueLow': 14688400000, 'revenueHigh': 14995000000}</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -7513,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>3.82</v>
+        <v>3.99</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -7536,12 +7544,12 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>0.1391</t>
+          <t>0.1328</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>15.34</t>
+          <t>15.38</t>
         </is>
       </c>
       <c r="O77" t="n">
@@ -7607,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>19.885</v>
+        <v>19.78</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -7630,12 +7638,12 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>0.201</t>
+          <t>0.199</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>15.43</t>
         </is>
       </c>
       <c r="O78" t="n">
@@ -7688,7 +7696,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -7701,13 +7709,13 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>231.6</v>
+        <v>230.31</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>180.65</v>
+        <v>218.73</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
@@ -7724,7 +7732,7 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>0.024300002</t>
+          <t>0.0241</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
@@ -7733,7 +7741,7 @@
         </is>
       </c>
       <c r="O79" t="n">
-        <v>180.27</v>
+        <v>180.46</v>
       </c>
       <c r="P79" t="n">
         <v>264.19</v>
@@ -7745,7 +7753,7 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.46, 'earningsLow': 2.42, 'earningsHigh': 2.5, 'revenueAverage': 4111250000, 'revenueLow': 4031000000, 'revenueHigh': 4164000000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.46, 'earningsLow': 2.35, 'earningsHigh': 2.5, 'revenueAverage': 4103950000, 'revenueLow': 4017000000, 'revenueHigh': 4164000000}</t>
         </is>
       </c>
       <c r="S79" t="inlineStr">
@@ -7795,7 +7803,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>9.904999999999999</v>
+        <v>10.01</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -7813,12 +7821,12 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>2023-06-30</t>
+          <t>2023-10-05</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>0.1578</t>
+          <t>0.1619</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
@@ -7889,7 +7897,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>157</v>
+        <v>155.75</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -7912,12 +7920,12 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>0.0297</t>
+          <t>0.0306</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>2.62</t>
+          <t>2.63</t>
         </is>
       </c>
       <c r="O81" t="n">
@@ -7933,7 +7941,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.37, 'earningsLow': 2.27, 'earningsHigh': 2.44, 'revenueAverage': 19863700000, 'revenueLow': 19439900000, 'revenueHigh': 20163100000}</t>
+          <t>{'earningsDate': ['2023-10-17'], 'earningsAverage': 2.51, 'earningsLow': 2.4, 'earningsHigh': 2.58, 'revenueAverage': 21038900000, 'revenueLow': 20590100000, 'revenueHigh': 21356000000}</t>
         </is>
       </c>
       <c r="S81" t="inlineStr">
@@ -7983,13 +7991,13 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.732</v>
+        <v>0.72</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
       </c>
       <c r="I82" t="n">
-        <v>0.79</v>
+        <v>0.704</v>
       </c>
       <c r="J82" t="n">
         <v>0</v>
@@ -8010,7 +8018,7 @@
         <v>0.7</v>
       </c>
       <c r="P82" t="n">
-        <v>7.41</v>
+        <v>7.025</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
@@ -8056,7 +8064,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -8069,13 +8077,13 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>22.52</v>
+        <v>22.7</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
       </c>
       <c r="I83" t="n">
-        <v>23.01</v>
+        <v>22.17</v>
       </c>
       <c r="J83" t="n">
         <v>26.26</v>
@@ -8092,12 +8100,12 @@
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>0.53360003</t>
+          <t>0.55</t>
         </is>
       </c>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="n">
-        <v>22.6</v>
+        <v>22.05</v>
       </c>
       <c r="P83" t="n">
         <v>41.06</v>
@@ -8159,13 +8167,13 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>122.54</v>
+        <v>120.85</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
       </c>
       <c r="I84" t="n">
-        <v>122.34</v>
+        <v>120.85</v>
       </c>
       <c r="J84" t="n">
         <v>0</v>
@@ -8182,12 +8190,12 @@
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>0.0382</t>
+          <t>0.039100002</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>3.29</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="O84" t="n">
@@ -8253,13 +8261,13 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>56.085</v>
+        <v>55.98</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
       </c>
       <c r="I85" t="n">
-        <v>57.94</v>
+        <v>55.81</v>
       </c>
       <c r="J85" t="n">
         <v>0</v>
@@ -8276,7 +8284,7 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>0.0325</t>
+          <t>0.032899998</t>
         </is>
       </c>
       <c r="N85" t="inlineStr">
@@ -8297,7 +8305,7 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': 0.66, 'earningsLow': 0.64, 'earningsHigh': 0.68, 'revenueAverage': 10824800000, 'revenueLow': 10683300000, 'revenueHigh': 11082300000}</t>
+          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': 0.7, 'earningsLow': 0.68, 'earningsHigh': 0.72, 'revenueAverage': 11465300000, 'revenueLow': 11315400000, 'revenueHigh': 11738000000}</t>
         </is>
       </c>
       <c r="S85" t="inlineStr">
@@ -8334,7 +8342,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -8347,7 +8355,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>12.2301</v>
+        <v>11.87</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -8370,7 +8378,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>0.1388</t>
+          <t>0.1423</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -8428,7 +8436,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -8441,13 +8449,13 @@
         <v>569.3099999999999</v>
       </c>
       <c r="G87" t="n">
-        <v>24.7</v>
+        <v>25.41</v>
       </c>
       <c r="H87" t="n">
-        <v>518.6999999999999</v>
+        <v>533.61</v>
       </c>
       <c r="I87" t="n">
-        <v>24.95</v>
+        <v>24.58</v>
       </c>
       <c r="J87" t="n">
         <v>29.82</v>
@@ -8464,7 +8472,7 @@
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>0.0732</t>
+          <t>0.071</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
@@ -8535,7 +8543,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>373.43</v>
+        <v>372.35</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -8563,11 +8571,11 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>1.58</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="O88" t="n">
-        <v>264.95</v>
+        <v>266.22</v>
       </c>
       <c r="P88" t="n">
         <v>393.67</v>
@@ -8629,7 +8637,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>5.46</v>
+        <v>5.68</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -8652,12 +8660,12 @@
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>0.18010001</t>
+          <t>0.17819999</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>8.18</t>
+          <t>8.32</t>
         </is>
       </c>
       <c r="O89" t="n">
@@ -8723,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>5.92</v>
+        <v>6.03</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -8746,7 +8754,7 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>0.136</t>
+          <t>0.1329</t>
         </is>
       </c>
       <c r="N90" t="inlineStr"/>
@@ -8813,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>209.0125</v>
+        <v>207.84</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -8836,12 +8844,12 @@
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>0.0211</t>
+          <t>0.0212</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>1.66</t>
+          <t>1.67</t>
         </is>
       </c>
       <c r="O91" t="n">
@@ -8857,7 +8865,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-21'], 'earningsAverage': 3.12, 'earningsLow': 2.89, 'earningsHigh': 3.27, 'revenueAverage': 21164600000, 'revenueLow': 20810000000, 'revenueHigh': 21999200000}</t>
+          <t>{'earningsDate': ['2023-11-21'], 'earningsAverage': 3.12, 'earningsLow': 2.89, 'earningsHigh': 3.27, 'revenueAverage': 21144200000, 'revenueLow': 20554000000, 'revenueHigh': 21999200000}</t>
         </is>
       </c>
       <c r="S91" t="inlineStr">
@@ -8894,7 +8902,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -8907,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1.09</v>
+        <v>1.06</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -8930,7 +8938,7 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>0.078099996</t>
+          <t>0.0809</t>
         </is>
       </c>
       <c r="N92" t="inlineStr"/>
@@ -8947,7 +8955,7 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-21', '2023-11-27'], 'earningsAverage': 0.03, 'earningsLow': 0.02, 'earningsHigh': 0.03, 'revenueAverage': 1209210000, 'revenueLow': 1146520000, 'revenueHigh': 1271900000}</t>
+          <t>{'earningsDate': ['2023-11-21', '2023-11-27'], 'earningsAverage': 0.04, 'earningsLow': 0.02, 'earningsHigh': 0.05, 'revenueAverage': 1204310000, 'revenueLow': 1141870000, 'revenueHigh': 1266750000}</t>
         </is>
       </c>
       <c r="S92" t="inlineStr">
@@ -8997,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>264.86</v>
+        <v>263.44</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -9020,16 +9028,16 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>0.0227</t>
+          <t>0.0231</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>2.24</t>
         </is>
       </c>
       <c r="O93" t="n">
-        <v>230.58</v>
+        <v>231.71</v>
       </c>
       <c r="P93" t="n">
         <v>299.35</v>
@@ -9041,7 +9049,7 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30'], 'earningsAverage': 2.83, 'earningsLow': 2.68, 'earningsHigh': 3.09, 'revenueAverage': 6194670000, 'revenueLow': 5994630000, 'revenueHigh': 6374360000}</t>
+          <t>{'earningsDate': ['2023-10-30'], 'earningsAverage': 2.99, 'earningsLow': 2.84, 'earningsHigh': 3.27, 'revenueAverage': 6561180000, 'revenueLow': 6349300000, 'revenueHigh': 6751500000}</t>
         </is>
       </c>
       <c r="S93" t="inlineStr">
@@ -9091,13 +9099,13 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>78.17829999999999</v>
+        <v>78.36</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
       </c>
       <c r="I94" t="n">
-        <v>76.13</v>
+        <v>76.3</v>
       </c>
       <c r="J94" t="n">
         <v>0</v>
@@ -9114,12 +9122,12 @@
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>0.0344</t>
+          <t>0.0352</t>
         </is>
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>2.35</t>
+          <t>2.38</t>
         </is>
       </c>
       <c r="O94" t="n">
@@ -9172,7 +9180,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -9185,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>9.895</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -9208,7 +9216,7 @@
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>0.139</t>
+          <t>0.1424</t>
         </is>
       </c>
       <c r="N95" t="inlineStr">
@@ -9279,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>74.81999999999999</v>
+        <v>75.64</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -9302,7 +9310,7 @@
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>0.0207</t>
+          <t>0.0211</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
@@ -9373,13 +9381,13 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>93.825</v>
+        <v>93.62</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
       </c>
       <c r="I97" t="n">
-        <v>93.31</v>
+        <v>93.26000000000001</v>
       </c>
       <c r="J97" t="n">
         <v>0</v>
@@ -9396,12 +9404,12 @@
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>0.0633</t>
+          <t>0.0643</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>3.83</t>
+          <t>3.89</t>
         </is>
       </c>
       <c r="O97" t="n">
@@ -9553,7 +9561,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>4.055</v>
+        <v>4.12</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -9576,12 +9584,12 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.1262</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>6.83</t>
         </is>
       </c>
       <c r="O99" t="n">
@@ -9647,7 +9655,7 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>219.89</v>
+        <v>223.17</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -9670,7 +9678,7 @@
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>0.0126</t>
+          <t>0.012200001</t>
         </is>
       </c>
       <c r="N100" t="inlineStr">
@@ -9741,13 +9749,13 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>61.71</v>
+        <v>57.29</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
       </c>
       <c r="I101" t="n">
-        <v>65.69</v>
+        <v>57.08</v>
       </c>
       <c r="J101" t="n">
         <v>0</v>
@@ -9764,7 +9772,7 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>0.0286</t>
+          <t>0.0328</t>
         </is>
       </c>
       <c r="N101" t="inlineStr">
@@ -9773,7 +9781,7 @@
         </is>
       </c>
       <c r="O101" t="n">
-        <v>61.61</v>
+        <v>56.98</v>
       </c>
       <c r="P101" t="n">
         <v>88.61</v>
@@ -9785,7 +9793,7 @@
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.86, 'earningsLow': 0.69, 'earningsHigh': 0.95, 'revenueAverage': 6970810000, 'revenueLow': 5509480000, 'revenueHigh': 7523260000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.86, 'earningsLow': 0.69, 'earningsHigh': 0.95, 'revenueAverage': 6972240000, 'revenueLow': 5509480000, 'revenueHigh': 7523260000}</t>
         </is>
       </c>
       <c r="S101" t="inlineStr">
@@ -9835,7 +9843,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>5.2801</v>
+        <v>5.3</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -9858,7 +9866,7 @@
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>0.14840001</t>
+          <t>0.1509</t>
         </is>
       </c>
       <c r="N102" t="inlineStr">
@@ -9916,7 +9924,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -9929,7 +9937,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>19.4099</v>
+        <v>18.81</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -9952,7 +9960,7 @@
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>0.1318</t>
+          <t>0.1387</t>
         </is>
       </c>
       <c r="N103" t="inlineStr">
@@ -10010,7 +10018,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -10023,7 +10031,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>155.26</v>
+        <v>156.35</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -10046,7 +10054,7 @@
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>0.0134000005</t>
+          <t>0.0128999995</t>
         </is>
       </c>
       <c r="N104" t="inlineStr">
@@ -10055,7 +10063,7 @@
         </is>
       </c>
       <c r="O104" t="n">
-        <v>103.83</v>
+        <v>109.27</v>
       </c>
       <c r="P104" t="n">
         <v>182.68</v>
@@ -10117,13 +10125,13 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>8.4292</v>
+        <v>8.49</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
       </c>
       <c r="I105" t="n">
-        <v>8.69</v>
+        <v>8.34</v>
       </c>
       <c r="J105" t="n">
         <v>0</v>
@@ -10140,7 +10148,7 @@
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>0.1429</t>
+          <t>0.1439</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
@@ -10198,7 +10206,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -10211,13 +10219,13 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>49.9211</v>
+        <v>49.94</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
       </c>
       <c r="I106" t="n">
-        <v>53.73</v>
+        <v>49.62</v>
       </c>
       <c r="J106" t="n">
         <v>0</v>
@@ -10234,7 +10242,7 @@
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>0.061100002</t>
+          <t>0.0619</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -10243,7 +10251,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>49.91</v>
+        <v>49.38</v>
       </c>
       <c r="P106" t="n">
         <v>68.84999999999999</v>
@@ -10255,7 +10263,7 @@
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.32, 'earningsLow': 0.28, 'earningsHigh': 0.36, 'revenueAverage': 1000340000, 'revenueLow': 947430000, 'revenueHigh': 1079210000}</t>
+          <t>{'earningsDate': ['2023-11-06'], 'earningsAverage': 0.32, 'earningsLow': 0.28, 'earningsHigh': 0.36, 'revenueAverage': 1000340000, 'revenueLow': 947430000, 'revenueHigh': 1079210000}</t>
         </is>
       </c>
       <c r="S106" t="inlineStr">
@@ -10292,7 +10300,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D107" t="n">
@@ -10305,13 +10313,13 @@
         <v>3683.5</v>
       </c>
       <c r="G107" t="n">
-        <v>6.9263</v>
+        <v>7.09</v>
       </c>
       <c r="H107" t="n">
-        <v>3463.15</v>
+        <v>3545</v>
       </c>
       <c r="I107" t="n">
-        <v>6.79</v>
+        <v>6.43</v>
       </c>
       <c r="J107" t="n">
         <v>8.1</v>
@@ -10328,7 +10336,7 @@
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>0.3298</t>
+          <t>0.3022</t>
         </is>
       </c>
       <c r="N107" t="inlineStr"/>
@@ -10382,7 +10390,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -10395,13 +10403,13 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>4.44</v>
+        <v>4.1</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
       </c>
       <c r="I108" t="n">
-        <v>5.6</v>
+        <v>4.1</v>
       </c>
       <c r="J108" t="n">
         <v>0</v>
@@ -10418,7 +10426,7 @@
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>0.3441</t>
+          <t>0.3823</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -10427,7 +10435,7 @@
         </is>
       </c>
       <c r="O108" t="n">
-        <v>4.43</v>
+        <v>4.05</v>
       </c>
       <c r="P108" t="n">
         <v>18.1</v>
@@ -10489,13 +10497,13 @@
         <v>2910.507</v>
       </c>
       <c r="G109" t="n">
-        <v>8.7056</v>
+        <v>8.51</v>
       </c>
       <c r="H109" t="n">
-        <v>2794.4976</v>
+        <v>2731.71</v>
       </c>
       <c r="I109" t="n">
-        <v>9.220000000000001</v>
+        <v>8.41</v>
       </c>
       <c r="J109" t="n">
         <v>9.970000000000001</v>
@@ -10512,7 +10520,7 @@
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>0.2212</t>
+          <t>0.2283</t>
         </is>
       </c>
       <c r="N109" t="inlineStr">
@@ -10583,10 +10591,10 @@
         <v>369</v>
       </c>
       <c r="G110" t="n">
-        <v>4.955</v>
+        <v>4.99</v>
       </c>
       <c r="H110" t="n">
-        <v>495.5</v>
+        <v>499</v>
       </c>
       <c r="I110" t="n">
         <v>4.8</v>
@@ -10606,7 +10614,7 @@
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>0.1894</t>
+          <t>0.1864</t>
         </is>
       </c>
       <c r="N110" t="inlineStr">
@@ -10677,7 +10685,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3</v>
+        <v>3.01</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -10700,12 +10708,12 @@
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>0.1443</t>
+          <t>0.14050001</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>14.91</t>
+          <t>14.95</t>
         </is>
       </c>
       <c r="O111" t="n">
@@ -10771,7 +10779,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>14.795</v>
+        <v>14.99</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -10794,7 +10802,7 @@
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>0.2505</t>
+          <t>0.2458</t>
         </is>
       </c>
       <c r="N112" t="inlineStr">
@@ -10815,7 +10823,7 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.78, 'earningsLow': 0.69, 'earningsHigh': 0.87, 'revenueAverage': 24885700000, 'revenueLow': 24188700000, 'revenueHigh': 25998000000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.77, 'earningsLow': 0.68, 'earningsHigh': 0.86, 'revenueAverage': 24479000000, 'revenueLow': 23646900000, 'revenueHigh': 25998000000}</t>
         </is>
       </c>
       <c r="S112" t="inlineStr">
@@ -10865,13 +10873,13 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>5.495</v>
+        <v>5.62</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
       </c>
       <c r="I113" t="n">
-        <v>6.1</v>
+        <v>5.47</v>
       </c>
       <c r="J113" t="n">
         <v>6.76</v>
@@ -10888,7 +10896,7 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>0.0912</t>
+          <t>0.08939999</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
@@ -10897,7 +10905,7 @@
         </is>
       </c>
       <c r="O113" t="n">
-        <v>5.43</v>
+        <v>5.41</v>
       </c>
       <c r="P113" t="n">
         <v>11.37</v>
@@ -10959,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>171.1</v>
+        <v>169.44</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -10982,12 +10990,12 @@
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>0.027999999</t>
+          <t>0.028499998</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2.76</t>
+          <t>2.75</t>
         </is>
       </c>
       <c r="O114" t="n">
@@ -11003,7 +11011,7 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-10'], 'earningsAverage': 2.03, 'earningsLow': 1.97, 'earningsHigh': 2.09, 'revenueAverage': 22122900000, 'revenueLow': 21532100000, 'revenueHigh': 22277900000}</t>
+          <t>{'earningsDate': ['2023-10-10'], 'earningsAverage': 2.15, 'earningsLow': 2.08, 'earningsHigh': 2.21, 'revenueAverage': 23431800000, 'revenueLow': 22806000000, 'revenueHigh': 23596000000}</t>
         </is>
       </c>
       <c r="S114" t="inlineStr">
@@ -11053,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>148.18</v>
+        <v>145.86</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -11076,12 +11084,12 @@
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>0.025</t>
+          <t>0.025799999</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2.51</t>
+          <t>2.49</t>
         </is>
       </c>
       <c r="O115" t="n">
@@ -11097,7 +11105,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.62, 'earningsLow': 1.57, 'earningsHigh': 1.68, 'revenueAverage': 20339600000, 'revenueLow': 20006300000, 'revenueHigh': 20815400000}</t>
+          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.71, 'earningsLow': 1.66, 'earningsHigh': 1.78, 'revenueAverage': 21543000000, 'revenueLow': 21190000000, 'revenueHigh': 22047000000}</t>
         </is>
       </c>
       <c r="S115" t="inlineStr">
@@ -11147,7 +11155,7 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>64.63</v>
+        <v>64.75</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -11170,7 +11178,7 @@
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>0.0138</t>
+          <t>0.0136</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
@@ -11241,7 +11249,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>128.94</v>
+        <v>129.8</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -11264,7 +11272,7 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>0.0202</t>
+          <t>0.020299999</t>
         </is>
       </c>
       <c r="N117" t="inlineStr">
@@ -11335,7 +11343,7 @@
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>19.2</v>
+        <v>19.25</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -11358,7 +11366,7 @@
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>0.1458</t>
+          <t>0.1436</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
@@ -11416,7 +11424,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - PRE</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -11429,7 +11437,7 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>485.84</v>
+        <v>484.28</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -11447,7 +11455,7 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>2023-07-07</t>
+          <t>2023-10-06</t>
         </is>
       </c>
       <c r="M119" t="inlineStr">
@@ -11617,7 +11625,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>7.205</v>
+        <v>7.13</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -11640,7 +11648,7 @@
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>0.0889</t>
+          <t>0.090500005</t>
         </is>
       </c>
       <c r="N121" t="inlineStr">
@@ -11711,7 +11719,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>3.532</v>
+        <v>3.53</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -11734,7 +11742,7 @@
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>0.1503</t>
+          <t>0.1481</t>
         </is>
       </c>
       <c r="N122" t="inlineStr">
@@ -11805,7 +11813,7 @@
         <v>0</v>
       </c>
       <c r="G123" t="n">
-        <v>19.04</v>
+        <v>19.28</v>
       </c>
       <c r="H123" t="n">
         <v>0</v>
@@ -11895,7 +11903,7 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>11.02</v>
+        <v>10.92</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -11918,7 +11926,7 @@
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>0.1164</t>
+          <t>0.119399995</t>
         </is>
       </c>
       <c r="N124" t="inlineStr">
@@ -11989,7 +11997,7 @@
         <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>253.495</v>
+        <v>255.05</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -12012,7 +12020,7 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>0.0095</t>
+          <t>0.0094</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
@@ -12033,7 +12041,7 @@
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 2.75, 'earningsLow': 2.46, 'earningsHigh': 3.04, 'revenueAverage': 6014120000, 'revenueLow': 5897000000, 'revenueHigh': 6166310000}</t>
+          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': 2.75, 'earningsLow': 2.46, 'earningsHigh': 3.04, 'revenueAverage': 6014120000, 'revenueLow': 5897000000, 'revenueHigh': 6166310000}</t>
         </is>
       </c>
       <c r="S125" t="inlineStr">
@@ -12070,7 +12078,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -12083,13 +12091,13 @@
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>126.55</v>
+        <v>122.91</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
       </c>
       <c r="I126" t="n">
-        <v>126.77</v>
+        <v>122.91</v>
       </c>
       <c r="J126" t="n">
         <v>0</v>
@@ -12106,7 +12114,7 @@
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>0.0335</t>
+          <t>0.034</t>
         </is>
       </c>
       <c r="N126" t="inlineStr">
@@ -12115,7 +12123,7 @@
         </is>
       </c>
       <c r="O126" t="n">
-        <v>125.23</v>
+        <v>122.64</v>
       </c>
       <c r="P126" t="n">
         <v>163.07</v>
@@ -12127,7 +12135,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.53, 'revenueAverage': 1947250000, 'revenueLow': 1913390000, 'revenueHigh': 1990000000}</t>
+          <t>{'earningsDate': ['2023-11-20', '2023-11-24'], 'earningsAverage': 2.47, 'earningsLow': 2.43, 'earningsHigh': 2.53, 'revenueAverage': 1946180000, 'revenueLow': 1913390000, 'revenueHigh': 1990000000}</t>
         </is>
       </c>
       <c r="S126" t="inlineStr">
@@ -12164,7 +12172,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -12177,7 +12185,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>35.33</v>
+        <v>37.3</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -12200,7 +12208,7 @@
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>0.092700005</t>
+          <t>0.0884</t>
         </is>
       </c>
       <c r="N127" t="inlineStr">
@@ -12271,7 +12279,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>7.4739</v>
+        <v>7.99</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -12349,7 +12357,7 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>362.88</v>
+        <v>365.41</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -12367,7 +12375,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>2023-08-25</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
@@ -12443,7 +12451,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>82.95999999999999</v>
+        <v>83.58</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -12466,7 +12474,7 @@
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>0.0395</t>
+          <t>0.039100002</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
@@ -12487,7 +12495,7 @@
       </c>
       <c r="R130" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.81, 'earningsLow': 0.71, 'earningsHigh': 0.89, 'revenueAverage': 3969830000, 'revenueLow': 3899800000, 'revenueHigh': 4036000000}</t>
+          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 0.82, 'earningsLow': 0.77, 'earningsHigh': 0.89, 'revenueAverage': 3972710000, 'revenueLow': 3899800000, 'revenueHigh': 4060500000}</t>
         </is>
       </c>
       <c r="S130" t="inlineStr">
@@ -12524,7 +12532,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -12537,13 +12545,13 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>65.56999999999999</v>
+        <v>66.05</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
       </c>
       <c r="I131" t="n">
-        <v>68.45</v>
+        <v>65.20999999999999</v>
       </c>
       <c r="J131" t="n">
         <v>0</v>
@@ -12560,7 +12568,7 @@
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>0.030199999</t>
+          <t>0.0301</t>
         </is>
       </c>
       <c r="N131" t="inlineStr">
@@ -12569,7 +12577,7 @@
         </is>
       </c>
       <c r="O131" t="n">
-        <v>65.53</v>
+        <v>64.81999999999999</v>
       </c>
       <c r="P131" t="n">
         <v>87.41</v>
@@ -12631,13 +12639,13 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>110.09</v>
+        <v>110.57</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
       </c>
       <c r="I132" t="n">
-        <v>119.34</v>
+        <v>109.48</v>
       </c>
       <c r="J132" t="n">
         <v>0</v>
@@ -12654,7 +12662,7 @@
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>0.0402</t>
+          <t>0.0401</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
@@ -12663,7 +12671,7 @@
         </is>
       </c>
       <c r="O132" t="n">
-        <v>108.9107</v>
+        <v>108.15</v>
       </c>
       <c r="P132" t="n">
         <v>181.7</v>
@@ -12725,7 +12733,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>10.34</v>
+        <v>10.46</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -12748,12 +12756,12 @@
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>0.15810001</t>
+          <t>0.1527</t>
         </is>
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>11.26</t>
+          <t>11.34</t>
         </is>
       </c>
       <c r="O133" t="n">
@@ -12806,7 +12814,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -12819,13 +12827,13 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>14.41</v>
+        <v>13.92</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
       </c>
       <c r="I134" t="n">
-        <v>10.24</v>
+        <v>10.91</v>
       </c>
       <c r="J134" t="n">
         <v>0</v>
@@ -12842,7 +12850,7 @@
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>0.1487</t>
+          <t>0.1527</t>
         </is>
       </c>
       <c r="N134" t="inlineStr"/>
@@ -12909,13 +12917,13 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>102.89</v>
+        <v>104.87</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
       </c>
       <c r="I135" t="n">
-        <v>103.8</v>
+        <v>103.3</v>
       </c>
       <c r="J135" t="n">
         <v>0</v>
@@ -12932,12 +12940,12 @@
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>0.047199998</t>
+          <t>0.0465</t>
         </is>
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2.96</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="O135" t="n">
@@ -12990,7 +12998,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D136" t="n">
@@ -13003,7 +13011,7 @@
         <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>6.52</v>
+        <v>6.73</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -13026,7 +13034,7 @@
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>0.1354</t>
+          <t>0.1452</t>
         </is>
       </c>
       <c r="N136" t="inlineStr">
@@ -13097,10 +13105,10 @@
         <v>281.915</v>
       </c>
       <c r="G137" t="n">
-        <v>242.0001</v>
+        <v>250.22</v>
       </c>
       <c r="H137" t="n">
-        <v>242.0001</v>
+        <v>250.22</v>
       </c>
       <c r="I137" t="n">
         <v>103.85</v>
@@ -13125,7 +13133,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.74, 'earningsLow': 0.61, 'earningsHigh': 0.96, 'revenueAverage': 23377800000, 'revenueLow': 21913500000, 'revenueHigh': 25759900000}</t>
+          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.78, 'earningsLow': 0.65, 'earningsHigh': 1.02, 'revenueAverage': 24616300000, 'revenueLow': 23210000000, 'revenueHigh': 26738000000}</t>
         </is>
       </c>
       <c r="S137" t="inlineStr">
@@ -13175,7 +13183,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>13.14</v>
+        <v>13.24</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -13198,12 +13206,12 @@
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>0.1294</t>
+          <t>0.138</t>
         </is>
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>13.19</t>
+          <t>13.33</t>
         </is>
       </c>
       <c r="O138" t="n">
@@ -13256,7 +13264,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>MONITOR</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -13269,13 +13277,13 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>20.855</v>
+        <v>22.24</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
       </c>
       <c r="I139" t="n">
-        <v>21.43</v>
+        <v>20.9</v>
       </c>
       <c r="J139" t="n">
         <v>0</v>
@@ -13292,16 +13300,16 @@
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>0.090900004</t>
+          <t>0.0919</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>4.17</t>
+          <t>4.27</t>
         </is>
       </c>
       <c r="O139" t="n">
-        <v>20.85</v>
+        <v>20.58</v>
       </c>
       <c r="P139" t="n">
         <v>42.29</v>
@@ -13313,7 +13321,7 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-12'], 'earningsAverage': 0.65, 'earningsLow': 0.63, 'earningsHigh': 0.68, 'revenueAverage': 32817200000, 'revenueLow': 32039400000, 'revenueHigh': 33766900000}</t>
+          <t>{'earningsDate': ['2023-10-12'], 'earningsAverage': 0.69, 'earningsLow': 0.66, 'earningsHigh': 0.72, 'revenueAverage': 34819800000, 'revenueLow': 33935000000, 'revenueHigh': 35764700000}</t>
         </is>
       </c>
       <c r="S139" t="inlineStr">
@@ -13350,7 +13358,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -13363,7 +13371,7 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>9.7599</v>
+        <v>9.4</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -13381,12 +13389,12 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>2023-06-30</t>
+          <t>2023-09-29</t>
         </is>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>0.1442</t>
+          <t>0.1494</t>
         </is>
       </c>
       <c r="N140" t="inlineStr">
@@ -13398,7 +13406,7 @@
         <v>7</v>
       </c>
       <c r="P140" t="n">
-        <v>12.48</v>
+        <v>11.91</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
@@ -13457,7 +13465,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>161.575</v>
+        <v>159.93</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -13480,12 +13488,12 @@
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>0.0139999995</t>
+          <t>0.0143</t>
         </is>
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>1.7</t>
+          <t>1.69</t>
         </is>
       </c>
       <c r="O141" t="n">
@@ -13501,7 +13509,7 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-16'], 'earningsAverage': 1.42, 'earningsLow': 1.37, 'earningsHigh': 1.51, 'revenueAverage': 149966000000, 'revenueLow': 148191000000, 'revenueHigh': 152101000000}</t>
+          <t>{'earningsDate': ['2023-11-16'], 'earningsAverage': 1.5, 'earningsLow': 1.45, 'earningsHigh': 1.6, 'revenueAverage': 158839000000, 'revenueLow': 156959000000, 'revenueHigh': 161100000000}</t>
         </is>
       </c>
       <c r="S141" t="inlineStr">
@@ -13551,7 +13559,7 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>372.755</v>
+        <v>375.21</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -13645,7 +13653,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>118.45</v>
+        <v>117.58</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -13668,19 +13676,19 @@
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>0.0313</t>
+          <t>0.031</t>
         </is>
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>5.28</t>
+          <t>5.27</t>
         </is>
       </c>
       <c r="O143" t="n">
-        <v>85.92</v>
+        <v>89.72</v>
       </c>
       <c r="P143" t="n">
-        <v>119.92</v>
+        <v>120.7</v>
       </c>
       <c r="Q143" t="inlineStr">
         <is>
@@ -13689,7 +13697,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.11, 'earningsLow': 1.84, 'earningsHigh': 2.46, 'revenueAverage': 77384700000, 'revenueLow': 56184200000, 'revenueHigh': 87467000000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.31, 'earningsLow': 1.95, 'earningsHigh': 3.03, 'revenueAverage': 87510100000, 'revenueLow': 63476100000, 'revenueHigh': 116823000000}</t>
         </is>
       </c>
       <c r="S143" t="inlineStr">
@@ -13726,7 +13734,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -13739,13 +13747,13 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>10.135</v>
+        <v>10.45</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
       </c>
       <c r="I144" t="n">
-        <v>11</v>
+        <v>10.24</v>
       </c>
       <c r="J144" t="n">
         <v>0</v>
@@ -13763,7 +13771,7 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="n">
-        <v>10.13</v>
+        <v>10.01</v>
       </c>
       <c r="P144" t="n">
         <v>29.38</v>
@@ -13775,7 +13783,7 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': -1.14, 'earningsLow': -1.59, 'earningsHigh': -0.58, 'revenueAverage': 1345680000, 'revenueLow': 1230230000, 'revenueHigh': 1479000000}</t>
+          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': -1.15, 'earningsLow': -1.62, 'earningsHigh': -0.58, 'revenueAverage': 1344470000, 'revenueLow': 1225380000, 'revenueHigh': 1479000000}</t>
         </is>
       </c>
       <c r="S144" t="inlineStr">

</xml_diff>

<commit_message>
chore: update portfolio and formatting
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>148.46</v>
+        <v>148.25</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -615,7 +615,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.88, 'earningsLow': 2.8, 'earningsHigh': 2.97, 'revenueAverage': 13680600000, 'revenueLow': 13570000000, 'revenueHigh': 13811000000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.88, 'earningsLow': 2.8, 'earningsHigh': 2.97, 'revenueAverage': 13685000000, 'revenueLow': 13570000000, 'revenueHigh': 13811000000}</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>95.31999999999999</v>
+        <v>95.73</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -746,7 +746,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>6.765</v>
+        <v>6.56</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>9.342000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>74.345</v>
+        <v>73.66</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -991,7 +991,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.54, 'earningsLow': 1.4, 'earningsHigh': 1.71, 'revenueAverage': 24168200000, 'revenueLow': 22968000000, 'revenueHigh': 25287600000}</t>
+          <t>{'earningsDate': ['2023-10-23', '2023-10-27'], 'earningsAverage': 1.53, 'earningsLow': 1.4, 'earningsHigh': 1.71, 'revenueAverage': 24168200000, 'revenueLow': 22968000000, 'revenueHigh': 25287600000}</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>239.38</v>
+        <v>238.91</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>11.5601</v>
+        <v>11.15</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>76.11</v>
+        <v>76.28</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>56.12</v>
+        <v>56.26</v>
       </c>
       <c r="P9" t="n">
         <v>78.43000000000001</v>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>12.51</v>
+        <v>12.99</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.1329</t>
+          <t>0.1299</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.365</v>
+        <v>9.0296</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6.37</v>
+        <v>6.38</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>167.86</v>
+        <v>159.44</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>162</v>
+        <v>159.6</v>
       </c>
       <c r="P13" t="n">
         <v>334.55</v>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9.058999999999999</v>
+        <v>8.93</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>8.94</v>
+        <v>8.93</v>
       </c>
       <c r="P14" t="n">
         <v>12.78</v>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>9</v>
+        <v>8.94</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>128.84</v>
+        <v>128.09</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>8.52</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-06', '2023-11-11'], 'earningsAverage': 0.15, 'earningsLow': 0.06, 'earningsHigh': 0.22, 'revenueAverage': 8610000, 'revenueLow': 7300000, 'revenueHigh': 9800000}</t>
+          <t>{'earningsDate': ['2023-11-06', '2023-11-11'], 'earningsAverage': 0.13, 'earningsLow': 0.06, 'earningsHigh': 0.18, 'revenueAverage': 8380000, 'revenueLow': 7300000, 'revenueHigh': 9800000}</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>66.51000000000001</v>
+        <v>66.05</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-31'], 'earningsAverage': 0.77, 'earningsLow': 0.69, 'earningsHigh': 0.81, 'revenueAverage': 898710000, 'revenueLow': 876300000, 'revenueHigh': 924700000}</t>
+          <t>{'earningsDate': ['2023-10-26'], 'earningsAverage': 0.77, 'earningsLow': 0.69, 'earningsHigh': 0.81, 'revenueAverage': 898710000, 'revenueLow': 876300000, 'revenueHigh': 924700000}</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>279.25</v>
+        <v>279.08</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -2185,7 +2185,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 3.12, 'earningsLow': 3.09, 'earningsHigh': 3.16, 'revenueAverage': 3329020000, 'revenueLow': 3127000000, 'revenueHigh': 3576200000}</t>
+          <t>{'earningsDate': ['2023-11-01', '2023-11-06'], 'earningsAverage': 3.12, 'earningsLow': 3.09, 'earningsHigh': 3.16, 'revenueAverage': 3322210000, 'revenueLow': 3127000000, 'revenueHigh': 3576200000}</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>9.970000000000001</v>
+        <v>9.84</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -2267,7 +2267,7 @@
         </is>
       </c>
       <c r="O20" t="n">
-        <v>7.91</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="P20" t="n">
         <v>12.75</v>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>22.0203</v>
+        <v>22.0101</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2419,10 +2419,10 @@
         <v>2103.093</v>
       </c>
       <c r="G22" t="n">
-        <v>20.58</v>
+        <v>19.695</v>
       </c>
       <c r="H22" t="n">
-        <v>9816.66</v>
+        <v>9394.514999999999</v>
       </c>
       <c r="I22" t="n">
         <v>4.21</v>
@@ -2451,10 +2451,10 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>20.205</v>
+        <v>19.68</v>
       </c>
       <c r="P22" t="n">
-        <v>33.375</v>
+        <v>33.4</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 0.23, 'earningsLow': 0.2, 'earningsHigh': 0.25, 'revenueAverage': 6990000, 'revenueLow': 4510000, 'revenueHigh': 9480000}</t>
+          <t>{'earningsDate': ['2023-10-24', '2023-10-30'], 'earningsAverage': 1.13, 'earningsLow': 1.0, 'earningsHigh': 1.25, 'revenueAverage': 6990000, 'revenueLow': 4510000, 'revenueHigh': 9480000}</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>104.41</v>
+        <v>101.945</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>10.8</v>
+        <v>10.7</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>8.8599</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>4.485</v>
+        <v>4.16</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.1322</t>
+          <t>0.1367</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>256.28</v>
+        <v>257.13</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>24.34</v>
+        <v>24.025</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 0.61, 'earningsLow': 0.58, 'earningsHigh': 0.66, 'revenueAverage': 1587260000, 'revenueLow': 1482900000, 'revenueHigh': 1936000000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 0.61, 'earningsLow': 0.58, 'earningsHigh': 0.66, 'revenueAverage': 1584430000, 'revenueLow': 1482900000, 'revenueHigh': 1936000000}</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>4.93</v>
+        <v>4.705</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>69.31</v>
+        <v>69.5748</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>0.0064999997</t>
+          <t>0.0066000004</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8.029999999999999</v>
+        <v>7.72</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -3351,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>86.42</v>
+        <v>86.66679999999999</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -3383,7 +3383,7 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>66.05</v>
+        <v>66.92</v>
       </c>
       <c r="P32" t="n">
         <v>95.45</v>
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>206.43</v>
+        <v>206.045</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -3477,7 +3477,7 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>181.23</v>
+        <v>181.32</v>
       </c>
       <c r="P33" t="n">
         <v>231.37</v>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': 4.24, 'earningsLow': 3.56, 'earningsHigh': 5.05, 'revenueAverage': 11619800000, 'revenueLow': 11421000000, 'revenueHigh': 11752000000}</t>
+          <t>{'earningsDate': ['2023-10-24'], 'earningsAverage': 4.27, 'earningsLow': 3.56, 'earningsHigh': 5.05, 'revenueAverage': 11619800000, 'revenueLow': 11421000000, 'revenueHigh': 11752000000}</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3539,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>91.845</v>
+        <v>91.69</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -3583,7 +3583,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.68, 'earningsLow': 0.66, 'earningsHigh': 0.75, 'revenueAverage': 1428230000, 'revenueLow': 1420870000, 'revenueHigh': 1445800000}</t>
+          <t>{'earningsDate': ['2023-11-03'], 'earningsAverage': 0.68, 'earningsLow': 0.66, 'earningsHigh': 0.75, 'revenueAverage': 1428230000, 'revenueLow': 1420870000, 'revenueHigh': 1445800000}</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -3633,10 +3633,10 @@
         <v>1446.798</v>
       </c>
       <c r="G35" t="n">
-        <v>3.57</v>
+        <v>3.48</v>
       </c>
       <c r="H35" t="n">
-        <v>1306.62</v>
+        <v>1273.68</v>
       </c>
       <c r="I35" t="n">
         <v>3.72</v>
@@ -3665,7 +3665,7 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>3.535</v>
+        <v>3.48</v>
       </c>
       <c r="P35" t="n">
         <v>7.24</v>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>85.09</v>
+        <v>85.53</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -3759,7 +3759,7 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>84.76000000000001</v>
+        <v>84.53</v>
       </c>
       <c r="P36" t="n">
         <v>108.05</v>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.86, 'earningsLow': 0.68, 'earningsHigh': 0.99, 'revenueAverage': 4384560000, 'revenueLow': 4165100000, 'revenueHigh': 4557000000}</t>
+          <t>{'earningsDate': ['2023-10-31', '2023-11-06'], 'earningsAverage': 0.85, 'earningsLow': 0.68, 'earningsHigh': 0.96, 'revenueAverage': 4384560000, 'revenueLow': 4165100000, 'revenueHigh': 4557000000}</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>5.39</v>
+        <v>5.195</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -3915,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>100.91</v>
+        <v>99.94</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -3947,7 +3947,7 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>89.62</v>
+        <v>93.65000000000001</v>
       </c>
       <c r="P38" t="n">
         <v>130.66</v>
@@ -4009,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>10.46</v>
+        <v>10.42</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -4045,7 +4045,7 @@
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-06', '2023-11-10'], 'earningsAverage': 0.39, 'earningsLow': 0.39, 'earningsHigh': 0.39, 'revenueAverage': 55800000, 'revenueLow': 55600000, 'revenueHigh': 56000000}</t>
+          <t>{'earningsDate': ['2023-11-09'], 'earningsAverage': 0.39, 'earningsLow': 0.39, 'earningsHigh': 0.39, 'revenueAverage': 55800000, 'revenueLow': 55600000, 'revenueHigh': 56000000}</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>70.745</v>
+        <v>70.87</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>0.027</t>
+          <t>0.0271</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>131.8542</v>
+        <v>130.08</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>0.0363</t>
+          <t>0.0365</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.36, 'earningsLow': 1.21, 'earningsHigh': 1.49, 'revenueAverage': 1802690000, 'revenueLow': 1747150000, 'revenueHigh': 1840000000}</t>
+          <t>{'earningsDate': ['2023-10-30', '2023-11-03'], 'earningsAverage': 1.36, 'earningsLow': 1.21, 'earningsHigh': 1.49, 'revenueAverage': 1768460000, 'revenueLow': 1477000000, 'revenueHigh': 1840000000}</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>10.985</v>
+        <v>11.01</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>7.9578</v>
+        <v>7.901</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>481.99</v>
+        <v>482.96</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>0.0112</t>
+          <t>0.0111</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4557,7 +4557,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>3.3101</v>
+        <v>3.2401</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         </is>
       </c>
       <c r="O45" t="n">
-        <v>3.3</v>
+        <v>3.2401</v>
       </c>
       <c r="P45" t="n">
         <v>4.4</v>
@@ -4651,7 +4651,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>167.12</v>
+        <v>165.9</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -4683,7 +4683,7 @@
         </is>
       </c>
       <c r="O46" t="n">
-        <v>148.3</v>
+        <v>149.74</v>
       </c>
       <c r="P46" t="n">
         <v>189.68</v>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 3.33, 'earningsLow': 2.74, 'earningsHigh': 4.02, 'revenueAverage': 49265100000, 'revenueLow': 36703000000, 'revenueHigh': 62131400000}</t>
+          <t>{'earningsDate': ['2023-10-27'], 'earningsAverage': 3.34, 'earningsLow': 2.74, 'earningsHigh': 4.02, 'revenueAverage': 49265100000, 'revenueLow': 36703000000, 'revenueHigh': 62131400000}</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4745,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>139.15</v>
+        <v>137.68</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>0.0146</t>
+          <t>0.0148</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -4839,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.475</v>
+        <v>3.5193</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -4929,10 +4929,10 @@
         <v>647</v>
       </c>
       <c r="G49" t="n">
-        <v>6.053</v>
+        <v>5.97</v>
       </c>
       <c r="H49" t="n">
-        <v>605.3</v>
+        <v>597</v>
       </c>
       <c r="I49" t="n">
         <v>6.2</v>
@@ -4961,7 +4961,7 @@
         </is>
       </c>
       <c r="O49" t="n">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="P49" t="n">
         <v>8.15</v>
@@ -5023,10 +5023,10 @@
         <v>153.75</v>
       </c>
       <c r="G50" t="n">
-        <v>10.145</v>
+        <v>10.08</v>
       </c>
       <c r="H50" t="n">
-        <v>152.175</v>
+        <v>151.2</v>
       </c>
       <c r="I50" t="n">
         <v>9.98</v>
@@ -5117,7 +5117,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>168.45</v>
+        <v>166.9</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -5211,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>83.58</v>
+        <v>81.36</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>0.0379</t>
+          <t>0.0397</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -5305,7 +5305,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>12.3899</v>
+        <v>12.22</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -5337,7 +5337,7 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>10.81</v>
+        <v>10.82</v>
       </c>
       <c r="P53" t="n">
         <v>14.62</v>
@@ -5399,10 +5399,10 @@
         <v>42</v>
       </c>
       <c r="G54" t="n">
-        <v>42.16</v>
+        <v>42.23</v>
       </c>
       <c r="H54" t="n">
-        <v>42.16</v>
+        <v>42.23</v>
       </c>
       <c r="I54" t="n">
         <v>39.27</v>
@@ -5489,7 +5489,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>96.28</v>
+        <v>95.44</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -5521,7 +5521,7 @@
         </is>
       </c>
       <c r="O55" t="n">
-        <v>73.94</v>
+        <v>76.08</v>
       </c>
       <c r="P55" t="n">
         <v>100.62</v>
@@ -5583,7 +5583,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>211.95</v>
+        <v>208.85</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -5677,7 +5677,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>114.6275</v>
+        <v>114.275</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -5771,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>6.0249</v>
+        <v>5.98</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -5865,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>18.645</v>
+        <v>18.05</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -5942,7 +5942,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -5955,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>90.56999999999999</v>
+        <v>87.905</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -6049,7 +6049,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>19.685</v>
+        <v>19.53</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -6081,7 +6081,7 @@
         </is>
       </c>
       <c r="O61" t="n">
-        <v>16.74</v>
+        <v>17.025</v>
       </c>
       <c r="P61" t="n">
         <v>20.8</v>
@@ -6143,7 +6143,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>222.01</v>
+        <v>222.7</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>9.859999999999999</v>
+        <v>9.52</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -6331,7 +6331,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>4.735</v>
+        <v>4.6381</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.22, 'earningsLow': 0.22, 'earningsHigh': 0.23, 'revenueAverage': 3524540000, 'revenueLow': 3524540000, 'revenueHigh': 3524540000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.22, 'earningsLow': 0.22, 'earningsHigh': 0.23, 'revenueAverage': 3517570000, 'revenueLow': 3517570000, 'revenueHigh': 3517570000}</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6425,7 +6425,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>5.8501</v>
+        <v>5.76</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -6519,10 +6519,10 @@
         <v>70.75</v>
       </c>
       <c r="G66" t="n">
-        <v>14.3</v>
+        <v>14.16</v>
       </c>
       <c r="H66" t="n">
-        <v>71.5</v>
+        <v>70.8</v>
       </c>
       <c r="I66" t="n">
         <v>12.41</v>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>MONITOR</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -6609,7 +6609,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>9.664999999999999</v>
+        <v>9.02</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -6703,7 +6703,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>8.09</v>
+        <v>7.94</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -6793,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>133.35</v>
+        <v>133.41</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -6871,7 +6871,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>144.53</v>
+        <v>144.825</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -6965,7 +6965,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>4.7695</v>
+        <v>4.5695</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -7059,7 +7059,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>9.795</v>
+        <v>9.5</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -7149,7 +7149,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>693.765</v>
+        <v>696.375</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -7243,7 +7243,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>6.6</v>
+        <v>6.185</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -7333,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>37.52</v>
+        <v>37.39</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -7427,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>141.19</v>
+        <v>140.87</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -7521,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>4.0001</v>
+        <v>4.07</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -7615,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>19.99</v>
+        <v>19.3632</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>230.355</v>
+        <v>229.8</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -7803,7 +7803,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>9.945</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -7897,7 +7897,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>154.57</v>
+        <v>154.49</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -7920,7 +7920,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>0.0306</t>
+          <t>0.0307</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -7991,7 +7991,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.72</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -8015,7 +8015,7 @@
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="n">
-        <v>0.7</v>
+        <v>0.667</v>
       </c>
       <c r="P82" t="n">
         <v>7.025</v>
@@ -8064,7 +8064,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -8077,7 +8077,7 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>22.46</v>
+        <v>22.22</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -8100,7 +8100,7 @@
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>0.5767</t>
+          <t>0.5869</t>
         </is>
       </c>
       <c r="N83" t="inlineStr"/>
@@ -8167,7 +8167,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>119.78</v>
+        <v>119.75</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -8261,7 +8261,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>55.76</v>
+        <v>55.27</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -8355,7 +8355,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>11.61</v>
+        <v>11.189</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -8449,10 +8449,10 @@
         <v>569.3099999999999</v>
       </c>
       <c r="G87" t="n">
-        <v>25.24</v>
+        <v>24.885</v>
       </c>
       <c r="H87" t="n">
-        <v>530.04</v>
+        <v>522.585</v>
       </c>
       <c r="I87" t="n">
         <v>24.58</v>
@@ -8543,7 +8543,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>369.03</v>
+        <v>369.77</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -8637,7 +8637,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>5.5671</v>
+        <v>5.57</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -8731,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>5.95</v>
+        <v>5.89</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -8754,7 +8754,7 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>0.1299</t>
+          <t>0.134</t>
         </is>
       </c>
       <c r="N90" t="inlineStr"/>
@@ -8771,7 +8771,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>{'earningsDate': [], 'earningsAverage': 0.01, 'earningsLow': 0.01, 'earningsHigh': 0.01, 'revenueAverage': 194430000, 'revenueLow': 194430000, 'revenueHigh': 194430000}</t>
+          <t>{'earningsDate': [], 'earningsAverage': 0.01, 'earningsLow': 0.01, 'earningsHigh': 0.01, 'revenueAverage': 194090000, 'revenueLow': 194090000, 'revenueHigh': 194090000}</t>
         </is>
       </c>
       <c r="S90" t="inlineStr">
@@ -8821,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>208.18</v>
+        <v>203.72</v>
       </c>
       <c r="H91" t="n">
         <v>0</v>
@@ -8915,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>1.055</v>
+        <v>1.035</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -9005,7 +9005,7 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>260.555</v>
+        <v>257.9</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -9037,7 +9037,7 @@
         </is>
       </c>
       <c r="O93" t="n">
-        <v>231.71</v>
+        <v>232.08</v>
       </c>
       <c r="P93" t="n">
         <v>299.35</v>
@@ -9099,7 +9099,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>77.63500000000001</v>
+        <v>77.17</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -9193,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>9.4</v>
+        <v>9.234999999999999</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -9274,7 +9274,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -9287,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>75.045</v>
+        <v>69.83499999999999</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -9319,7 +9319,7 @@
         </is>
       </c>
       <c r="O96" t="n">
-        <v>70.59999999999999</v>
+        <v>69.34999999999999</v>
       </c>
       <c r="P96" t="n">
         <v>94.39</v>
@@ -9368,7 +9368,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -9381,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>91.45999999999999</v>
+        <v>89.23999999999999</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -9413,7 +9413,7 @@
         </is>
       </c>
       <c r="O97" t="n">
-        <v>90.42</v>
+        <v>89.1842</v>
       </c>
       <c r="P97" t="n">
         <v>133.91</v>
@@ -9475,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>20.01</v>
+        <v>20.19</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -9561,7 +9561,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>4.14</v>
+        <v>3.93</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -9655,7 +9655,7 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>221.83</v>
+        <v>220.77</v>
       </c>
       <c r="H100" t="n">
         <v>0</v>
@@ -9736,7 +9736,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -9749,7 +9749,7 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>54.365</v>
+        <v>52.0549</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -9772,16 +9772,16 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>0.0328</t>
+          <t>0.0326</t>
         </is>
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2.12</t>
+          <t>2.13</t>
         </is>
       </c>
       <c r="O101" t="n">
-        <v>54.06</v>
+        <v>50.18</v>
       </c>
       <c r="P101" t="n">
         <v>88.61</v>
@@ -9793,7 +9793,7 @@
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.86, 'earningsLow': 0.69, 'earningsHigh': 0.95, 'revenueAverage': 6972240000, 'revenueLow': 5509480000, 'revenueHigh': 7523260000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 0.86, 'earningsLow': 0.69, 'earningsHigh': 0.95, 'revenueAverage': 6973990000, 'revenueLow': 5509480000, 'revenueHigh': 7523260000}</t>
         </is>
       </c>
       <c r="S101" t="inlineStr">
@@ -9843,7 +9843,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>5.3</v>
+        <v>5.37</v>
       </c>
       <c r="H102" t="n">
         <v>0</v>
@@ -9937,7 +9937,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>18.525</v>
+        <v>18.145</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -10031,7 +10031,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>156.03</v>
+        <v>154.1</v>
       </c>
       <c r="H104" t="n">
         <v>0</v>
@@ -10054,16 +10054,16 @@
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>0.0128999995</t>
+          <t>0.012999999</t>
         </is>
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>2.31</t>
+          <t>2.29</t>
         </is>
       </c>
       <c r="O104" t="n">
-        <v>109.27</v>
+        <v>113.94</v>
       </c>
       <c r="P104" t="n">
         <v>182.68</v>
@@ -10112,7 +10112,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -10125,7 +10125,7 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>8.395</v>
+        <v>8.27</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -10157,7 +10157,7 @@
         </is>
       </c>
       <c r="O105" t="n">
-        <v>8.279999999999999</v>
+        <v>8.26</v>
       </c>
       <c r="P105" t="n">
         <v>12.96</v>
@@ -10219,7 +10219,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>49.6801</v>
+        <v>48.805</v>
       </c>
       <c r="H106" t="n">
         <v>0</v>
@@ -10251,7 +10251,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>49.38</v>
+        <v>48.71</v>
       </c>
       <c r="P106" t="n">
         <v>68.84999999999999</v>
@@ -10313,10 +10313,10 @@
         <v>3683.5</v>
       </c>
       <c r="G107" t="n">
-        <v>7.13</v>
+        <v>6.7174</v>
       </c>
       <c r="H107" t="n">
-        <v>3565</v>
+        <v>3358.7</v>
       </c>
       <c r="I107" t="n">
         <v>6.43</v>
@@ -10390,7 +10390,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -10403,7 +10403,7 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>4.015</v>
+        <v>3.94</v>
       </c>
       <c r="H108" t="n">
         <v>0</v>
@@ -10435,7 +10435,7 @@
         </is>
       </c>
       <c r="O108" t="n">
-        <v>4.01</v>
+        <v>3.89</v>
       </c>
       <c r="P108" t="n">
         <v>18.1</v>
@@ -10447,7 +10447,7 @@
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': -0.08, 'earningsLow': -0.09, 'earningsHigh': -0.08, 'revenueAverage': 132740000, 'revenueLow': 131720000, 'revenueHigh': 133770000}</t>
+          <t>{'earningsDate': ['2023-10-30'], 'earningsAverage': -0.08, 'earningsLow': -0.09, 'earningsHigh': -0.08, 'revenueAverage': 132740000, 'revenueLow': 131720000, 'revenueHigh': 133770000}</t>
         </is>
       </c>
       <c r="S108" t="inlineStr">
@@ -10484,29 +10484,29 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>321</v>
+        <v>344</v>
       </c>
       <c r="E109" t="n">
-        <v>9.067</v>
+        <v>9.01</v>
       </c>
       <c r="F109" t="n">
-        <v>2910.507</v>
+        <v>3099.44</v>
       </c>
       <c r="G109" t="n">
-        <v>8.370100000000001</v>
+        <v>7.905</v>
       </c>
       <c r="H109" t="n">
-        <v>2686.8021</v>
+        <v>2719.32</v>
       </c>
       <c r="I109" t="n">
         <v>8.41</v>
       </c>
       <c r="J109" t="n">
-        <v>9.970000000000001</v>
+        <v>9.91</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -10529,7 +10529,7 @@
         </is>
       </c>
       <c r="O109" t="n">
-        <v>7.95</v>
+        <v>7.87</v>
       </c>
       <c r="P109" t="n">
         <v>12.66</v>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': -0.22, 'earningsLow': -0.3, 'earningsHigh': -0.15, 'revenueAverage': -7620000, 'revenueLow': -7960000, 'revenueHigh': -7280000}</t>
+          <t>{'earningsDate': ['2023-10-26'], 'earningsAverage': -0.22, 'earningsLow': -0.3, 'earningsHigh': -0.15, 'revenueAverage': -7620000, 'revenueLow': -7960000, 'revenueHigh': -7280000}</t>
         </is>
       </c>
       <c r="S109" t="inlineStr">
@@ -10591,10 +10591,10 @@
         <v>369</v>
       </c>
       <c r="G110" t="n">
-        <v>4.9949</v>
+        <v>4.9597</v>
       </c>
       <c r="H110" t="n">
-        <v>499.49</v>
+        <v>495.97</v>
       </c>
       <c r="I110" t="n">
         <v>4.8</v>
@@ -10685,7 +10685,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>3.015</v>
+        <v>2.99</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -10779,7 +10779,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>14.875</v>
+        <v>14.565</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -10860,7 +10860,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -10873,7 +10873,7 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
-        <v>5.605</v>
+        <v>5.39</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -10896,16 +10896,16 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>0.08939999</t>
+          <t>0.088999994</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>5.88</t>
+          <t>6.03</t>
         </is>
       </c>
       <c r="O113" t="n">
-        <v>5.41</v>
+        <v>5.385</v>
       </c>
       <c r="P113" t="n">
         <v>11.37</v>
@@ -10967,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>168.8</v>
+        <v>168.94</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -11061,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>145.38</v>
+        <v>146.1496</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -11105,7 +11105,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.71, 'earningsLow': 1.66, 'earningsHigh': 1.78, 'revenueAverage': 21543000000, 'revenueLow': 21190000000, 'revenueHigh': 22047000000}</t>
+          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 1.71, 'earningsLow': 1.66, 'earningsHigh': 1.78, 'revenueAverage': 21563900000, 'revenueLow': 21190000000, 'revenueHigh': 22047000000}</t>
         </is>
       </c>
       <c r="S115" t="inlineStr">
@@ -11155,7 +11155,7 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>64.83</v>
+        <v>63.55</v>
       </c>
       <c r="H116" t="n">
         <v>0</v>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>1.68</t>
+          <t>1.65</t>
         </is>
       </c>
       <c r="O116" t="n">
@@ -11249,7 +11249,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>129.68</v>
+        <v>128.31</v>
       </c>
       <c r="H117" t="n">
         <v>0</v>
@@ -11272,12 +11272,12 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>0.020299999</t>
+          <t>0.02</t>
         </is>
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>1.7</t>
+          <t>1.71</t>
         </is>
       </c>
       <c r="O117" t="n">
@@ -11343,7 +11343,7 @@
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>19.25</v>
+        <v>18.91</v>
       </c>
       <c r="H118" t="n">
         <v>0</v>
@@ -11437,7 +11437,7 @@
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>482.94</v>
+        <v>481.05</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -11625,7 +11625,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>6.97</v>
+        <v>6.92</v>
       </c>
       <c r="H121" t="n">
         <v>0</v>
@@ -11719,7 +11719,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>3.48</v>
+        <v>3.405</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -11813,7 +11813,7 @@
         <v>0</v>
       </c>
       <c r="G123" t="n">
-        <v>19.64</v>
+        <v>19.21</v>
       </c>
       <c r="H123" t="n">
         <v>0</v>
@@ -11903,7 +11903,7 @@
         <v>0</v>
       </c>
       <c r="G124" t="n">
-        <v>10.8288</v>
+        <v>10.83</v>
       </c>
       <c r="H124" t="n">
         <v>0</v>
@@ -11926,12 +11926,12 @@
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>0.119399995</t>
+          <t>0.1193</t>
         </is>
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>7.83</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="O124" t="n">
@@ -11997,7 +11997,7 @@
         <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>253.815</v>
+        <v>251.63</v>
       </c>
       <c r="H125" t="n">
         <v>0</v>
@@ -12020,7 +12020,7 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>0.0094</t>
+          <t>0.0095</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
@@ -12091,7 +12091,7 @@
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>122.1725</v>
+        <v>121.22</v>
       </c>
       <c r="H126" t="n">
         <v>0</v>
@@ -12123,7 +12123,7 @@
         </is>
       </c>
       <c r="O126" t="n">
-        <v>121.74</v>
+        <v>120.47</v>
       </c>
       <c r="P126" t="n">
         <v>163.07</v>
@@ -12185,7 +12185,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>36.84</v>
+        <v>35.375</v>
       </c>
       <c r="H127" t="n">
         <v>0</v>
@@ -12279,7 +12279,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>8.109999999999999</v>
+        <v>7.655</v>
       </c>
       <c r="H128" t="n">
         <v>0</v>
@@ -12357,7 +12357,7 @@
         <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>371.365</v>
+        <v>364.935</v>
       </c>
       <c r="H129" t="n">
         <v>0</v>
@@ -12401,7 +12401,7 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 3.06, 'earningsLow': 2.97, 'earningsHigh': 3.22, 'revenueAverage': 3036000000, 'revenueLow': 3000880000, 'revenueHigh': 3099880000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 3.06, 'earningsLow': 2.97, 'earningsHigh': 3.22, 'revenueAverage': 3037580000, 'revenueLow': 3003100000, 'revenueHigh': 3099880000}</t>
         </is>
       </c>
       <c r="S129" t="inlineStr">
@@ -12451,7 +12451,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>83.005</v>
+        <v>79.6122</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -12545,7 +12545,7 @@
         <v>0</v>
       </c>
       <c r="G131" t="n">
-        <v>65.3437</v>
+        <v>65.075</v>
       </c>
       <c r="H131" t="n">
         <v>0</v>
@@ -12626,7 +12626,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>BUY BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -12639,7 +12639,7 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>107.96</v>
+        <v>107.15</v>
       </c>
       <c r="H132" t="n">
         <v>0</v>
@@ -12662,7 +12662,7 @@
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>0.0398</t>
+          <t>0.041199997</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
@@ -12671,7 +12671,7 @@
         </is>
       </c>
       <c r="O132" t="n">
-        <v>107.04</v>
+        <v>105.75</v>
       </c>
       <c r="P132" t="n">
         <v>181.7</v>
@@ -12720,7 +12720,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>MONITOR - POST</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -12733,7 +12733,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>10.3402</v>
+        <v>10.0159</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -12827,7 +12827,7 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>13.8691</v>
+        <v>13.6142</v>
       </c>
       <c r="H134" t="n">
         <v>0</v>
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>104.375</v>
+        <v>103.095</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -12961,7 +12961,7 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 1.83, 'earningsLow': 1.72, 'earningsHigh': 2.02, 'revenueAverage': 1636440000, 'revenueLow': 1577100000, 'revenueHigh': 1683400000}</t>
+          <t>{'earningsDate': ['2023-10-25', '2023-10-30'], 'earningsAverage': 1.84, 'earningsLow': 1.72, 'earningsHigh': 2.02, 'revenueAverage': 1636440000, 'revenueLow': 1577100000, 'revenueHigh': 1683400000}</t>
         </is>
       </c>
       <c r="S135" t="inlineStr">
@@ -13011,7 +13011,7 @@
         <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>6.655</v>
+        <v>6.31</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -13105,10 +13105,10 @@
         <v>281.915</v>
       </c>
       <c r="G137" t="n">
-        <v>248.3887</v>
+        <v>247.33</v>
       </c>
       <c r="H137" t="n">
-        <v>248.3887</v>
+        <v>247.33</v>
       </c>
       <c r="I137" t="n">
         <v>103.85</v>
@@ -13133,7 +13133,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-17', '2023-10-23'], 'earningsAverage': 0.78, 'earningsLow': 0.65, 'earningsHigh': 1.02, 'revenueAverage': 24570900000, 'revenueLow': 23210000000, 'revenueHigh': 26000000000}</t>
+          <t>{'earningsDate': ['2023-10-18'], 'earningsAverage': 0.77, 'earningsLow': 0.6, 'earningsHigh': 1.02, 'revenueAverage': 24450800000, 'revenueLow': 23161800000, 'revenueHigh': 26000000000}</t>
         </is>
       </c>
       <c r="S137" t="inlineStr">
@@ -13170,7 +13170,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>MONITOR - PRE</t>
+          <t>MONITOR - POST</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -13183,7 +13183,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>12.49</v>
+        <v>12.29</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -13277,7 +13277,7 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>22.1</v>
+        <v>22.47</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -13371,7 +13371,7 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>9.42</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="H140" t="n">
         <v>0</v>
@@ -13465,7 +13465,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>158.75</v>
+        <v>160.27</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -13559,7 +13559,7 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>369.44</v>
+        <v>369.445</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -13653,7 +13653,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>116.11</v>
+        <v>115.44</v>
       </c>
       <c r="H143" t="n">
         <v>0</v>
@@ -13685,7 +13685,7 @@
         </is>
       </c>
       <c r="O143" t="n">
-        <v>89.72</v>
+        <v>92.70999999999999</v>
       </c>
       <c r="P143" t="n">
         <v>120.7</v>
@@ -13697,7 +13697,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.31, 'earningsLow': 1.95, 'earningsHigh': 3.03, 'revenueAverage': 87510100000, 'revenueLow': 63476100000, 'revenueHigh': 116823000000}</t>
+          <t>{'earningsDate': ['2023-10-26', '2023-10-30'], 'earningsAverage': 2.34, 'earningsLow': 1.95, 'earningsHigh': 3.03, 'revenueAverage': 87510100000, 'revenueLow': 63476100000, 'revenueHigh': 116823000000}</t>
         </is>
       </c>
       <c r="S143" t="inlineStr">
@@ -13734,7 +13734,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>BUY BUY</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -13747,7 +13747,7 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>10.39</v>
+        <v>9.738</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -13771,7 +13771,7 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="n">
-        <v>10.01</v>
+        <v>9.68</v>
       </c>
       <c r="P144" t="n">
         <v>29.38</v>
@@ -13783,7 +13783,7 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': -1.15, 'earningsLow': -1.62, 'earningsHigh': -0.58, 'revenueAverage': 1344470000, 'revenueLow': 1225380000, 'revenueHigh': 1479000000}</t>
+          <t>{'earningsDate': ['2023-11-13', '2023-11-17'], 'earningsAverage': -1.16, 'earningsLow': -1.62, 'earningsHigh': -0.58, 'revenueAverage': 1328470000, 'revenueLow': 1225380000, 'revenueHigh': 1479000000}</t>
         </is>
       </c>
       <c r="S144" t="inlineStr">

</xml_diff>